<commit_message>
Fixed problems with 64-bit integers in fixed point computations.
git-svn-id: https://svn.code.sf.net/p/half/code/trunk@388 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -3672,16 +3672,16 @@
         <v>50</v>
       </c>
       <c r="B32" s="2">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="C32" s="2">
-        <v>218</v>
+        <v>158</v>
       </c>
       <c r="D32" s="2">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="E32" s="2">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="F32" s="2">
         <v>5526</v>
@@ -3951,13 +3951,13 @@
         <v>121</v>
       </c>
       <c r="C35" s="11">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D35" s="11">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E35" s="11">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F35" s="11">
         <v>24722</v>

</xml_diff>

<commit_message>
Tested exception handling for 2 argument functions.
git-svn-id: https://svn.code.sf.net/p/half/code/trunk@404 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -2337,16 +2337,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C18" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D18" s="2">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E18" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F18" s="2">
         <v>7735</v>
@@ -4172,7 +4172,7 @@
       </c>
       <c r="B38" s="24">
         <f>COUNTIF(B7:B36,"=0")/COUNTA(B7:B36)</f>
-        <v>0.73333333333333328</v>
+        <v>0.76666666666666672</v>
       </c>
       <c r="C38" s="24">
         <f>COUNTIF(C7:C36,"=0")/COUNTA(C7:C36)</f>
@@ -4259,7 +4259,7 @@
       </c>
       <c r="B39" s="25">
         <f>COUNTIF(B3:B36,"=0")/COUNTA(B3:B36)</f>
-        <v>0.76470588235294112</v>
+        <v>0.79411764705882348</v>
       </c>
       <c r="C39" s="25">
         <f>COUNTIF(C3:C36,"=0")/COUNTA(C3:C36)</f>

</xml_diff>

<commit_message>
Fixed exception handling for integral conversions.
git-svn-id: https://svn.code.sf.net/p/half/code/trunk@405 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -181,7 +181,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,25 +204,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="18">
@@ -439,12 +427,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -473,8 +460,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -489,8 +474,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -821,134 +805,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="30"/>
-      <c r="B1" s="33" t="s">
+      <c r="A1" s="28"/>
+      <c r="B1" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33" t="s">
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33" t="s">
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33" t="s">
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33" t="s">
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33" t="s">
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="34"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="32"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="31" t="s">
+      <c r="M2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="O2" s="31" t="s">
+      <c r="O2" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="P2" s="31" t="s">
+      <c r="P2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="Q2" s="31" t="s">
+      <c r="Q2" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="R2" s="31" t="s">
+      <c r="R2" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="S2" s="31" t="s">
+      <c r="S2" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="T2" s="31" t="s">
+      <c r="T2" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="32" t="s">
+      <c r="U2" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="V2" s="32" t="s">
+      <c r="V2" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="W2" s="31" t="s">
+      <c r="W2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="X2" s="31" t="s">
+      <c r="X2" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="Y2" s="31" t="s">
+      <c r="Y2" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="Z2" s="31" t="s">
+      <c r="Z2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="AA2" s="31" t="s">
+      <c r="AA2" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="AB2" s="31" t="s">
+      <c r="AB2" s="29" t="s">
         <v>52</v>
       </c>
     </row>
@@ -969,13 +953,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>5950</v>
+        <v>5376</v>
       </c>
       <c r="G3" s="1">
-        <v>4275</v>
+        <v>4217</v>
       </c>
       <c r="H3" s="1">
-        <v>3762</v>
+        <v>3461</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -990,25 +974,25 @@
         <v>92258304</v>
       </c>
       <c r="M3" s="1">
-        <v>2531</v>
+        <v>2464</v>
       </c>
       <c r="N3" s="1">
-        <v>2090</v>
+        <v>2023</v>
       </c>
       <c r="O3" s="1">
         <v>378</v>
       </c>
       <c r="P3" s="6">
         <f>M3/F3</f>
-        <v>0.42537815126050421</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="Q3" s="6">
         <f>N3/G3</f>
-        <v>0.48888888888888887</v>
+        <v>0.47972492293099361</v>
       </c>
       <c r="R3" s="6">
         <f>O3/H3</f>
-        <v>0.10047846889952153</v>
+        <v>0.10921698930944813</v>
       </c>
       <c r="S3" s="1">
         <v>0</v>
@@ -1023,25 +1007,25 @@
         <v>0</v>
       </c>
       <c r="W3" s="1">
-        <v>4672</v>
+        <v>4502</v>
       </c>
       <c r="X3" s="1">
-        <v>2532</v>
+        <v>2439</v>
       </c>
       <c r="Y3" s="1">
-        <v>1147</v>
+        <v>1152</v>
       </c>
       <c r="Z3" s="6">
         <f>W3/F3</f>
-        <v>0.78521008403361348</v>
+        <v>0.83742559523809523</v>
       </c>
       <c r="AA3" s="7">
         <f>X3/G3</f>
-        <v>0.59228070175438596</v>
+        <v>0.57837325112639315</v>
       </c>
       <c r="AB3" s="7">
         <f>Y3/H3</f>
-        <v>0.30489101541733121</v>
+        <v>0.33285177694308005</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -1061,13 +1045,13 @@
         <v>0</v>
       </c>
       <c r="F4" s="2">
-        <v>7512</v>
+        <v>6799</v>
       </c>
       <c r="G4" s="2">
-        <v>4336</v>
+        <v>4173</v>
       </c>
       <c r="H4" s="2">
-        <v>3791</v>
+        <v>3529</v>
       </c>
       <c r="I4" s="2">
         <v>0</v>
@@ -1082,25 +1066,25 @@
         <v>92258304</v>
       </c>
       <c r="M4" s="2">
-        <v>2541</v>
+        <v>2454</v>
       </c>
       <c r="N4" s="2">
-        <v>2088</v>
+        <v>2012</v>
       </c>
       <c r="O4" s="1">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="P4" s="6">
         <f t="shared" ref="P4:P36" si="0">M4/F4</f>
-        <v>0.33825878594249204</v>
+        <v>0.36093543168112957</v>
       </c>
       <c r="Q4" s="6">
         <f t="shared" ref="Q4:Q36" si="1">N4/G4</f>
-        <v>0.48154981549815495</v>
+        <v>0.48214713635274381</v>
       </c>
       <c r="R4" s="6">
         <f t="shared" ref="R4:R36" si="2">O4/H4</f>
-        <v>9.9182273806383545E-2</v>
+        <v>0.10682913006517428</v>
       </c>
       <c r="S4" s="2">
         <v>0</v>
@@ -1115,25 +1099,25 @@
         <v>0</v>
       </c>
       <c r="W4" s="2">
-        <v>5712</v>
+        <v>5497</v>
       </c>
       <c r="X4" s="2">
-        <v>2505</v>
+        <v>2421</v>
       </c>
       <c r="Y4" s="1">
-        <v>1144</v>
+        <v>1148</v>
       </c>
       <c r="Z4" s="6">
         <f t="shared" ref="Z4:Z36" si="3">W4/F4</f>
-        <v>0.76038338658146964</v>
+        <v>0.80850125018385055</v>
       </c>
       <c r="AA4" s="7">
         <f t="shared" ref="AA4:AA36" si="4">X4/G4</f>
-        <v>0.57772140221402213</v>
+        <v>0.5801581595974119</v>
       </c>
       <c r="AB4" s="7">
         <f t="shared" ref="AB4:AB36" si="5">Y4/H4</f>
-        <v>0.30176734370878394</v>
+        <v>0.32530461887220175</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -1153,13 +1137,13 @@
         <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>3142</v>
+        <v>3023</v>
       </c>
       <c r="G5" s="2">
-        <v>2623</v>
+        <v>2549</v>
       </c>
       <c r="H5" s="2">
-        <v>1820</v>
+        <v>1887</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
@@ -1174,25 +1158,25 @@
         <v>0</v>
       </c>
       <c r="M5" s="2">
-        <v>3279</v>
+        <v>3173</v>
       </c>
       <c r="N5" s="2">
-        <v>2823</v>
+        <v>2724</v>
       </c>
       <c r="O5" s="1">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="P5" s="6">
         <f t="shared" si="0"/>
-        <v>1.0436028007638447</v>
+        <v>1.0496195831955011</v>
       </c>
       <c r="Q5" s="6">
         <f t="shared" si="1"/>
-        <v>1.0762485703393061</v>
+        <v>1.0686543742644175</v>
       </c>
       <c r="R5" s="6">
         <f t="shared" si="2"/>
-        <v>0.20659340659340658</v>
+        <v>0.20084790673025968</v>
       </c>
       <c r="S5" s="2">
         <v>0</v>
@@ -1207,25 +1191,25 @@
         <v>0</v>
       </c>
       <c r="W5" s="2">
-        <v>5420</v>
+        <v>5218</v>
       </c>
       <c r="X5" s="2">
-        <v>3150</v>
+        <v>3040</v>
       </c>
       <c r="Y5" s="1">
-        <v>1775</v>
+        <v>1789</v>
       </c>
       <c r="Z5" s="6">
         <f t="shared" si="3"/>
-        <v>1.7250159134309357</v>
+        <v>1.7260999007608335</v>
       </c>
       <c r="AA5" s="7">
         <f t="shared" si="4"/>
-        <v>1.2009149828440717</v>
+        <v>1.1926245586504511</v>
       </c>
       <c r="AB5" s="7">
         <f t="shared" si="5"/>
-        <v>0.97527472527472525</v>
+        <v>0.94806571277159513</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -1245,10 +1229,10 @@
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>3888</v>
+        <v>3708</v>
       </c>
       <c r="G6" s="2">
-        <v>3200</v>
+        <v>3091</v>
       </c>
       <c r="H6" s="2">
         <v>2104</v>
@@ -1266,25 +1250,25 @@
         <v>0</v>
       </c>
       <c r="M6" s="2">
-        <v>3634</v>
+        <v>3514</v>
       </c>
       <c r="N6" s="2">
-        <v>3181</v>
+        <v>3080</v>
       </c>
       <c r="O6" s="1">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="P6" s="6">
         <f t="shared" si="0"/>
-        <v>0.93467078189300412</v>
+        <v>0.94768069039913705</v>
       </c>
       <c r="Q6" s="6">
         <f t="shared" si="1"/>
-        <v>0.99406249999999996</v>
+        <v>0.99644128113879005</v>
       </c>
       <c r="R6" s="6">
         <f t="shared" si="2"/>
-        <v>0.17918250950570341</v>
+        <v>0.17965779467680609</v>
       </c>
       <c r="S6" s="2">
         <v>0</v>
@@ -1299,25 +1283,25 @@
         <v>0</v>
       </c>
       <c r="W6" s="2">
-        <v>7668</v>
+        <v>7318</v>
       </c>
       <c r="X6" s="2">
-        <v>3658</v>
+        <v>3526</v>
       </c>
       <c r="Y6" s="1">
-        <v>2056</v>
+        <v>2071</v>
       </c>
       <c r="Z6" s="6">
         <f t="shared" si="3"/>
-        <v>1.9722222222222223</v>
+        <v>1.9735706580366774</v>
       </c>
       <c r="AA6" s="7">
         <f t="shared" si="4"/>
-        <v>1.1431249999999999</v>
+        <v>1.1407311549660304</v>
       </c>
       <c r="AB6" s="7">
         <f t="shared" si="5"/>
-        <v>0.97718631178707227</v>
+        <v>0.98431558935361219</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -1337,13 +1321,13 @@
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <v>1254</v>
+        <v>1170</v>
       </c>
       <c r="G7" s="2">
-        <v>795</v>
+        <v>773</v>
       </c>
       <c r="H7" s="2">
-        <v>589</v>
+        <v>608</v>
       </c>
       <c r="I7" s="2">
         <v>0</v>
@@ -1358,25 +1342,25 @@
         <v>11280</v>
       </c>
       <c r="M7" s="2">
-        <v>735</v>
+        <v>719</v>
       </c>
       <c r="N7" s="2">
-        <v>587</v>
+        <v>568</v>
       </c>
       <c r="O7" s="1">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="P7" s="6">
         <f t="shared" si="0"/>
-        <v>0.5861244019138756</v>
+        <v>0.61452991452991457</v>
       </c>
       <c r="Q7" s="6">
         <f t="shared" si="1"/>
-        <v>0.73836477987421378</v>
+        <v>0.7347994825355757</v>
       </c>
       <c r="R7" s="6">
         <f t="shared" si="2"/>
-        <v>0.44482173174872663</v>
+        <v>0.43421052631578949</v>
       </c>
       <c r="S7" s="2">
         <v>0</v>
@@ -1391,25 +1375,25 @@
         <v>0</v>
       </c>
       <c r="W7" s="2">
-        <v>1501</v>
+        <v>1047</v>
       </c>
       <c r="X7" s="2">
-        <v>656</v>
+        <v>631</v>
       </c>
       <c r="Y7" s="1">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="Z7" s="6">
         <f t="shared" si="3"/>
-        <v>1.196969696969697</v>
+        <v>0.89487179487179491</v>
       </c>
       <c r="AA7" s="7">
         <f t="shared" si="4"/>
-        <v>0.82515723270440255</v>
+        <v>0.81630012936610608</v>
       </c>
       <c r="AB7" s="7">
         <f t="shared" si="5"/>
-        <v>0.63157894736842102</v>
+        <v>0.61019736842105265</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -1429,13 +1413,13 @@
         <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>24089</v>
+        <v>22923</v>
       </c>
       <c r="G8" s="2">
-        <v>18884</v>
+        <v>18320</v>
       </c>
       <c r="H8" s="2">
-        <v>14420</v>
+        <v>14699</v>
       </c>
       <c r="I8" s="2">
         <v>666</v>
@@ -1450,25 +1434,25 @@
         <v>429655</v>
       </c>
       <c r="M8" s="2">
-        <v>11457</v>
+        <v>11087</v>
       </c>
       <c r="N8" s="2">
-        <v>9595</v>
+        <v>9334</v>
       </c>
       <c r="O8" s="1">
-        <v>1964</v>
+        <v>2016</v>
       </c>
       <c r="P8" s="6">
         <f t="shared" si="0"/>
-        <v>0.47561127485574328</v>
+        <v>0.48366269685468743</v>
       </c>
       <c r="Q8" s="6">
         <f t="shared" si="1"/>
-        <v>0.50810209701334463</v>
+        <v>0.50949781659388649</v>
       </c>
       <c r="R8" s="6">
         <f t="shared" si="2"/>
-        <v>0.13619972260748961</v>
+        <v>0.13715218722362066</v>
       </c>
       <c r="S8" s="2">
         <v>0</v>
@@ -1483,25 +1467,25 @@
         <v>0</v>
       </c>
       <c r="W8" s="2">
-        <v>26779</v>
+        <v>26402</v>
       </c>
       <c r="X8" s="2">
-        <v>12823</v>
+        <v>12422</v>
       </c>
       <c r="Y8" s="1">
-        <v>5347</v>
+        <v>6039</v>
       </c>
       <c r="Z8" s="6">
         <f t="shared" si="3"/>
-        <v>1.1116692266179584</v>
+        <v>1.15176896566767</v>
       </c>
       <c r="AA8" s="7">
         <f t="shared" si="4"/>
-        <v>0.67904045753018427</v>
+        <v>0.67805676855895192</v>
       </c>
       <c r="AB8" s="7">
         <f t="shared" si="5"/>
-        <v>0.37080443828016646</v>
+        <v>0.4108442751207565</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -1521,13 +1505,13 @@
         <v>0</v>
       </c>
       <c r="F9" s="2">
-        <v>5109</v>
+        <v>4928</v>
       </c>
       <c r="G9" s="2">
-        <v>4440</v>
+        <v>4299</v>
       </c>
       <c r="H9" s="2">
-        <v>3788</v>
+        <v>3913</v>
       </c>
       <c r="I9" s="2">
         <v>2</v>
@@ -1542,25 +1526,25 @@
         <v>9848</v>
       </c>
       <c r="M9" s="2">
-        <v>2157</v>
+        <v>2136</v>
       </c>
       <c r="N9" s="2">
-        <v>2246</v>
+        <v>2295</v>
       </c>
       <c r="O9" s="1">
-        <v>1192</v>
+        <v>1204</v>
       </c>
       <c r="P9" s="6">
         <f t="shared" si="0"/>
-        <v>0.42219612448620081</v>
+        <v>0.43344155844155846</v>
       </c>
       <c r="Q9" s="6">
         <f t="shared" si="1"/>
-        <v>0.50585585585585591</v>
+        <v>0.53384508025122124</v>
       </c>
       <c r="R9" s="6">
         <f t="shared" si="2"/>
-        <v>0.3146779303062302</v>
+        <v>0.30769230769230771</v>
       </c>
       <c r="S9" s="2">
         <v>0</v>
@@ -1575,25 +1559,25 @@
         <v>6772</v>
       </c>
       <c r="W9" s="2">
-        <v>2690</v>
+        <v>2734</v>
       </c>
       <c r="X9" s="2">
-        <v>2231</v>
+        <v>2170</v>
       </c>
       <c r="Y9" s="1">
-        <v>1483</v>
+        <v>1538</v>
       </c>
       <c r="Z9" s="6">
         <f t="shared" si="3"/>
-        <v>0.52652182423174787</v>
+        <v>0.55478896103896103</v>
       </c>
       <c r="AA9" s="7">
         <f t="shared" si="4"/>
-        <v>0.50247747747747751</v>
+        <v>0.50476855082577343</v>
       </c>
       <c r="AB9" s="7">
         <f t="shared" si="5"/>
-        <v>0.39149947201689544</v>
+        <v>0.39304881165346284</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -1613,13 +1597,13 @@
         <v>0</v>
       </c>
       <c r="F10" s="2">
-        <v>4590</v>
+        <v>4548</v>
       </c>
       <c r="G10" s="2">
-        <v>4730</v>
+        <v>4653</v>
       </c>
       <c r="H10" s="2">
-        <v>4074</v>
+        <v>4180</v>
       </c>
       <c r="I10" s="2">
         <v>1</v>
@@ -1634,25 +1618,25 @@
         <v>9218</v>
       </c>
       <c r="M10" s="2">
-        <v>8345</v>
+        <v>8087</v>
       </c>
       <c r="N10" s="2">
-        <v>4538</v>
+        <v>4383</v>
       </c>
       <c r="O10" s="1">
-        <v>3160</v>
+        <v>3256</v>
       </c>
       <c r="P10" s="6">
         <f t="shared" si="0"/>
-        <v>1.818082788671024</v>
+        <v>1.7781442392260334</v>
       </c>
       <c r="Q10" s="6">
         <f t="shared" si="1"/>
-        <v>0.95940803382663853</v>
+        <v>0.94197292069632499</v>
       </c>
       <c r="R10" s="6">
         <f t="shared" si="2"/>
-        <v>0.77565046637211588</v>
+        <v>0.77894736842105261</v>
       </c>
       <c r="S10" s="2">
         <v>0</v>
@@ -1667,25 +1651,25 @@
         <v>6144</v>
       </c>
       <c r="W10" s="2">
-        <v>7511</v>
+        <v>7358</v>
       </c>
       <c r="X10" s="2">
-        <v>4482</v>
+        <v>4353</v>
       </c>
       <c r="Y10" s="1">
-        <v>3398</v>
+        <v>3525</v>
       </c>
       <c r="Z10" s="6">
         <f t="shared" si="3"/>
-        <v>1.6363834422657952</v>
+        <v>1.6178540017590151</v>
       </c>
       <c r="AA10" s="7">
         <f t="shared" si="4"/>
-        <v>0.94756871035940804</v>
+        <v>0.93552546744036102</v>
       </c>
       <c r="AB10" s="7">
         <f t="shared" si="5"/>
-        <v>0.83406971035837019</v>
+        <v>0.84330143540669855</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -1705,13 +1689,13 @@
         <v>310</v>
       </c>
       <c r="F11" s="2">
-        <v>5689</v>
+        <v>5499</v>
       </c>
       <c r="G11" s="2">
-        <v>5457</v>
+        <v>5233</v>
       </c>
       <c r="H11" s="2">
-        <v>4708</v>
+        <v>4892</v>
       </c>
       <c r="I11" s="2">
         <v>2</v>
@@ -1726,25 +1710,25 @@
         <v>9846</v>
       </c>
       <c r="M11" s="2">
-        <v>4908</v>
+        <v>4775</v>
       </c>
       <c r="N11" s="2">
-        <v>2576</v>
+        <v>2629</v>
       </c>
       <c r="O11" s="1">
-        <v>1467</v>
+        <v>1507</v>
       </c>
       <c r="P11" s="6">
         <f t="shared" si="0"/>
-        <v>0.86271752504833887</v>
+        <v>0.86833969812693212</v>
       </c>
       <c r="Q11" s="6">
         <f t="shared" si="1"/>
-        <v>0.47205424225765075</v>
+        <v>0.50238868717752727</v>
       </c>
       <c r="R11" s="6">
         <f t="shared" si="2"/>
-        <v>0.31159728122344943</v>
+        <v>0.30805396565821752</v>
       </c>
       <c r="S11" s="2">
         <v>0</v>
@@ -1759,25 +1743,25 @@
         <v>6772</v>
       </c>
       <c r="W11" s="2">
-        <v>4554</v>
+        <v>4396</v>
       </c>
       <c r="X11" s="2">
-        <v>2490</v>
+        <v>2410</v>
       </c>
       <c r="Y11" s="1">
-        <v>1680</v>
+        <v>1744</v>
       </c>
       <c r="Z11" s="6">
         <f t="shared" si="3"/>
-        <v>0.80049217788715066</v>
+        <v>0.79941807601382064</v>
       </c>
       <c r="AA11" s="7">
         <f t="shared" si="4"/>
-        <v>0.45629466739967017</v>
+        <v>0.46053888782725017</v>
       </c>
       <c r="AB11" s="7">
         <f t="shared" si="5"/>
-        <v>0.356839422259983</v>
+        <v>0.35650040883074408</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -1797,13 +1781,13 @@
         <v>0</v>
       </c>
       <c r="F12" s="2">
-        <v>3621</v>
+        <v>3466</v>
       </c>
       <c r="G12" s="2">
-        <v>3193</v>
+        <v>3094</v>
       </c>
       <c r="H12" s="2">
-        <v>2914</v>
+        <v>2922</v>
       </c>
       <c r="I12" s="2">
         <v>1</v>
@@ -1818,25 +1802,25 @@
         <v>4</v>
       </c>
       <c r="M12" s="2">
-        <v>760</v>
+        <v>734</v>
       </c>
       <c r="N12" s="2">
-        <v>569</v>
+        <v>549</v>
       </c>
       <c r="O12" s="1">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="P12" s="6">
         <f t="shared" si="0"/>
-        <v>0.20988677161005248</v>
+        <v>0.21177149451817656</v>
       </c>
       <c r="Q12" s="6">
         <f t="shared" si="1"/>
-        <v>0.17820231756968369</v>
+        <v>0.17744020685197157</v>
       </c>
       <c r="R12" s="6">
         <f t="shared" si="2"/>
-        <v>5.3877831159917636E-2</v>
+        <v>5.4414784394250515E-2</v>
       </c>
       <c r="S12" s="2">
         <v>0</v>
@@ -1851,25 +1835,25 @@
         <v>0</v>
       </c>
       <c r="W12" s="2">
-        <v>1072</v>
+        <v>1030</v>
       </c>
       <c r="X12" s="2">
-        <v>636</v>
+        <v>618</v>
       </c>
       <c r="Y12" s="1">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="Z12" s="6">
         <f t="shared" si="3"/>
-        <v>0.296050814692074</v>
+        <v>0.29717253317945758</v>
       </c>
       <c r="AA12" s="7">
         <f t="shared" si="4"/>
-        <v>0.19918571875978702</v>
+        <v>0.19974143503555269</v>
       </c>
       <c r="AB12" s="7">
         <f t="shared" si="5"/>
-        <v>0.11942347288949898</v>
+        <v>0.12080766598220397</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
@@ -1889,13 +1873,13 @@
         <v>0</v>
       </c>
       <c r="F13" s="2">
-        <v>3661</v>
+        <v>3526</v>
       </c>
       <c r="G13" s="2">
-        <v>3250</v>
+        <v>3174</v>
       </c>
       <c r="H13" s="2">
-        <v>2896</v>
+        <v>2957</v>
       </c>
       <c r="I13" s="2">
         <v>5</v>
@@ -1910,25 +1894,25 @@
         <v>1</v>
       </c>
       <c r="M13" s="2">
-        <v>765</v>
+        <v>740</v>
       </c>
       <c r="N13" s="2">
-        <v>610</v>
+        <v>591</v>
       </c>
       <c r="O13" s="1">
         <v>168</v>
       </c>
       <c r="P13" s="6">
         <f t="shared" si="0"/>
-        <v>0.20895930073750341</v>
+        <v>0.20986954055587068</v>
       </c>
       <c r="Q13" s="6">
         <f t="shared" si="1"/>
-        <v>0.18769230769230769</v>
+        <v>0.18620037807183365</v>
       </c>
       <c r="R13" s="6">
         <f t="shared" si="2"/>
-        <v>5.8011049723756904E-2</v>
+        <v>5.6814338856949614E-2</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -1943,25 +1927,25 @@
         <v>0</v>
       </c>
       <c r="W13" s="2">
-        <v>1093</v>
+        <v>1057</v>
       </c>
       <c r="X13" s="2">
-        <v>674</v>
+        <v>655</v>
       </c>
       <c r="Y13" s="1">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="Z13" s="6">
         <f t="shared" si="3"/>
-        <v>0.29855230811253758</v>
+        <v>0.2997731140102099</v>
       </c>
       <c r="AA13" s="7">
         <f t="shared" si="4"/>
-        <v>0.20738461538461539</v>
+        <v>0.20636420919974796</v>
       </c>
       <c r="AB13" s="7">
         <f t="shared" si="5"/>
-        <v>0.12430939226519337</v>
+        <v>0.12275955360162327</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
@@ -1981,13 +1965,13 @@
         <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>5235</v>
+        <v>5078</v>
       </c>
       <c r="G14" s="2">
-        <v>3451</v>
+        <v>3233</v>
       </c>
       <c r="H14" s="2">
-        <v>2915</v>
+        <v>3031</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
@@ -2002,25 +1986,25 @@
         <v>0</v>
       </c>
       <c r="M14" s="2">
-        <v>1776</v>
+        <v>1720</v>
       </c>
       <c r="N14" s="2">
-        <v>1196</v>
+        <v>1159</v>
       </c>
       <c r="O14" s="1">
-        <v>923</v>
+        <v>928</v>
       </c>
       <c r="P14" s="6">
         <f>M14/F14</f>
-        <v>0.33925501432664756</v>
+        <v>0.3387160299330445</v>
       </c>
       <c r="Q14" s="6">
         <f>N14/G14</f>
-        <v>0.34656621269197335</v>
+        <v>0.35849056603773582</v>
       </c>
       <c r="R14" s="6">
         <f>O14/H14</f>
-        <v>0.31663807890222984</v>
+        <v>0.30616958099637082</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -2035,25 +2019,25 @@
         <v>0</v>
       </c>
       <c r="W14" s="2">
-        <v>2032</v>
+        <v>1953</v>
       </c>
       <c r="X14" s="2">
-        <v>904</v>
+        <v>875</v>
       </c>
       <c r="Y14" s="1">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="Z14" s="6">
         <f>W14/F14</f>
-        <v>0.38815663801337152</v>
+        <v>0.38460023631350926</v>
       </c>
       <c r="AA14" s="7">
         <f>X14/G14</f>
-        <v>0.26195305708490291</v>
+        <v>0.27064645839777296</v>
       </c>
       <c r="AB14" s="7">
         <f>Y14/H14</f>
-        <v>0.1934819897084048</v>
+        <v>0.1883866710656549</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
@@ -2073,13 +2057,13 @@
         <v>868</v>
       </c>
       <c r="F15" s="2">
-        <v>6644</v>
+        <v>6353</v>
       </c>
       <c r="G15" s="2">
-        <v>5938</v>
+        <v>5670</v>
       </c>
       <c r="H15" s="2">
-        <v>5210</v>
+        <v>5236</v>
       </c>
       <c r="I15" s="2">
         <v>2</v>
@@ -2094,25 +2078,25 @@
         <v>5</v>
       </c>
       <c r="M15" s="2">
-        <v>1825</v>
+        <v>1750</v>
       </c>
       <c r="N15" s="2">
-        <v>1311</v>
+        <v>1264</v>
       </c>
       <c r="O15" s="1">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="P15" s="6">
         <f t="shared" si="0"/>
-        <v>0.27468392534617703</v>
+        <v>0.27546041240358887</v>
       </c>
       <c r="Q15" s="6">
         <f t="shared" si="1"/>
-        <v>0.22078140788144157</v>
+        <v>0.22292768959435627</v>
       </c>
       <c r="R15" s="6">
         <f t="shared" si="2"/>
-        <v>0.11055662188099807</v>
+        <v>0.11077158135981666</v>
       </c>
       <c r="S15" s="2">
         <v>0</v>
@@ -2127,25 +2111,25 @@
         <v>0</v>
       </c>
       <c r="W15" s="2">
-        <v>2108</v>
+        <v>2028</v>
       </c>
       <c r="X15" s="2">
-        <v>1487</v>
+        <v>1422</v>
       </c>
       <c r="Y15" s="1">
-        <v>885</v>
+        <v>893</v>
       </c>
       <c r="Z15" s="6">
         <f t="shared" si="3"/>
-        <v>0.3172787477423239</v>
+        <v>0.31921926648827326</v>
       </c>
       <c r="AA15" s="7">
         <f t="shared" si="4"/>
-        <v>0.25042101717750082</v>
+        <v>0.25079365079365079</v>
       </c>
       <c r="AB15" s="7">
         <f t="shared" si="5"/>
-        <v>0.16986564299424184</v>
+        <v>0.17055003819709702</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -2165,13 +2149,13 @@
         <v>0</v>
       </c>
       <c r="F16" s="2">
-        <v>1524</v>
+        <v>1473</v>
       </c>
       <c r="G16" s="2">
-        <v>1486</v>
+        <v>1445</v>
       </c>
       <c r="H16" s="2">
-        <v>1272</v>
+        <v>1356</v>
       </c>
       <c r="I16" s="2">
         <v>0</v>
@@ -2186,25 +2170,25 @@
         <v>0</v>
       </c>
       <c r="M16" s="2">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="N16" s="2">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="O16" s="1">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="P16" s="6">
         <f t="shared" si="0"/>
-        <v>0.27624671916010501</v>
+        <v>0.27562797012898849</v>
       </c>
       <c r="Q16" s="6">
         <f t="shared" si="1"/>
-        <v>0.24764468371467024</v>
+        <v>0.24636678200692042</v>
       </c>
       <c r="R16" s="6">
         <f t="shared" si="2"/>
-        <v>7.0754716981132074E-2</v>
+        <v>9.9557522123893807E-2</v>
       </c>
       <c r="S16" s="2">
         <v>0</v>
@@ -2219,25 +2203,25 @@
         <v>0</v>
       </c>
       <c r="W16" s="2">
-        <v>706</v>
+        <v>681</v>
       </c>
       <c r="X16" s="2">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="Y16" s="1">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="Z16" s="6">
         <f t="shared" si="3"/>
-        <v>0.46325459317585299</v>
+        <v>0.46232179226069248</v>
       </c>
       <c r="AA16" s="7">
         <f t="shared" si="4"/>
-        <v>0.26783310901749663</v>
+        <v>0.2685121107266436</v>
       </c>
       <c r="AB16" s="7">
         <f t="shared" si="5"/>
-        <v>0.19496855345911951</v>
+        <v>0.18141592920353983</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
@@ -2257,13 +2241,13 @@
         <v>0</v>
       </c>
       <c r="F17" s="2">
-        <v>13288</v>
+        <v>12919</v>
       </c>
       <c r="G17" s="2">
-        <v>13746</v>
+        <v>13338</v>
       </c>
       <c r="H17" s="2">
-        <v>12476</v>
+        <v>12184</v>
       </c>
       <c r="I17" s="2">
         <v>20</v>
@@ -2278,25 +2262,25 @@
         <v>0</v>
       </c>
       <c r="M17" s="2">
-        <v>4862</v>
+        <v>4695</v>
       </c>
       <c r="N17" s="2">
-        <v>3189</v>
+        <v>3078</v>
       </c>
       <c r="O17" s="1">
-        <v>2242</v>
+        <v>2255</v>
       </c>
       <c r="P17" s="6">
         <f t="shared" si="0"/>
-        <v>0.36589403973509932</v>
+        <v>0.36341822122455297</v>
       </c>
       <c r="Q17" s="6">
         <f t="shared" si="1"/>
-        <v>0.23199476211261458</v>
+        <v>0.23076923076923078</v>
       </c>
       <c r="R17" s="6">
         <f t="shared" si="2"/>
-        <v>0.17970503366463611</v>
+        <v>0.18507879185817466</v>
       </c>
       <c r="S17" s="2">
         <v>0</v>
@@ -2311,25 +2295,25 @@
         <v>0</v>
       </c>
       <c r="W17" s="2">
-        <v>6438</v>
+        <v>6205</v>
       </c>
       <c r="X17" s="2">
-        <v>4686</v>
+        <v>4528</v>
       </c>
       <c r="Y17" s="1">
-        <v>3190</v>
+        <v>3205</v>
       </c>
       <c r="Z17" s="6">
         <f t="shared" si="3"/>
-        <v>0.48449729078868153</v>
+        <v>0.48030033284309931</v>
       </c>
       <c r="AA17" s="7">
         <f t="shared" si="4"/>
-        <v>0.34089917066783065</v>
+        <v>0.33948118158644475</v>
       </c>
       <c r="AB17" s="7">
         <f t="shared" si="5"/>
-        <v>0.25569092657903175</v>
+        <v>0.26304990151017726</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
@@ -2349,13 +2333,13 @@
         <v>5</v>
       </c>
       <c r="F18" s="2">
-        <v>7735</v>
+        <v>7346</v>
       </c>
       <c r="G18" s="2">
-        <v>7621</v>
+        <v>7389</v>
       </c>
       <c r="H18" s="2">
-        <v>6296</v>
+        <v>6399</v>
       </c>
       <c r="I18" s="2">
         <v>53</v>
@@ -2370,25 +2354,25 @@
         <v>148569</v>
       </c>
       <c r="M18" s="2">
-        <v>4192</v>
+        <v>4044</v>
       </c>
       <c r="N18" s="2">
-        <v>4262</v>
+        <v>4261</v>
       </c>
       <c r="O18" s="1">
-        <v>3072</v>
+        <v>3042</v>
       </c>
       <c r="P18" s="6">
         <f t="shared" si="0"/>
-        <v>0.54195216548157721</v>
+        <v>0.55050367546964329</v>
       </c>
       <c r="Q18" s="6">
         <f t="shared" si="1"/>
-        <v>0.5592441936753707</v>
+        <v>0.57666802002977402</v>
       </c>
       <c r="R18" s="6">
         <f t="shared" si="2"/>
-        <v>0.48792884371029227</v>
+        <v>0.47538677918424754</v>
       </c>
       <c r="S18" s="2">
         <v>42</v>
@@ -2403,25 +2387,25 @@
         <v>121458</v>
       </c>
       <c r="W18" s="2">
-        <v>4688</v>
+        <v>4505</v>
       </c>
       <c r="X18" s="2">
-        <v>5011</v>
+        <v>5185</v>
       </c>
       <c r="Y18" s="1">
-        <v>3663</v>
+        <v>3700</v>
       </c>
       <c r="Z18" s="6">
         <f t="shared" si="3"/>
-        <v>0.60607627666451191</v>
+        <v>0.61325891641709773</v>
       </c>
       <c r="AA18" s="7">
         <f t="shared" si="4"/>
-        <v>0.65752525915234217</v>
+        <v>0.70171877114629855</v>
       </c>
       <c r="AB18" s="7">
         <f t="shared" si="5"/>
-        <v>0.58179796696315123</v>
+        <v>0.57821534614783565</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
@@ -2441,13 +2425,13 @@
         <v>0</v>
       </c>
       <c r="F19" s="2">
-        <v>3850</v>
+        <v>3734</v>
       </c>
       <c r="G19" s="2">
-        <v>3869</v>
+        <v>3723</v>
       </c>
       <c r="H19" s="2">
-        <v>3257</v>
+        <v>3185</v>
       </c>
       <c r="I19" s="2">
         <v>13</v>
@@ -2462,25 +2446,25 @@
         <v>4</v>
       </c>
       <c r="M19" s="2">
-        <v>1355</v>
+        <v>1314</v>
       </c>
       <c r="N19" s="2">
-        <v>1094</v>
+        <v>1037</v>
       </c>
       <c r="O19" s="1">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="P19" s="6">
         <f t="shared" si="0"/>
-        <v>0.35194805194805195</v>
+        <v>0.3519014461703267</v>
       </c>
       <c r="Q19" s="6">
         <f t="shared" si="1"/>
-        <v>0.28276040320496254</v>
+        <v>0.27853881278538811</v>
       </c>
       <c r="R19" s="6">
         <f t="shared" si="2"/>
-        <v>0.10469757445501995</v>
+        <v>0.10549450549450549</v>
       </c>
       <c r="S19" s="2">
         <v>2</v>
@@ -2495,25 +2479,25 @@
         <v>8</v>
       </c>
       <c r="W19" s="2">
-        <v>7805</v>
+        <v>7499</v>
       </c>
       <c r="X19" s="2">
-        <v>1296</v>
+        <v>1256</v>
       </c>
       <c r="Y19" s="1">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="Z19" s="6">
         <f t="shared" si="3"/>
-        <v>2.0272727272727273</v>
+        <v>2.0083020889126941</v>
       </c>
       <c r="AA19" s="7">
         <f t="shared" si="4"/>
-        <v>0.33497027655724992</v>
+        <v>0.33736234219715283</v>
       </c>
       <c r="AB19" s="7">
         <f t="shared" si="5"/>
-        <v>0.21983420325452871</v>
+        <v>0.22543171114599686</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
@@ -2533,13 +2517,13 @@
         <v>0</v>
       </c>
       <c r="F20" s="2">
-        <v>4777</v>
+        <v>4513</v>
       </c>
       <c r="G20" s="2">
-        <v>4489</v>
+        <v>4330</v>
       </c>
       <c r="H20" s="2">
-        <v>2919</v>
+        <v>2991</v>
       </c>
       <c r="I20" s="2">
         <v>4</v>
@@ -2554,25 +2538,25 @@
         <v>4062</v>
       </c>
       <c r="M20" s="2">
-        <v>1667</v>
+        <v>1621</v>
       </c>
       <c r="N20" s="2">
-        <v>1804</v>
+        <v>1741</v>
       </c>
       <c r="O20" s="1">
-        <v>855</v>
+        <v>860</v>
       </c>
       <c r="P20" s="6">
         <f t="shared" si="0"/>
-        <v>0.3489637848021771</v>
+        <v>0.3591845778861068</v>
       </c>
       <c r="Q20" s="6">
         <f t="shared" si="1"/>
-        <v>0.401871240810871</v>
+        <v>0.4020785219399538</v>
       </c>
       <c r="R20" s="6">
         <f t="shared" si="2"/>
-        <v>0.29290853031860226</v>
+        <v>0.28752925442995653</v>
       </c>
       <c r="S20" s="2">
         <v>0</v>
@@ -2587,25 +2571,25 @@
         <v>0</v>
       </c>
       <c r="W20" s="2">
-        <v>2267</v>
+        <v>2178</v>
       </c>
       <c r="X20" s="2">
-        <v>1645</v>
+        <v>1597</v>
       </c>
       <c r="Y20" s="1">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="Z20" s="6">
         <f t="shared" si="3"/>
-        <v>0.4745656269625288</v>
+        <v>0.48260580545091958</v>
       </c>
       <c r="AA20" s="7">
         <f t="shared" si="4"/>
-        <v>0.36645132546224102</v>
+        <v>0.36882217090069286</v>
       </c>
       <c r="AB20" s="7">
         <f t="shared" si="5"/>
-        <v>0.36348064405618363</v>
+        <v>0.35406218655967903</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
@@ -2625,13 +2609,13 @@
         <v>0</v>
       </c>
       <c r="F21" s="2">
-        <v>4826</v>
+        <v>4571</v>
       </c>
       <c r="G21" s="2">
-        <v>4406</v>
+        <v>4248</v>
       </c>
       <c r="H21" s="2">
-        <v>3035</v>
+        <v>3024</v>
       </c>
       <c r="I21" s="2">
         <v>2</v>
@@ -2646,25 +2630,25 @@
         <v>6154</v>
       </c>
       <c r="M21" s="2">
-        <v>1643</v>
+        <v>1592</v>
       </c>
       <c r="N21" s="2">
-        <v>1576</v>
+        <v>1523</v>
       </c>
       <c r="O21" s="1">
-        <v>827</v>
+        <v>830</v>
       </c>
       <c r="P21" s="6">
         <f t="shared" si="0"/>
-        <v>0.34044757563199335</v>
+        <v>0.34828265149857801</v>
       </c>
       <c r="Q21" s="6">
         <f t="shared" si="1"/>
-        <v>0.35769405356332273</v>
+        <v>0.3585216572504708</v>
       </c>
       <c r="R21" s="6">
         <f t="shared" si="2"/>
-        <v>0.27248764415156507</v>
+        <v>0.27447089947089948</v>
       </c>
       <c r="S21" s="2">
         <v>0</v>
@@ -2679,25 +2663,25 @@
         <v>0</v>
       </c>
       <c r="W21" s="2">
-        <v>2257</v>
+        <v>2187</v>
       </c>
       <c r="X21" s="2">
-        <v>1626</v>
+        <v>1570</v>
       </c>
       <c r="Y21" s="1">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="Z21" s="6">
         <f t="shared" si="3"/>
-        <v>0.46767509324492335</v>
+        <v>0.47845110479107417</v>
       </c>
       <c r="AA21" s="7">
         <f t="shared" si="4"/>
-        <v>0.36904221516114388</v>
+        <v>0.36958568738229758</v>
       </c>
       <c r="AB21" s="7">
         <f t="shared" si="5"/>
-        <v>0.34365733113673808</v>
+        <v>0.34424603174603174</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
@@ -2717,13 +2701,13 @@
         <v>0</v>
       </c>
       <c r="F22" s="2">
-        <v>6080</v>
+        <v>5920</v>
       </c>
       <c r="G22" s="2">
-        <v>5414</v>
+        <v>5268</v>
       </c>
       <c r="H22" s="2">
-        <v>3712</v>
+        <v>3778</v>
       </c>
       <c r="I22" s="2">
         <v>6</v>
@@ -2738,25 +2722,25 @@
         <v>3525</v>
       </c>
       <c r="M22" s="2">
-        <v>2251</v>
+        <v>2179</v>
       </c>
       <c r="N22" s="2">
-        <v>1545</v>
+        <v>1500</v>
       </c>
       <c r="O22" s="1">
-        <v>744</v>
+        <v>763</v>
       </c>
       <c r="P22" s="6">
         <f t="shared" si="0"/>
-        <v>0.37023026315789476</v>
+        <v>0.3680743243243243</v>
       </c>
       <c r="Q22" s="6">
         <f t="shared" si="1"/>
-        <v>0.28537125969708166</v>
+        <v>0.2847380410022779</v>
       </c>
       <c r="R22" s="6">
         <f t="shared" si="2"/>
-        <v>0.20043103448275862</v>
+        <v>0.2019587083112758</v>
       </c>
       <c r="S22" s="2">
         <v>0</v>
@@ -2771,25 +2755,25 @@
         <v>0</v>
       </c>
       <c r="W22" s="2">
-        <v>2867</v>
+        <v>2760</v>
       </c>
       <c r="X22" s="2">
-        <v>2158</v>
+        <v>2084</v>
       </c>
       <c r="Y22" s="1">
-        <v>1162</v>
+        <v>1166</v>
       </c>
       <c r="Z22" s="6">
         <f t="shared" si="3"/>
-        <v>0.47154605263157895</v>
+        <v>0.46621621621621623</v>
       </c>
       <c r="AA22" s="7">
         <f t="shared" si="4"/>
-        <v>0.39859623199113409</v>
+        <v>0.39559605163249811</v>
       </c>
       <c r="AB22" s="7">
         <f t="shared" si="5"/>
-        <v>0.31303879310344829</v>
+        <v>0.30862890418210692</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
@@ -2809,13 +2793,13 @@
         <v>0</v>
       </c>
       <c r="F23" s="2">
-        <v>1640</v>
+        <v>1574</v>
       </c>
       <c r="G23" s="2">
-        <v>1542</v>
+        <v>1493</v>
       </c>
       <c r="H23">
-        <v>1172</v>
+        <v>1217</v>
       </c>
       <c r="I23" s="2">
         <v>0</v>
@@ -2830,25 +2814,25 @@
         <v>4057</v>
       </c>
       <c r="M23" s="2">
-        <v>744</v>
+        <v>698</v>
       </c>
       <c r="N23" s="2">
-        <v>698</v>
+        <v>674</v>
       </c>
       <c r="O23" s="1">
-        <v>301</v>
+        <v>313</v>
       </c>
       <c r="P23" s="6">
         <f t="shared" si="0"/>
-        <v>0.45365853658536587</v>
+        <v>0.4434561626429479</v>
       </c>
       <c r="Q23" s="6">
         <f t="shared" si="1"/>
-        <v>0.45265888456549935</v>
+        <v>0.45144005358338912</v>
       </c>
       <c r="R23" s="6">
         <f t="shared" si="2"/>
-        <v>0.25682593856655289</v>
+        <v>0.257189811010682</v>
       </c>
       <c r="S23" s="2">
         <v>0</v>
@@ -2863,25 +2847,25 @@
         <v>0</v>
       </c>
       <c r="W23" s="2">
-        <v>1033</v>
+        <v>943</v>
       </c>
       <c r="X23" s="2">
-        <v>822</v>
+        <v>793</v>
       </c>
       <c r="Y23" s="1">
-        <v>536</v>
+        <v>561</v>
       </c>
       <c r="Z23" s="6">
         <f t="shared" si="3"/>
-        <v>0.62987804878048781</v>
+        <v>0.59911054637865313</v>
       </c>
       <c r="AA23" s="7">
         <f t="shared" si="4"/>
-        <v>0.53307392996108949</v>
+        <v>0.53114534494306764</v>
       </c>
       <c r="AB23" s="7">
         <f t="shared" si="5"/>
-        <v>0.45733788395904434</v>
+        <v>0.46096959737058341</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
@@ -2901,13 +2885,13 @@
         <v>0</v>
       </c>
       <c r="F24" s="2">
-        <v>3908</v>
+        <v>3764</v>
       </c>
       <c r="G24" s="2">
-        <v>3876</v>
+        <v>3768</v>
       </c>
       <c r="H24" s="2">
-        <v>2753</v>
+        <v>2769</v>
       </c>
       <c r="I24" s="2">
         <v>3</v>
@@ -2922,25 +2906,25 @@
         <v>1</v>
       </c>
       <c r="M24" s="2">
-        <v>722</v>
+        <v>700</v>
       </c>
       <c r="N24" s="2">
-        <v>719</v>
+        <v>696</v>
       </c>
       <c r="O24" s="1">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="P24" s="6">
         <f t="shared" si="0"/>
-        <v>0.18474923234390994</v>
+        <v>0.18597236981934112</v>
       </c>
       <c r="Q24" s="6">
         <f t="shared" si="1"/>
-        <v>0.18550051599587203</v>
+        <v>0.18471337579617833</v>
       </c>
       <c r="R24" s="6">
         <f t="shared" si="2"/>
-        <v>0.12350163458045768</v>
+        <v>0.12387143373058866</v>
       </c>
       <c r="S24" s="2">
         <v>0</v>
@@ -2955,25 +2939,25 @@
         <v>0</v>
       </c>
       <c r="W24" s="2">
-        <v>1005</v>
+        <v>971</v>
       </c>
       <c r="X24" s="2">
-        <v>807</v>
+        <v>779</v>
       </c>
       <c r="Y24" s="1">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="Z24" s="6">
         <f t="shared" si="3"/>
-        <v>0.25716479017400207</v>
+        <v>0.25797024442082889</v>
       </c>
       <c r="AA24" s="7">
         <f t="shared" si="4"/>
-        <v>0.20820433436532507</v>
+        <v>0.20674097664543525</v>
       </c>
       <c r="AB24" s="7">
         <f t="shared" si="5"/>
-        <v>0.19469669451507446</v>
+        <v>0.19465511014806788</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
@@ -2993,13 +2977,13 @@
         <v>0</v>
       </c>
       <c r="F25" s="2">
-        <v>4135</v>
+        <v>4016</v>
       </c>
       <c r="G25" s="2">
-        <v>3650</v>
+        <v>3554</v>
       </c>
       <c r="H25" s="2">
-        <v>2654</v>
+        <v>2566</v>
       </c>
       <c r="I25" s="2">
         <v>6</v>
@@ -3014,25 +2998,25 @@
         <v>3525</v>
       </c>
       <c r="M25" s="2">
-        <v>1999</v>
+        <v>2067</v>
       </c>
       <c r="N25" s="2">
-        <v>1661</v>
+        <v>1606</v>
       </c>
       <c r="O25" s="1">
-        <v>865</v>
+        <v>875</v>
       </c>
       <c r="P25" s="6">
         <f t="shared" si="0"/>
-        <v>0.48343409915356711</v>
+        <v>0.514691235059761</v>
       </c>
       <c r="Q25" s="6">
         <f t="shared" si="1"/>
-        <v>0.45506849315068493</v>
+        <v>0.45188519977490155</v>
       </c>
       <c r="R25" s="6">
         <f t="shared" si="2"/>
-        <v>0.32592313489073099</v>
+        <v>0.34099766173031959</v>
       </c>
       <c r="S25" s="2">
         <v>0</v>
@@ -3047,25 +3031,25 @@
         <v>0</v>
       </c>
       <c r="W25" s="2">
-        <v>2795</v>
+        <v>2695</v>
       </c>
       <c r="X25" s="2">
-        <v>1908</v>
+        <v>1844</v>
       </c>
       <c r="Y25" s="1">
-        <v>1281</v>
+        <v>1293</v>
       </c>
       <c r="Z25" s="6">
         <f t="shared" si="3"/>
-        <v>0.67593712212817414</v>
+        <v>0.67106573705179284</v>
       </c>
       <c r="AA25" s="7">
         <f t="shared" si="4"/>
-        <v>0.52273972602739727</v>
+        <v>0.51885199774901525</v>
       </c>
       <c r="AB25" s="7">
         <f t="shared" si="5"/>
-        <v>0.48266767143933687</v>
+        <v>0.50389711613406074</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
@@ -3085,13 +3069,13 @@
         <v>4083</v>
       </c>
       <c r="F26" s="2">
-        <v>7120</v>
+        <v>6845</v>
       </c>
       <c r="G26" s="2">
-        <v>6255</v>
+        <v>5971</v>
       </c>
       <c r="H26" s="2">
-        <v>4136</v>
+        <v>4193</v>
       </c>
       <c r="I26" s="2">
         <v>377</v>
@@ -3106,25 +3090,25 @@
         <v>1176</v>
       </c>
       <c r="M26" s="2">
-        <v>5465</v>
+        <v>5158</v>
       </c>
       <c r="N26" s="2">
-        <v>2244</v>
+        <v>2169</v>
       </c>
       <c r="O26" s="1">
-        <v>1358</v>
+        <v>1355</v>
       </c>
       <c r="P26" s="6">
         <f t="shared" si="0"/>
-        <v>0.7675561797752809</v>
+        <v>0.75354273192111032</v>
       </c>
       <c r="Q26" s="6">
         <f t="shared" si="1"/>
-        <v>0.35875299760191848</v>
+        <v>0.3632557360576118</v>
       </c>
       <c r="R26" s="6">
         <f t="shared" si="2"/>
-        <v>0.32833655705996134</v>
+        <v>0.32315764369186739</v>
       </c>
       <c r="S26" s="2">
         <v>0</v>
@@ -3139,25 +3123,25 @@
         <v>0</v>
       </c>
       <c r="W26" s="2">
-        <v>5610</v>
+        <v>5370</v>
       </c>
       <c r="X26" s="2">
-        <v>3062</v>
+        <v>2969</v>
       </c>
       <c r="Y26" s="1">
-        <v>1832</v>
+        <v>1837</v>
       </c>
       <c r="Z26" s="6">
         <f t="shared" si="3"/>
-        <v>0.7879213483146067</v>
+        <v>0.7845142439737034</v>
       </c>
       <c r="AA26" s="7">
         <f t="shared" si="4"/>
-        <v>0.48952837729816145</v>
+        <v>0.4972366437782616</v>
       </c>
       <c r="AB26" s="7">
         <f t="shared" si="5"/>
-        <v>0.44294003868471954</v>
+        <v>0.4381111376103029</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
@@ -3177,13 +3161,13 @@
         <v>0</v>
       </c>
       <c r="F27" s="2">
-        <v>6467</v>
+        <v>6162</v>
       </c>
       <c r="G27" s="2">
-        <v>5960</v>
+        <v>5724</v>
       </c>
       <c r="H27" s="2">
-        <v>5251</v>
+        <v>5306</v>
       </c>
       <c r="I27" s="2">
         <v>2</v>
@@ -3198,25 +3182,25 @@
         <v>13892</v>
       </c>
       <c r="M27" s="2">
-        <v>10723</v>
+        <v>10265</v>
       </c>
       <c r="N27" s="2">
-        <v>2900</v>
+        <v>3081</v>
       </c>
       <c r="O27" s="1">
-        <v>1824</v>
+        <v>1809</v>
       </c>
       <c r="P27" s="6">
         <f t="shared" si="0"/>
-        <v>1.658110406680068</v>
+        <v>1.6658552418046089</v>
       </c>
       <c r="Q27" s="6">
         <f t="shared" si="1"/>
-        <v>0.48657718120805371</v>
+        <v>0.5382599580712788</v>
       </c>
       <c r="R27" s="6">
         <f t="shared" si="2"/>
-        <v>0.34736240716054084</v>
+        <v>0.34093479080286471</v>
       </c>
       <c r="S27" s="2">
         <v>0</v>
@@ -3231,25 +3215,25 @@
         <v>6771</v>
       </c>
       <c r="W27" s="2">
-        <v>10761</v>
+        <v>10389</v>
       </c>
       <c r="X27" s="2">
-        <v>2960</v>
+        <v>2861</v>
       </c>
       <c r="Y27" s="1">
-        <v>2112</v>
+        <v>2089</v>
       </c>
       <c r="Z27" s="6">
         <f t="shared" si="3"/>
-        <v>1.6639863924539973</v>
+        <v>1.6859785783836416</v>
       </c>
       <c r="AA27" s="7">
         <f t="shared" si="4"/>
-        <v>0.49664429530201343</v>
+        <v>0.4998252969951083</v>
       </c>
       <c r="AB27" s="7">
         <f t="shared" si="5"/>
-        <v>0.40220910302799467</v>
+        <v>0.39370523935167734</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
@@ -3269,13 +3253,13 @@
         <v>0</v>
       </c>
       <c r="F28" s="2">
-        <v>7398</v>
+        <v>7139</v>
       </c>
       <c r="G28" s="2">
-        <v>6710</v>
+        <v>6439</v>
       </c>
       <c r="H28" s="2">
-        <v>5789</v>
+        <v>5912</v>
       </c>
       <c r="I28" s="2">
         <v>2</v>
@@ -3290,25 +3274,25 @@
         <v>19670</v>
       </c>
       <c r="M28" s="2">
-        <v>10703</v>
+        <v>10215</v>
       </c>
       <c r="N28" s="2">
-        <v>2924</v>
+        <v>3116</v>
       </c>
       <c r="O28" s="1">
-        <v>1852</v>
+        <v>1834</v>
       </c>
       <c r="P28" s="6">
         <f t="shared" si="0"/>
-        <v>1.446742362800757</v>
+        <v>1.4308726712424709</v>
       </c>
       <c r="Q28" s="6">
         <f t="shared" si="1"/>
-        <v>0.43576751117734724</v>
+        <v>0.48392607547755861</v>
       </c>
       <c r="R28" s="6">
         <f t="shared" si="2"/>
-        <v>0.31991708412506475</v>
+        <v>0.31021650879566981</v>
       </c>
       <c r="S28" s="2">
         <v>0</v>
@@ -3323,25 +3307,25 @@
         <v>13542</v>
       </c>
       <c r="W28" s="2">
-        <v>10760</v>
+        <v>10397</v>
       </c>
       <c r="X28" s="2">
-        <v>2923</v>
+        <v>2952</v>
       </c>
       <c r="Y28" s="1">
-        <v>2003</v>
+        <v>2015</v>
       </c>
       <c r="Z28" s="6">
         <f t="shared" si="3"/>
-        <v>1.4544471478778047</v>
+        <v>1.4563664378764534</v>
       </c>
       <c r="AA28" s="7">
         <f t="shared" si="4"/>
-        <v>0.43561847988077496</v>
+        <v>0.45845628203137134</v>
       </c>
       <c r="AB28" s="7">
         <f t="shared" si="5"/>
-        <v>0.34600103644843672</v>
+        <v>0.34083220568335587</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
@@ -3361,13 +3345,13 @@
         <v>0</v>
       </c>
       <c r="F29" s="2">
-        <v>3030</v>
+        <v>2928</v>
       </c>
       <c r="G29" s="2">
-        <v>2657</v>
+        <v>2543</v>
       </c>
       <c r="H29">
-        <v>2246</v>
+        <v>2299</v>
       </c>
       <c r="I29" s="2">
         <v>0</v>
@@ -3382,25 +3366,25 @@
         <v>16707</v>
       </c>
       <c r="M29" s="2">
-        <v>5073</v>
+        <v>4766</v>
       </c>
       <c r="N29" s="2">
-        <v>1634</v>
+        <v>1578</v>
       </c>
       <c r="O29" s="1">
-        <v>796</v>
+        <v>829</v>
       </c>
       <c r="P29" s="6">
         <f t="shared" si="0"/>
-        <v>1.6742574257425742</v>
+        <v>1.6277322404371584</v>
       </c>
       <c r="Q29" s="6">
         <f t="shared" si="1"/>
-        <v>0.61497929996236356</v>
+        <v>0.62052693668895009</v>
       </c>
       <c r="R29" s="6">
         <f t="shared" si="2"/>
-        <v>0.35440783615316118</v>
+        <v>0.36059156154849936</v>
       </c>
       <c r="S29" s="2">
         <v>0</v>
@@ -3415,25 +3399,25 @@
         <v>12097</v>
       </c>
       <c r="W29" s="2">
-        <v>5222</v>
+        <v>5133</v>
       </c>
       <c r="X29" s="2">
-        <v>1641</v>
+        <v>1585</v>
       </c>
       <c r="Y29" s="1">
-        <v>1158</v>
+        <v>1191</v>
       </c>
       <c r="Z29" s="6">
         <f t="shared" si="3"/>
-        <v>1.7234323432343235</v>
+        <v>1.7530737704918034</v>
       </c>
       <c r="AA29" s="7">
         <f t="shared" si="4"/>
-        <v>0.61761385020700033</v>
+        <v>0.6232795910342116</v>
       </c>
       <c r="AB29" s="7">
         <f t="shared" si="5"/>
-        <v>0.51558325912733749</v>
+        <v>0.51805132666376685</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
@@ -3453,13 +3437,13 @@
         <v>0</v>
       </c>
       <c r="F30" s="2">
-        <v>8414</v>
+        <v>8087</v>
       </c>
       <c r="G30" s="2">
-        <v>8162</v>
+        <v>7889</v>
       </c>
       <c r="H30" s="2">
-        <v>6956</v>
+        <v>7166</v>
       </c>
       <c r="I30" s="2">
         <v>4</v>
@@ -3474,25 +3458,25 @@
         <v>4490</v>
       </c>
       <c r="M30" s="2">
-        <v>4216</v>
+        <v>4144</v>
       </c>
       <c r="N30" s="2">
-        <v>3044</v>
+        <v>2955</v>
       </c>
       <c r="O30" s="1">
-        <v>1892</v>
+        <v>1914</v>
       </c>
       <c r="P30" s="6">
         <f t="shared" si="0"/>
-        <v>0.50106964582838132</v>
+        <v>0.51242735254111538</v>
       </c>
       <c r="Q30" s="6">
         <f t="shared" si="1"/>
-        <v>0.37294780691007107</v>
+        <v>0.37457218912409684</v>
       </c>
       <c r="R30" s="6">
         <f t="shared" si="2"/>
-        <v>0.2719953996549741</v>
+        <v>0.2670946134524142</v>
       </c>
       <c r="S30" s="2">
         <v>0</v>
@@ -3507,25 +3491,25 @@
         <v>0</v>
       </c>
       <c r="W30" s="2">
-        <v>4354</v>
+        <v>4181</v>
       </c>
       <c r="X30" s="2">
-        <v>3440</v>
+        <v>3331</v>
       </c>
       <c r="Y30" s="1">
-        <v>2212</v>
+        <v>2239</v>
       </c>
       <c r="Z30" s="6">
         <f t="shared" si="3"/>
-        <v>0.51747088186356072</v>
+        <v>0.51700259676023252</v>
       </c>
       <c r="AA30" s="7">
         <f t="shared" si="4"/>
-        <v>0.4214653271257045</v>
+        <v>0.42223348966915958</v>
       </c>
       <c r="AB30" s="7">
         <f t="shared" si="5"/>
-        <v>0.31799884991374355</v>
+        <v>0.31244766955065589</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
@@ -3545,13 +3529,13 @@
         <v>0</v>
       </c>
       <c r="F31" s="2">
-        <v>3169</v>
+        <v>3052</v>
       </c>
       <c r="G31" s="2">
-        <v>2747</v>
+        <v>2710</v>
       </c>
       <c r="H31" s="2">
-        <v>2478</v>
+        <v>2489</v>
       </c>
       <c r="I31" s="2">
         <v>1</v>
@@ -3566,25 +3550,25 @@
         <v>1</v>
       </c>
       <c r="M31" s="2">
-        <v>945</v>
+        <v>916</v>
       </c>
       <c r="N31" s="2">
-        <v>599</v>
+        <v>574</v>
       </c>
       <c r="O31" s="1">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="P31" s="6">
         <f t="shared" si="0"/>
-        <v>0.29820132533922372</v>
+        <v>0.30013106159895153</v>
       </c>
       <c r="Q31" s="6">
         <f t="shared" si="1"/>
-        <v>0.21805606115762649</v>
+        <v>0.2118081180811808</v>
       </c>
       <c r="R31" s="6">
         <f t="shared" si="2"/>
-        <v>0.10734463276836158</v>
+        <v>0.10727199678585778</v>
       </c>
       <c r="S31" s="2">
         <v>0</v>
@@ -3599,25 +3583,25 @@
         <v>0</v>
       </c>
       <c r="W31" s="2">
-        <v>939</v>
+        <v>902</v>
       </c>
       <c r="X31" s="2">
-        <v>676</v>
+        <v>656</v>
       </c>
       <c r="Y31" s="1">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="Z31" s="6">
         <f t="shared" si="3"/>
-        <v>0.29630798359103816</v>
+        <v>0.29554390563564875</v>
       </c>
       <c r="AA31" s="7">
         <f t="shared" si="4"/>
-        <v>0.24608663997087732</v>
+        <v>0.24206642066420664</v>
       </c>
       <c r="AB31" s="7">
         <f t="shared" si="5"/>
-        <v>0.1529459241323648</v>
+        <v>0.14985938127762152</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
@@ -3637,13 +3621,13 @@
         <v>0</v>
       </c>
       <c r="F32" s="2">
-        <v>1699</v>
+        <v>1626</v>
       </c>
       <c r="G32" s="2">
-        <v>1446</v>
+        <v>1407</v>
       </c>
       <c r="H32">
-        <v>1135</v>
+        <v>1273</v>
       </c>
       <c r="I32" s="2">
         <v>0</v>
@@ -3658,25 +3642,25 @@
         <v>3009</v>
       </c>
       <c r="M32" s="2">
-        <v>1731</v>
+        <v>1680</v>
       </c>
       <c r="N32" s="2">
-        <v>1166</v>
+        <v>1130</v>
       </c>
       <c r="O32" s="1">
-        <v>585</v>
+        <v>611</v>
       </c>
       <c r="P32" s="6">
         <f t="shared" si="0"/>
-        <v>1.0188346085932902</v>
+        <v>1.033210332103321</v>
       </c>
       <c r="Q32" s="6">
         <f t="shared" si="1"/>
-        <v>0.80636237897648688</v>
+        <v>0.80312722103766876</v>
       </c>
       <c r="R32" s="6">
         <f t="shared" si="2"/>
-        <v>0.51541850220264318</v>
+        <v>0.47996857816182248</v>
       </c>
       <c r="S32" s="2">
         <v>0</v>
@@ -3691,25 +3675,25 @@
         <v>0</v>
       </c>
       <c r="W32" s="2">
-        <v>1904</v>
+        <v>1838</v>
       </c>
       <c r="X32" s="2">
-        <v>1351</v>
+        <v>1304</v>
       </c>
       <c r="Y32" s="1">
-        <v>781</v>
+        <v>823</v>
       </c>
       <c r="Z32" s="6">
         <f t="shared" si="3"/>
-        <v>1.1206592113007652</v>
+        <v>1.1303813038130381</v>
       </c>
       <c r="AA32" s="7">
         <f t="shared" si="4"/>
-        <v>0.93430152143845091</v>
+        <v>0.92679459843638945</v>
       </c>
       <c r="AB32" s="7">
         <f t="shared" si="5"/>
-        <v>0.68810572687224669</v>
+        <v>0.64650432050274942</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.25">
@@ -3729,13 +3713,13 @@
         <v>153</v>
       </c>
       <c r="F33" s="2">
-        <v>5558</v>
+        <v>5382</v>
       </c>
       <c r="G33" s="2">
-        <v>7603</v>
+        <v>7250</v>
       </c>
       <c r="H33" s="2">
-        <v>6171</v>
+        <v>6044</v>
       </c>
       <c r="I33" s="2">
         <v>2</v>
@@ -3750,25 +3734,25 @@
         <v>14432</v>
       </c>
       <c r="M33" s="2">
-        <v>2133</v>
+        <v>2095</v>
       </c>
       <c r="N33" s="2">
-        <v>1536</v>
+        <v>1484</v>
       </c>
       <c r="O33" s="2">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c r="P33" s="13">
         <f t="shared" si="0"/>
-        <v>0.38377114069809282</v>
+        <v>0.38926049795615014</v>
       </c>
       <c r="Q33" s="13">
         <f t="shared" si="1"/>
-        <v>0.20202551624358805</v>
+        <v>0.2046896551724138</v>
       </c>
       <c r="R33" s="6">
         <f t="shared" si="2"/>
-        <v>0.11165127207907957</v>
+        <v>0.11465916611515553</v>
       </c>
       <c r="S33" s="2">
         <v>0</v>
@@ -3783,25 +3767,25 @@
         <v>13864</v>
       </c>
       <c r="W33" s="2">
-        <v>3013</v>
+        <v>2882</v>
       </c>
       <c r="X33" s="2">
-        <v>1787</v>
+        <v>1740</v>
       </c>
       <c r="Y33" s="2">
-        <v>1152</v>
+        <v>1178</v>
       </c>
       <c r="Z33" s="13">
         <f t="shared" si="3"/>
-        <v>0.54210147535084563</v>
+        <v>0.53548866592344857</v>
       </c>
       <c r="AA33" s="14">
         <f t="shared" si="4"/>
-        <v>0.23503880047349732</v>
+        <v>0.24</v>
       </c>
       <c r="AB33" s="7">
         <f t="shared" si="5"/>
-        <v>0.18667963052989792</v>
+        <v>0.19490403706154863</v>
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
@@ -3821,13 +3805,13 @@
         <v>185</v>
       </c>
       <c r="F34" s="2">
-        <v>5174</v>
+        <v>5000</v>
       </c>
       <c r="G34" s="2">
-        <v>7370</v>
+        <v>7099</v>
       </c>
       <c r="H34" s="2">
-        <v>6082</v>
+        <v>5938</v>
       </c>
       <c r="I34" s="2">
         <v>2</v>
@@ -3842,25 +3826,25 @@
         <v>14454</v>
       </c>
       <c r="M34" s="2">
-        <v>4815</v>
+        <v>4663</v>
       </c>
       <c r="N34" s="2">
-        <v>2621</v>
+        <v>2531</v>
       </c>
       <c r="O34" s="2">
-        <v>1477</v>
+        <v>1524</v>
       </c>
       <c r="P34" s="13">
         <f t="shared" si="0"/>
-        <v>0.93061461151913416</v>
+        <v>0.93259999999999998</v>
       </c>
       <c r="Q34" s="13">
         <f t="shared" si="1"/>
-        <v>0.35563093622795117</v>
+        <v>0.35652908860402871</v>
       </c>
       <c r="R34" s="6">
         <f t="shared" si="2"/>
-        <v>0.24284774745149623</v>
+        <v>0.25665207140451329</v>
       </c>
       <c r="S34" s="2">
         <v>0</v>
@@ -3875,25 +3859,25 @@
         <v>13867</v>
       </c>
       <c r="W34" s="2">
-        <v>5450</v>
+        <v>5242</v>
       </c>
       <c r="X34" s="2">
-        <v>2952</v>
+        <v>2855</v>
       </c>
       <c r="Y34" s="2">
-        <v>1907</v>
+        <v>1897</v>
       </c>
       <c r="Z34" s="13">
         <f t="shared" si="3"/>
-        <v>1.0533436412833397</v>
+        <v>1.0484</v>
       </c>
       <c r="AA34" s="14">
         <f t="shared" si="4"/>
-        <v>0.4005427408412483</v>
+        <v>0.40216931962248204</v>
       </c>
       <c r="AB34" s="7">
         <f t="shared" si="5"/>
-        <v>0.31354817494245313</v>
+        <v>0.31946783428763892</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.25">
@@ -3913,13 +3897,13 @@
         <v>16</v>
       </c>
       <c r="F35" s="2">
-        <v>25318</v>
+        <v>24650</v>
       </c>
       <c r="G35" s="2">
-        <v>30673</v>
-      </c>
-      <c r="H35" s="28">
-        <v>22222</v>
+        <v>29508</v>
+      </c>
+      <c r="H35" s="2">
+        <v>25902</v>
       </c>
       <c r="I35" s="2">
         <v>6</v>
@@ -3934,25 +3918,25 @@
         <v>6</v>
       </c>
       <c r="M35" s="2">
-        <v>9189</v>
+        <v>8841</v>
       </c>
       <c r="N35" s="2">
-        <v>5850</v>
+        <v>5647</v>
       </c>
       <c r="O35" s="2">
-        <v>3916</v>
+        <v>3906</v>
       </c>
       <c r="P35" s="13">
         <f t="shared" si="0"/>
-        <v>0.36294336045501224</v>
+        <v>0.35866125760649087</v>
       </c>
       <c r="Q35" s="13">
         <f t="shared" si="1"/>
-        <v>0.19072148143318227</v>
+        <v>0.19137183136776467</v>
       </c>
       <c r="R35" s="6">
         <f t="shared" si="2"/>
-        <v>0.17622176221762217</v>
+        <v>0.1507991660875608</v>
       </c>
       <c r="S35" s="2">
         <v>0</v>
@@ -3967,25 +3951,25 @@
         <v>0</v>
       </c>
       <c r="W35" s="2">
-        <v>10270</v>
+        <v>9901</v>
       </c>
       <c r="X35" s="2">
-        <v>7386</v>
+        <v>7156</v>
       </c>
       <c r="Y35" s="2">
-        <v>5196</v>
+        <v>5230</v>
       </c>
       <c r="Z35" s="13">
         <f t="shared" si="3"/>
-        <v>0.40564025594438741</v>
+        <v>0.40166328600405682</v>
       </c>
       <c r="AA35" s="14">
         <f t="shared" si="4"/>
-        <v>0.24079809604538194</v>
+        <v>0.24251050562559306</v>
       </c>
       <c r="AB35" s="7">
         <f t="shared" si="5"/>
-        <v>0.23382233822338222</v>
+        <v>0.20191491004555634</v>
       </c>
     </row>
     <row r="36" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4005,13 +3989,13 @@
         <v>56</v>
       </c>
       <c r="F36" s="9">
-        <v>23520</v>
+        <v>22880</v>
       </c>
       <c r="G36" s="9">
-        <v>23455</v>
-      </c>
-      <c r="H36" s="29">
-        <v>22222</v>
+        <v>22440</v>
+      </c>
+      <c r="H36" s="9">
+        <v>19388</v>
       </c>
       <c r="I36" s="9">
         <v>2</v>
@@ -4026,25 +4010,25 @@
         <v>13140</v>
       </c>
       <c r="M36" s="9">
-        <v>9580</v>
+        <v>9274</v>
       </c>
       <c r="N36" s="9">
-        <v>5206</v>
+        <v>5024</v>
       </c>
       <c r="O36" s="9">
-        <v>3489</v>
+        <v>3482</v>
       </c>
       <c r="P36" s="10">
         <f t="shared" si="0"/>
-        <v>0.40731292517006801</v>
+        <v>0.40533216783216786</v>
       </c>
       <c r="Q36" s="10">
         <f t="shared" si="1"/>
-        <v>0.22195693881901513</v>
+        <v>0.22388591800356505</v>
       </c>
       <c r="R36" s="10">
         <f t="shared" si="2"/>
-        <v>0.15700657006570065</v>
+        <v>0.17959562616051167</v>
       </c>
       <c r="S36" s="9">
         <v>0</v>
@@ -4059,25 +4043,25 @@
         <v>9794</v>
       </c>
       <c r="W36" s="9">
-        <v>23473</v>
+        <v>22756</v>
       </c>
       <c r="X36" s="9">
-        <v>15871</v>
+        <v>15345</v>
       </c>
       <c r="Y36" s="9">
-        <v>11068</v>
+        <v>11097</v>
       </c>
       <c r="Z36" s="10">
         <f t="shared" si="3"/>
-        <v>0.99800170068027216</v>
+        <v>0.99458041958041954</v>
       </c>
       <c r="AA36" s="11">
         <f t="shared" si="4"/>
-        <v>0.6766574291195907</v>
+        <v>0.68382352941176472</v>
       </c>
       <c r="AB36" s="11">
         <f t="shared" si="5"/>
-        <v>0.49806498064980648</v>
+        <v>0.57236434908190637</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
@@ -4124,15 +4108,15 @@
       <c r="O37" s="1"/>
       <c r="P37" s="15">
         <f>AVERAGE(P3:P6)</f>
-        <v>0.68547762996496131</v>
+        <v>0.70414225965227528</v>
       </c>
       <c r="Q37" s="15">
         <f>AVERAGE(Q3:Q6)</f>
-        <v>0.76018744368158753</v>
+        <v>0.75674192867173617</v>
       </c>
       <c r="R37" s="15">
         <f>AVERAGE(R3:R6)</f>
-        <v>0.14635916470125376</v>
+        <v>0.14913795519542206</v>
       </c>
       <c r="S37" s="23">
         <f>COUNTIF(S3:S6,"=0")/COUNTA(S3:S6)</f>
@@ -4155,15 +4139,15 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="15">
         <f>AVERAGE(Z3:Z6)</f>
-        <v>1.3107079015670604</v>
+        <v>1.3363993510548642</v>
       </c>
       <c r="AA37" s="16">
         <f>AVERAGE(AA3:AA6)</f>
-        <v>0.87851052170311994</v>
+        <v>0.87297178108507167</v>
       </c>
       <c r="AB37" s="16">
         <f>AVERAGE(AB3:AB6)</f>
-        <v>0.63977984904697816</v>
+        <v>0.64763442448512232</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
@@ -4210,15 +4194,15 @@
       <c r="O38" s="2"/>
       <c r="P38" s="17">
         <f>AVERAGE(P7:P36)</f>
-        <v>0.61214851958657301</v>
+        <v>0.61282245912859745</v>
       </c>
       <c r="Q38" s="17">
         <f>AVERAGE(Q7:Q36)</f>
-        <v>0.39468712849572218</v>
+        <v>0.40017450834783452</v>
       </c>
       <c r="R38" s="17">
         <f>AVERAGE(R7:R36)</f>
-        <v>0.25899015235550887</v>
+        <v>0.25789012437565523</v>
       </c>
       <c r="S38" s="24">
         <f>COUNTIF(S7:S36,"=0")/COUNTA(S7:S36)</f>
@@ -4241,15 +4225,15 @@
       <c r="Y38" s="2"/>
       <c r="Z38" s="17">
         <f>AVERAGE(Z7:Z36)</f>
-        <v>0.78977516267503556</v>
+        <v>0.78140209808427419</v>
       </c>
       <c r="AA38" s="17">
         <f>AVERAGE(AA7:AA36)</f>
-        <v>0.45077046966479656</v>
+        <v>0.45329826232077536</v>
       </c>
       <c r="AB38" s="26">
         <f>AVERAGE(AB7:AB36)</f>
-        <v>0.35656474063864046</v>
+        <v>0.35730434911813835</v>
       </c>
       <c r="AC38" s="27"/>
     </row>
@@ -4297,15 +4281,15 @@
       <c r="O39" s="12"/>
       <c r="P39" s="18">
         <f>AVERAGE(P3:P36)</f>
-        <v>0.62077547374873621</v>
+        <v>0.62356596507255957</v>
       </c>
       <c r="Q39" s="18">
         <f>AVERAGE(Q3:Q36)</f>
-        <v>0.43768716557641224</v>
+        <v>0.44212361662123473</v>
       </c>
       <c r="R39" s="18">
         <f>AVERAGE(R3:R36)</f>
-        <v>0.24573944792559654</v>
+        <v>0.24509575153092189</v>
       </c>
       <c r="S39" s="25">
         <f>COUNTIF(S3:S36,"=0")/COUNTA(S3:S36)</f>
@@ -4328,15 +4312,15 @@
       <c r="Y39" s="12"/>
       <c r="Z39" s="18">
         <f>AVERAGE(Z3:Z36)</f>
-        <v>0.85106136725056791</v>
+        <v>0.84669589255140254</v>
       </c>
       <c r="AA39" s="19">
         <f>AVERAGE(AA3:AA36)</f>
-        <v>0.50109282872812877</v>
+        <v>0.50267161746951616</v>
       </c>
       <c r="AB39" s="19">
         <f>AVERAGE(AB3:AB36)</f>
-        <v>0.38988416515726837</v>
+        <v>0.39146082857307762</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved accuracy of atan2.
git-svn-id: https://svn.code.sf.net/p/half/code/trunk@406 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -123,15 +123,9 @@
     <t>fma</t>
   </si>
   <si>
-    <t>functions</t>
-  </si>
-  <si>
     <t>fdim</t>
   </si>
   <si>
-    <t>operators</t>
-  </si>
-  <si>
     <t>half accuracy</t>
   </si>
   <si>
@@ -175,13 +169,19 @@
   </si>
   <si>
     <t>F16C</t>
+  </si>
+  <si>
+    <t>ops</t>
+  </si>
+  <si>
+    <t>funcs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,16 +204,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -426,12 +438,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -467,14 +491,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -792,7 +821,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC39"/>
+  <dimension ref="A1:AC123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -801,142 +830,149 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="18" width="8.7109375" customWidth="1"/>
+    <col min="19" max="22" width="10.7109375" customWidth="1"/>
+    <col min="23" max="28" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="28"/>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31" t="s">
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31" t="s">
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31" t="s">
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="32"/>
-    </row>
-    <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="33"/>
+    </row>
+    <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="F2" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="L2" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="N2" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="O2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="29" t="s">
+      <c r="P2" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="T2" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="V2" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" s="30" t="s">
+      <c r="W2" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="X2" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="Y2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="N2" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="O2" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="P2" s="29" t="s">
+      <c r="Z2" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA2" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB2" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="Q2" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="R2" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="S2" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="T2" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="U2" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="V2" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="W2" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="X2" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y2" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z2" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA2" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB2" s="29" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC2" s="27"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +1064,7 @@
         <v>0.33285177694308005</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1120,7 +1156,7 @@
         <v>0.32530461887220175</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1212,7 +1248,7 @@
         <v>0.94806571277159513</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1304,9 +1340,9 @@
         <v>0.98431558935361219</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -1333,13 +1369,13 @@
         <v>0</v>
       </c>
       <c r="J7" s="2">
-        <v>11280</v>
+        <v>46123008</v>
       </c>
       <c r="K7" s="2">
-        <v>11348</v>
+        <v>46135296</v>
       </c>
       <c r="L7" s="2">
-        <v>11280</v>
+        <v>46123008</v>
       </c>
       <c r="M7" s="2">
         <v>719</v>
@@ -1396,7 +1432,7 @@
         <v>0.61019736842105265</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
@@ -1488,7 +1524,7 @@
         <v>0.4108442751207565</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
@@ -1580,7 +1616,7 @@
         <v>0.39304881165346284</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1672,7 +1708,7 @@
         <v>0.84330143540669855</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
@@ -1764,7 +1800,7 @@
         <v>0.35650040883074408</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
@@ -1856,7 +1892,7 @@
         <v>0.12080766598220397</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
@@ -1948,7 +1984,7 @@
         <v>0.12275955360162327</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -2040,7 +2076,7 @@
         <v>0.1883866710656549</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
@@ -2132,7 +2168,7 @@
         <v>0.17055003819709702</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -2321,16 +2357,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="2">
-        <v>0</v>
+        <v>8278</v>
       </c>
       <c r="C18" s="2">
-        <v>5</v>
+        <v>12013</v>
       </c>
       <c r="D18" s="2">
-        <v>6</v>
+        <v>12913</v>
       </c>
       <c r="E18" s="2">
-        <v>5</v>
+        <v>13016</v>
       </c>
       <c r="F18" s="2">
         <v>7346</v>
@@ -2342,16 +2378,16 @@
         <v>6399</v>
       </c>
       <c r="I18" s="2">
-        <v>53</v>
+        <v>64079</v>
       </c>
       <c r="J18" s="2">
-        <v>148538</v>
+        <v>601827096</v>
       </c>
       <c r="K18" s="2">
-        <v>146678</v>
+        <v>594665760</v>
       </c>
       <c r="L18" s="2">
-        <v>148569</v>
+        <v>601709992</v>
       </c>
       <c r="M18" s="2">
         <v>4044</v>
@@ -2375,16 +2411,16 @@
         <v>0.47538677918424754</v>
       </c>
       <c r="S18" s="2">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="T18" s="2">
-        <v>121437</v>
+        <v>495461850</v>
       </c>
       <c r="U18" s="2">
-        <v>120719</v>
+        <v>492989872</v>
       </c>
       <c r="V18" s="2">
-        <v>121458</v>
+        <v>495283947</v>
       </c>
       <c r="W18" s="2">
         <v>4505</v>
@@ -2434,16 +2470,16 @@
         <v>3185</v>
       </c>
       <c r="I19" s="2">
-        <v>13</v>
+        <v>50512</v>
       </c>
       <c r="J19" s="2">
-        <v>4</v>
+        <v>18280</v>
       </c>
       <c r="K19" s="2">
-        <v>377364</v>
+        <v>1558157760</v>
       </c>
       <c r="L19" s="2">
-        <v>4</v>
+        <v>18280</v>
       </c>
       <c r="M19" s="2">
         <v>1314</v>
@@ -2467,16 +2503,16 @@
         <v>0.10549450549450549</v>
       </c>
       <c r="S19" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T19" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="U19" s="2">
-        <v>26458</v>
+        <v>96159496</v>
       </c>
       <c r="V19" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="W19" s="2">
         <v>7499</v>
@@ -3057,54 +3093,54 @@
         <v>21</v>
       </c>
       <c r="B26" s="2">
-        <v>1967</v>
+        <v>238856</v>
       </c>
       <c r="C26" s="2">
-        <v>3650</v>
+        <v>3907448</v>
       </c>
       <c r="D26" s="2">
-        <v>4118</v>
+        <v>913439</v>
       </c>
       <c r="E26" s="2">
-        <v>4083</v>
+        <v>913439</v>
       </c>
       <c r="F26" s="2">
-        <v>6845</v>
+        <v>4777</v>
       </c>
       <c r="G26" s="2">
-        <v>5971</v>
-      </c>
-      <c r="H26" s="2">
+        <v>4678</v>
+      </c>
+      <c r="H26" s="31">
         <v>4193</v>
       </c>
       <c r="I26" s="2">
-        <v>377</v>
+        <v>716930</v>
       </c>
       <c r="J26" s="2">
-        <v>2343</v>
+        <v>1250114</v>
       </c>
       <c r="K26" s="2">
-        <v>1194</v>
+        <v>700113</v>
       </c>
       <c r="L26" s="2">
-        <v>1176</v>
+        <v>700113</v>
       </c>
       <c r="M26" s="2">
-        <v>5158</v>
+        <v>5323</v>
       </c>
       <c r="N26" s="2">
-        <v>2169</v>
+        <v>2262</v>
       </c>
       <c r="O26" s="1">
         <v>1355</v>
       </c>
       <c r="P26" s="6">
         <f t="shared" si="0"/>
-        <v>0.75354273192111032</v>
+        <v>1.11429767636592</v>
       </c>
       <c r="Q26" s="6">
         <f t="shared" si="1"/>
-        <v>0.3632557360576118</v>
+        <v>0.48353997434801199</v>
       </c>
       <c r="R26" s="6">
         <f t="shared" si="2"/>
@@ -3123,21 +3159,21 @@
         <v>0</v>
       </c>
       <c r="W26" s="2">
-        <v>5370</v>
+        <v>5581</v>
       </c>
       <c r="X26" s="2">
-        <v>2969</v>
+        <v>3096</v>
       </c>
       <c r="Y26" s="1">
         <v>1837</v>
       </c>
       <c r="Z26" s="6">
         <f t="shared" si="3"/>
-        <v>0.7845142439737034</v>
+        <v>1.1683064684948712</v>
       </c>
       <c r="AA26" s="7">
         <f t="shared" si="4"/>
-        <v>0.4972366437782616</v>
+        <v>0.66182129115006416</v>
       </c>
       <c r="AB26" s="7">
         <f t="shared" si="5"/>
@@ -4066,7 +4102,7 @@
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B37" s="23">
         <f>COUNTIF(B3:B6,"=0")/COUNTA(B3:B6)</f>
@@ -4152,11 +4188,11 @@
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B38" s="24">
         <f>COUNTIF(B7:B36,"=0")/COUNTA(B7:B36)</f>
-        <v>0.76666666666666672</v>
+        <v>0.73333333333333328</v>
       </c>
       <c r="C38" s="24">
         <f>COUNTIF(C7:C36,"=0")/COUNTA(C7:C36)</f>
@@ -4194,11 +4230,11 @@
       <c r="O38" s="2"/>
       <c r="P38" s="17">
         <f>AVERAGE(P7:P36)</f>
-        <v>0.61282245912859745</v>
+        <v>0.62484762394342441</v>
       </c>
       <c r="Q38" s="17">
         <f>AVERAGE(Q7:Q36)</f>
-        <v>0.40017450834783452</v>
+        <v>0.40418398295751451</v>
       </c>
       <c r="R38" s="17">
         <f>AVERAGE(R7:R36)</f>
@@ -4206,11 +4242,11 @@
       </c>
       <c r="S38" s="24">
         <f>COUNTIF(S7:S36,"=0")/COUNTA(S7:S36)</f>
-        <v>0.93333333333333335</v>
+        <v>1</v>
       </c>
       <c r="T38" s="24">
         <f>COUNTIF(T7:T36,"=0")/COUNTA(T7:T36)</f>
-        <v>0.6333333333333333</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="U38" s="24">
         <f>COUNTIF(U7:U36,"=0")/COUNTA(U7:U36)</f>
@@ -4218,18 +4254,18 @@
       </c>
       <c r="V38" s="24">
         <f>COUNTIF(V7:V36,"=0")/COUNTA(V7:V36)</f>
-        <v>0.6333333333333333</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="W38" s="2"/>
       <c r="X38" s="2"/>
       <c r="Y38" s="2"/>
       <c r="Z38" s="17">
         <f>AVERAGE(Z7:Z36)</f>
-        <v>0.78140209808427419</v>
+        <v>0.79419517223497982</v>
       </c>
       <c r="AA38" s="17">
         <f>AVERAGE(AA7:AA36)</f>
-        <v>0.45329826232077536</v>
+        <v>0.45878441723316876</v>
       </c>
       <c r="AB38" s="26">
         <f>AVERAGE(AB7:AB36)</f>
@@ -4243,7 +4279,7 @@
       </c>
       <c r="B39" s="25">
         <f>COUNTIF(B3:B36,"=0")/COUNTA(B3:B36)</f>
-        <v>0.79411764705882348</v>
+        <v>0.76470588235294112</v>
       </c>
       <c r="C39" s="25">
         <f>COUNTIF(C3:C36,"=0")/COUNTA(C3:C36)</f>
@@ -4281,11 +4317,11 @@
       <c r="O39" s="12"/>
       <c r="P39" s="18">
         <f>AVERAGE(P3:P36)</f>
-        <v>0.62356596507255957</v>
+        <v>0.63417640461505398</v>
       </c>
       <c r="Q39" s="18">
         <f>AVERAGE(Q3:Q36)</f>
-        <v>0.44212361662123473</v>
+        <v>0.44566138833565827</v>
       </c>
       <c r="R39" s="18">
         <f>AVERAGE(R3:R36)</f>
@@ -4293,11 +4329,11 @@
       </c>
       <c r="S39" s="25">
         <f>COUNTIF(S3:S36,"=0")/COUNTA(S3:S36)</f>
-        <v>0.94117647058823528</v>
+        <v>1</v>
       </c>
       <c r="T39" s="25">
         <f>COUNTIF(T3:T36,"=0")/COUNTA(T3:T36)</f>
-        <v>0.67647058823529416</v>
+        <v>0.70588235294117652</v>
       </c>
       <c r="U39" s="25">
         <f>COUNTIF(U3:U36,"=0")/COUNTA(U3:U36)</f>
@@ -4305,23 +4341,359 @@
       </c>
       <c r="V39" s="25">
         <f>COUNTIF(V3:V36,"=0")/COUNTA(V3:V36)</f>
-        <v>0.67647058823529416</v>
+        <v>0.70588235294117652</v>
       </c>
       <c r="W39" s="12"/>
       <c r="X39" s="12"/>
       <c r="Y39" s="12"/>
       <c r="Z39" s="18">
         <f>AVERAGE(Z3:Z36)</f>
-        <v>0.84669589255140254</v>
+        <v>0.85798389915496631</v>
       </c>
       <c r="AA39" s="19">
         <f>AVERAGE(AA3:AA36)</f>
-        <v>0.50267161746951616</v>
+        <v>0.50751234239221621</v>
       </c>
       <c r="AB39" s="19">
         <f>AVERAGE(AB3:AB36)</f>
         <v>0.39146082857307762</v>
       </c>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A48" s="27"/>
+      <c r="B48" s="27"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="27"/>
+      <c r="B49" s="27"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="27"/>
+      <c r="B51" s="27"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="27"/>
+      <c r="B52" s="27"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="27"/>
+      <c r="B53" s="27"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="27"/>
+      <c r="B54" s="27"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="27"/>
+      <c r="B55" s="27"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="27"/>
+      <c r="B57" s="27"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="27"/>
+      <c r="B58" s="27"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="27"/>
+      <c r="B59" s="27"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="27"/>
+      <c r="B60" s="27"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="27"/>
+      <c r="B61" s="27"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="27"/>
+      <c r="B62" s="27"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="27"/>
+      <c r="B63" s="27"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="27"/>
+      <c r="B64" s="27"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="27"/>
+      <c r="B65" s="27"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="27"/>
+      <c r="B66" s="27"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="27"/>
+      <c r="B67" s="27"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="27"/>
+      <c r="B68" s="27"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="27"/>
+      <c r="B69" s="27"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="27"/>
+      <c r="B70" s="27"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="27"/>
+      <c r="B71" s="27"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="27"/>
+      <c r="B72" s="27"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="27"/>
+      <c r="B73" s="27"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="27"/>
+      <c r="B74" s="27"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="27"/>
+      <c r="B75" s="27"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="27"/>
+      <c r="B76" s="27"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="27"/>
+      <c r="B77" s="27"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="27"/>
+      <c r="B78" s="27"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="27"/>
+      <c r="B79" s="27"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="27"/>
+      <c r="B80" s="27"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="27"/>
+      <c r="B81" s="27"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="27"/>
+      <c r="B82" s="27"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="27"/>
+      <c r="B83" s="27"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="27"/>
+      <c r="B84" s="27"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="27"/>
+      <c r="B85" s="27"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="27"/>
+      <c r="B86" s="27"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="27"/>
+      <c r="B87" s="27"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="27"/>
+      <c r="B88" s="27"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="27"/>
+      <c r="B89" s="27"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="27"/>
+      <c r="B90" s="27"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="27"/>
+      <c r="B91" s="27"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="27"/>
+      <c r="B92" s="27"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="27"/>
+      <c r="B93" s="27"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="27"/>
+      <c r="B94" s="27"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="27"/>
+      <c r="B95" s="27"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="27"/>
+      <c r="B96" s="27"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="27"/>
+      <c r="B97" s="27"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="27"/>
+      <c r="B98" s="27"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="27"/>
+      <c r="B99" s="27"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="27"/>
+      <c r="B100" s="27"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="27"/>
+      <c r="B101" s="27"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="27"/>
+      <c r="B102" s="27"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="27"/>
+      <c r="B103" s="27"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="27"/>
+      <c r="B104" s="27"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="27"/>
+      <c r="B105" s="27"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="27"/>
+      <c r="B106" s="27"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="27"/>
+      <c r="B107" s="27"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="27"/>
+      <c r="B108" s="27"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="27"/>
+      <c r="B109" s="27"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="27"/>
+      <c r="B110" s="27"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="27"/>
+      <c r="B111" s="27"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="27"/>
+      <c r="B112" s="27"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="27"/>
+      <c r="B113" s="27"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="27"/>
+      <c r="B114" s="27"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="27"/>
+      <c r="B115" s="27"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="27"/>
+      <c r="B116" s="27"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="27"/>
+      <c r="B117" s="27"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="27"/>
+      <c r="B118" s="27"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="27"/>
+      <c r="B119" s="27"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="27"/>
+      <c r="B120" s="27"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="27"/>
+      <c r="B121" s="27"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="27"/>
+      <c r="B122" s="27"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="27"/>
+      <c r="B123" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4335,7 +4707,7 @@
     <mergeCell ref="S1:V1"/>
   </mergeCells>
   <conditionalFormatting sqref="Z3:AB39 P3:R39">
-    <cfRule type="dataBar" priority="10">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4348,8 +4720,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:E6 I3:L6 S3:V6">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="B3:E7 B18:E19 B26:E26 I3:L7 I18:L19 I26:L26 S3:V7 S18:V19 S26:V26">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4360,20 +4732,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18:E19 B26:E26 I18:L19 I26:L26 S18:V19 S26:V26 B7:E7 I7:L7 S7:V7">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="1048576"/>
-        <color rgb="FF99FF99"/>
-        <color rgb="FFFFFFCC"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B20:E25 I20:L25 S20:V25 I27:L36 S27:V36 B27:E36 S9:V17 I9:L17 B9:E17">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4385,7 +4745,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37:E39 I37:L39 S37:V39">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4399,7 +4759,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:E8 I8:L8 S8:V8">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>

</xml_diff>

<commit_message>
Improved accuracy of rsqrt function.
git-svn-id: https://svn.code.sf.net/p/half/code/trunk@412 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -184,7 +184,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,13 +207,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="19">
@@ -441,11 +453,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -492,8 +505,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -979,10 +994,10 @@
         <v>0</v>
       </c>
       <c r="F3" s="30">
-        <v>45052</v>
+        <v>43513</v>
       </c>
       <c r="G3" s="30">
-        <v>57291</v>
+        <v>57380</v>
       </c>
       <c r="H3" s="30">
         <v>69936</v>
@@ -1010,11 +1025,11 @@
       </c>
       <c r="P3" s="6">
         <f>F3/M3</f>
-        <v>0.43961748633879782</v>
+        <v>0.4245999219359875</v>
       </c>
       <c r="Q3" s="6">
         <f>G3/N3</f>
-        <v>0.51943424452604381</v>
+        <v>0.52024117140396209</v>
       </c>
       <c r="R3" s="6">
         <f>H3/O3</f>
@@ -1043,11 +1058,11 @@
       </c>
       <c r="Z3" s="6">
         <f>F3/W3</f>
-        <v>0.8068340556610194</v>
+        <v>0.77927218023568179</v>
       </c>
       <c r="AA3" s="7">
         <f>G3/X3</f>
-        <v>0.59897123859109869</v>
+        <v>0.59990172401175135</v>
       </c>
       <c r="AB3" s="7">
         <f>H3/Y3</f>
@@ -1071,10 +1086,10 @@
         <v>0</v>
       </c>
       <c r="F4" s="31">
-        <v>36200</v>
+        <v>35043</v>
       </c>
       <c r="G4" s="31">
-        <v>57613</v>
+        <v>57116</v>
       </c>
       <c r="H4" s="31">
         <v>69492</v>
@@ -1102,11 +1117,11 @@
       </c>
       <c r="P4" s="6">
         <f t="shared" ref="P4:P37" si="0">F4/M4</f>
-        <v>0.35392692679969889</v>
+        <v>0.34261495292380795</v>
       </c>
       <c r="Q4" s="6">
         <f t="shared" ref="Q4:Q37" si="1">G4/N4</f>
-        <v>0.51877898338661022</v>
+        <v>0.51430372338030705</v>
       </c>
       <c r="R4" s="6">
         <f t="shared" ref="R4:R37" si="2">H4/O4</f>
@@ -1135,11 +1150,11 @@
       </c>
       <c r="Z4" s="6">
         <f t="shared" ref="Z4:Z37" si="3">F4/W4</f>
-        <v>0.78994457294985376</v>
+        <v>0.76469689695805876</v>
       </c>
       <c r="AA4" s="7">
         <f t="shared" ref="AA4:AA37" si="4">G4/X4</f>
-        <v>0.60404915179601171</v>
+        <v>0.59883830652771075</v>
       </c>
       <c r="AB4" s="7">
         <f t="shared" ref="AB4:AB37" si="5">H4/Y4</f>
@@ -1163,10 +1178,10 @@
         <v>0</v>
       </c>
       <c r="F5" s="31">
-        <v>80535</v>
+        <v>78428</v>
       </c>
       <c r="G5" s="31">
-        <v>92418</v>
+        <v>92022</v>
       </c>
       <c r="H5" s="31">
         <v>129255</v>
@@ -1194,11 +1209,11 @@
       </c>
       <c r="P5" s="6">
         <f t="shared" si="0"/>
-        <v>1.0185021246458923</v>
+        <v>0.99185552407932009</v>
       </c>
       <c r="Q5" s="6">
         <f t="shared" si="1"/>
-        <v>1.1249634823254455</v>
+        <v>1.1201431492842535</v>
       </c>
       <c r="R5" s="6">
         <f t="shared" si="2"/>
@@ -1227,11 +1242,11 @@
       </c>
       <c r="Z5" s="6">
         <f t="shared" si="3"/>
-        <v>1.6632246339398196</v>
+        <v>1.6197104562070177</v>
       </c>
       <c r="AA5" s="7">
         <f t="shared" si="4"/>
-        <v>1.1982729559422245</v>
+        <v>1.1931385006353241</v>
       </c>
       <c r="AB5" s="7">
         <f t="shared" si="5"/>
@@ -1255,10 +1270,10 @@
         <v>0</v>
       </c>
       <c r="F6" s="31">
-        <v>67406</v>
+        <v>65079</v>
       </c>
       <c r="G6" s="31">
-        <v>77231</v>
+        <v>76909</v>
       </c>
       <c r="H6" s="31">
         <v>115168</v>
@@ -1286,11 +1301,11 @@
       </c>
       <c r="P6" s="6">
         <f t="shared" si="0"/>
-        <v>0.95299090921943708</v>
+        <v>0.92009161470925049</v>
       </c>
       <c r="Q6" s="6">
         <f t="shared" si="1"/>
-        <v>1.0396160887357313</v>
+        <v>1.0352816067197932</v>
       </c>
       <c r="R6" s="6">
         <f t="shared" si="2"/>
@@ -1319,11 +1334,11 @@
       </c>
       <c r="Z6" s="6">
         <f t="shared" si="3"/>
-        <v>1.9536838444148166</v>
+        <v>1.8862384789287578</v>
       </c>
       <c r="AA6" s="7">
         <f t="shared" si="4"/>
-        <v>1.1628547767823534</v>
+        <v>1.1580064744410148</v>
       </c>
       <c r="AB6" s="7">
         <f t="shared" si="5"/>
@@ -1347,10 +1362,10 @@
         <v>0</v>
       </c>
       <c r="F7" s="31">
-        <v>53858</v>
+        <v>52088</v>
       </c>
       <c r="G7" s="31">
-        <v>75471</v>
+        <v>76683</v>
       </c>
       <c r="H7" s="31">
         <v>98482</v>
@@ -1378,11 +1393,11 @@
       </c>
       <c r="P7" s="6">
         <f t="shared" si="0"/>
-        <v>0.61488754424021008</v>
+        <v>0.5946797579632378</v>
       </c>
       <c r="Q7" s="6">
         <f t="shared" si="1"/>
-        <v>0.76741844952411942</v>
+        <v>0.77974253640283087</v>
       </c>
       <c r="R7" s="6">
         <f t="shared" si="2"/>
@@ -1411,11 +1426,11 @@
       </c>
       <c r="Z7" s="6">
         <f t="shared" si="3"/>
-        <v>0.90726546838940081</v>
+        <v>0.87744891599144248</v>
       </c>
       <c r="AA7" s="7">
         <f t="shared" si="4"/>
-        <v>0.83105942981731695</v>
+        <v>0.84440553665224138</v>
       </c>
       <c r="AB7" s="7">
         <f t="shared" si="5"/>
@@ -1439,10 +1454,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="31">
-        <v>43846</v>
+        <v>42537</v>
       </c>
       <c r="G8" s="31">
-        <v>49869</v>
+        <v>50910</v>
       </c>
       <c r="H8" s="31">
         <v>67064</v>
@@ -1470,11 +1485,11 @@
       </c>
       <c r="P8" s="6">
         <f t="shared" si="0"/>
-        <v>0.50724788579229285</v>
+        <v>0.49210425849442962</v>
       </c>
       <c r="Q8" s="6">
         <f t="shared" si="1"/>
-        <v>0.52059127493658197</v>
+        <v>0.53145845729855001</v>
       </c>
       <c r="R8" s="6">
         <f t="shared" si="2"/>
@@ -1503,11 +1518,11 @@
       </c>
       <c r="Z8" s="6">
         <f t="shared" si="3"/>
-        <v>1.1572529560810811</v>
+        <v>1.1227037584459461</v>
       </c>
       <c r="AA8" s="7">
         <f t="shared" si="4"/>
-        <v>0.66141011697923024</v>
+        <v>0.67521684925329584</v>
       </c>
       <c r="AB8" s="7">
         <f t="shared" si="5"/>
@@ -1531,10 +1546,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="31">
-        <v>13410</v>
+        <v>13047</v>
       </c>
       <c r="G9" s="31">
-        <v>14461</v>
+        <v>14418</v>
       </c>
       <c r="H9" s="31">
         <v>16790</v>
@@ -1562,11 +1577,11 @@
       </c>
       <c r="P9" s="6">
         <f t="shared" si="0"/>
-        <v>0.44477611940298506</v>
+        <v>0.43273631840796017</v>
       </c>
       <c r="Q9" s="6">
         <f t="shared" si="1"/>
-        <v>0.50722553490003508</v>
+        <v>0.50571729217818306</v>
       </c>
       <c r="R9" s="6">
         <f t="shared" si="2"/>
@@ -1595,11 +1610,11 @@
       </c>
       <c r="Z9" s="6">
         <f t="shared" si="3"/>
-        <v>0.55037964293043296</v>
+        <v>0.5354812230658732</v>
       </c>
       <c r="AA9" s="7">
         <f t="shared" si="4"/>
-        <v>0.51122423728214372</v>
+        <v>0.5097041043588928</v>
       </c>
       <c r="AB9" s="7">
         <f t="shared" si="5"/>
@@ -1623,10 +1638,10 @@
         <v>0</v>
       </c>
       <c r="F10" s="31">
-        <v>14089</v>
+        <v>13691</v>
       </c>
       <c r="G10" s="31">
-        <v>13738</v>
+        <v>13767</v>
       </c>
       <c r="H10" s="31">
         <v>15499</v>
@@ -1654,11 +1669,11 @@
       </c>
       <c r="P10" s="6">
         <f t="shared" si="0"/>
-        <v>1.789079365079365</v>
+        <v>1.7385396825396826</v>
       </c>
       <c r="Q10" s="6">
         <f t="shared" si="1"/>
-        <v>0.96440856440856437</v>
+        <v>0.96644436644436649</v>
       </c>
       <c r="R10" s="6">
         <f t="shared" si="2"/>
@@ -1687,11 +1702,11 @@
       </c>
       <c r="Z10" s="6">
         <f t="shared" si="3"/>
-        <v>1.5882087701499268</v>
+        <v>1.5433434787509863</v>
       </c>
       <c r="AA10" s="7">
         <f t="shared" si="4"/>
-        <v>0.95026630697931802</v>
+        <v>0.95227225565470019</v>
       </c>
       <c r="AB10" s="7">
         <f t="shared" si="5"/>
@@ -1715,10 +1730,10 @@
         <v>310</v>
       </c>
       <c r="F11" s="31">
-        <v>11714</v>
+        <v>11405</v>
       </c>
       <c r="G11" s="31">
-        <v>11783</v>
+        <v>11768</v>
       </c>
       <c r="H11" s="31">
         <v>13395</v>
@@ -1746,11 +1761,11 @@
       </c>
       <c r="P11" s="6">
         <f t="shared" si="0"/>
-        <v>0.88108311395261374</v>
+        <v>0.8578412937194434</v>
       </c>
       <c r="Q11" s="6">
         <f t="shared" si="1"/>
-        <v>0.46090357911206725</v>
+        <v>0.46031683942890672</v>
       </c>
       <c r="R11" s="6">
         <f t="shared" si="2"/>
@@ -1779,11 +1794,11 @@
       </c>
       <c r="Z11" s="6">
         <f t="shared" si="3"/>
-        <v>0.81009681881051177</v>
+        <v>0.7887275242047026</v>
       </c>
       <c r="AA11" s="7">
         <f t="shared" si="4"/>
-        <v>0.46070534876446667</v>
+        <v>0.46011886143259306</v>
       </c>
       <c r="AB11" s="7">
         <f t="shared" si="5"/>
@@ -1807,10 +1822,10 @@
         <v>0</v>
       </c>
       <c r="F12" s="31">
-        <v>9149</v>
+        <v>8923</v>
       </c>
       <c r="G12" s="31">
-        <v>9782</v>
+        <v>9771</v>
       </c>
       <c r="H12" s="31">
         <v>10793</v>
@@ -1838,11 +1853,11 @@
       </c>
       <c r="P12" s="6">
         <f t="shared" si="0"/>
-        <v>0.21273775752220619</v>
+        <v>0.20748267683579036</v>
       </c>
       <c r="Q12" s="6">
         <f t="shared" si="1"/>
-        <v>0.17236396955173386</v>
+        <v>0.172170143783479</v>
       </c>
       <c r="R12" s="6">
         <f t="shared" si="2"/>
@@ -1871,11 +1886,11 @@
       </c>
       <c r="Z12" s="6">
         <f t="shared" si="3"/>
-        <v>0.29705509919153217</v>
+        <v>0.28971719861034451</v>
       </c>
       <c r="AA12" s="7">
         <f t="shared" si="4"/>
-        <v>0.19454277872797424</v>
+        <v>0.19432401256911022</v>
       </c>
       <c r="AB12" s="7">
         <f t="shared" si="5"/>
@@ -1899,10 +1914,10 @@
         <v>0</v>
       </c>
       <c r="F13" s="31">
-        <v>9004</v>
+        <v>8688</v>
       </c>
       <c r="G13" s="31">
-        <v>9236</v>
+        <v>9289</v>
       </c>
       <c r="H13" s="31">
         <v>11182</v>
@@ -1930,11 +1945,11 @@
       </c>
       <c r="P13" s="6">
         <f t="shared" si="0"/>
-        <v>0.21133669757070767</v>
+        <v>0.20391972773148692</v>
       </c>
       <c r="Q13" s="6">
         <f t="shared" si="1"/>
-        <v>0.17409334238106008</v>
+        <v>0.17509236221066124</v>
       </c>
       <c r="R13" s="6">
         <f t="shared" si="2"/>
@@ -1963,11 +1978,11 @@
       </c>
       <c r="Z13" s="6">
         <f t="shared" si="3"/>
-        <v>0.29838282078472961</v>
+        <v>0.28791092258748674</v>
       </c>
       <c r="AA13" s="7">
         <f t="shared" si="4"/>
-        <v>0.19390732926035564</v>
+        <v>0.19502004996745817</v>
       </c>
       <c r="AB13" s="7">
         <f t="shared" si="5"/>
@@ -1991,10 +2006,10 @@
         <v>0</v>
       </c>
       <c r="F14" s="31">
-        <v>5973</v>
+        <v>5795</v>
       </c>
       <c r="G14" s="31">
-        <v>9905</v>
+        <v>9930</v>
       </c>
       <c r="H14" s="31">
         <v>10845</v>
@@ -2022,11 +2037,11 @@
       </c>
       <c r="P14" s="6">
         <f t="shared" si="0"/>
-        <v>0.32057750107342209</v>
+        <v>0.31102404465435807</v>
       </c>
       <c r="Q14" s="6">
         <f t="shared" si="1"/>
-        <v>0.36832515246169867</v>
+        <v>0.36925479696564034</v>
       </c>
       <c r="R14" s="6">
         <f t="shared" si="2"/>
@@ -2055,11 +2070,11 @@
       </c>
       <c r="Z14" s="6">
         <f t="shared" si="3"/>
-        <v>0.36790883892824144</v>
+        <v>0.3569448721897136</v>
       </c>
       <c r="AA14" s="7">
         <f t="shared" si="4"/>
-        <v>0.28126419809177644</v>
+        <v>0.28197410268059975</v>
       </c>
       <c r="AB14" s="7">
         <f t="shared" si="5"/>
@@ -2083,10 +2098,10 @@
         <v>868</v>
       </c>
       <c r="F15" s="31">
-        <v>7319</v>
+        <v>7093</v>
       </c>
       <c r="G15" s="31">
-        <v>8237</v>
+        <v>8216</v>
       </c>
       <c r="H15" s="31">
         <v>9356</v>
@@ -2114,11 +2129,11 @@
       </c>
       <c r="P15" s="6">
         <f t="shared" si="0"/>
-        <v>0.27172823463894563</v>
+        <v>0.26333766474846854</v>
       </c>
       <c r="Q15" s="6">
         <f t="shared" si="1"/>
-        <v>0.22229718788794733</v>
+        <v>0.22173044745506559</v>
       </c>
       <c r="R15" s="6">
         <f t="shared" si="2"/>
@@ -2147,11 +2162,11 @@
       </c>
       <c r="Z15" s="6">
         <f t="shared" si="3"/>
-        <v>0.31459273586933162</v>
+        <v>0.30487857296367937</v>
       </c>
       <c r="AA15" s="7">
         <f t="shared" si="4"/>
-        <v>0.25305683563748083</v>
+        <v>0.25241167434715822</v>
       </c>
       <c r="AB15" s="7">
         <f t="shared" si="5"/>
@@ -2175,10 +2190,10 @@
         <v>0</v>
       </c>
       <c r="F16" s="31">
-        <v>22297</v>
+        <v>21223</v>
       </c>
       <c r="G16" s="31">
-        <v>21646</v>
+        <v>21779</v>
       </c>
       <c r="H16" s="31">
         <v>24463</v>
@@ -2206,11 +2221,11 @@
       </c>
       <c r="P16" s="6">
         <f t="shared" si="0"/>
-        <v>0.28895598983982168</v>
+        <v>0.27503758229226066</v>
       </c>
       <c r="Q16" s="6">
         <f t="shared" si="1"/>
-        <v>0.25091575091575091</v>
+        <v>0.25245745815366066</v>
       </c>
       <c r="R16" s="6">
         <f t="shared" si="2"/>
@@ -2239,11 +2254,11 @@
       </c>
       <c r="Z16" s="6">
         <f t="shared" si="3"/>
-        <v>0.47673722471669872</v>
+        <v>0.45377378661535173</v>
       </c>
       <c r="AA16" s="7">
         <f t="shared" si="4"/>
-        <v>0.27497110046874407</v>
+        <v>0.27666061152678445</v>
       </c>
       <c r="AB16" s="7">
         <f t="shared" si="5"/>
@@ -2255,24 +2270,24 @@
         <v>50</v>
       </c>
       <c r="B17" s="2">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="C17" s="2">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E17" s="2">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="F17" s="31">
-        <v>46102</v>
+        <v>44739</v>
       </c>
       <c r="G17" s="31">
-        <v>48005</v>
-      </c>
-      <c r="H17" s="31">
+        <v>48418</v>
+      </c>
+      <c r="H17" s="36">
         <v>75106</v>
       </c>
       <c r="I17" s="2">
@@ -2298,11 +2313,11 @@
       </c>
       <c r="P17" s="6">
         <f t="shared" si="0"/>
-        <v>0.66604062527088326</v>
+        <v>0.64634921552197411</v>
       </c>
       <c r="Q17" s="6">
         <f t="shared" si="1"/>
-        <v>0.63584465813663937</v>
+        <v>0.64131500172189992</v>
       </c>
       <c r="R17" s="6">
         <f t="shared" si="2"/>
@@ -2331,11 +2346,11 @@
       </c>
       <c r="Z17" s="6">
         <f t="shared" si="3"/>
-        <v>1.2747684225079496</v>
+        <v>1.2370800497718788</v>
       </c>
       <c r="AA17" s="7">
         <f t="shared" si="4"/>
-        <v>0.72509629182085944</v>
+        <v>0.73133449135261686</v>
       </c>
       <c r="AB17" s="7">
         <f t="shared" si="5"/>
@@ -2359,10 +2374,10 @@
         <v>0</v>
       </c>
       <c r="F18" s="31">
-        <v>4940</v>
+        <v>4723</v>
       </c>
       <c r="G18" s="31">
-        <v>4756</v>
+        <v>4742</v>
       </c>
       <c r="H18" s="31">
         <v>5298</v>
@@ -2390,11 +2405,11 @@
       </c>
       <c r="P18" s="6">
         <f t="shared" si="0"/>
-        <v>0.36725893985577279</v>
+        <v>0.35112631031150099</v>
       </c>
       <c r="Q18" s="6">
         <f t="shared" si="1"/>
-        <v>0.23434343434343435</v>
+        <v>0.23365360926336537</v>
       </c>
       <c r="R18" s="6">
         <f t="shared" si="2"/>
@@ -2423,11 +2438,11 @@
       </c>
       <c r="Z18" s="6">
         <f t="shared" si="3"/>
-        <v>0.48308233913553689</v>
+        <v>0.46186192059456288</v>
       </c>
       <c r="AA18" s="7">
         <f t="shared" si="4"/>
-        <v>0.34322003319621852</v>
+        <v>0.34220971350220103</v>
       </c>
       <c r="AB18" s="7">
         <f t="shared" si="5"/>
@@ -2451,10 +2466,10 @@
         <v>13016</v>
       </c>
       <c r="F19" s="31">
-        <v>8531</v>
+        <v>8258</v>
       </c>
       <c r="G19" s="31">
-        <v>8456</v>
+        <v>8657</v>
       </c>
       <c r="H19" s="31">
         <v>10277</v>
@@ -2482,11 +2497,11 @@
       </c>
       <c r="P19" s="6">
         <f t="shared" si="0"/>
-        <v>0.54759612298607097</v>
+        <v>0.53007253353873807</v>
       </c>
       <c r="Q19" s="6">
         <f t="shared" si="1"/>
-        <v>0.56595944046583224</v>
+        <v>0.57941235526403856</v>
       </c>
       <c r="R19" s="6">
         <f t="shared" si="2"/>
@@ -2515,11 +2530,11 @@
       </c>
       <c r="Z19" s="6">
         <f t="shared" si="3"/>
-        <v>0.6135644418872267</v>
+        <v>0.59392980437284237</v>
       </c>
       <c r="AA19" s="7">
         <f t="shared" si="4"/>
-        <v>0.6937402576093199</v>
+        <v>0.71023053572893591</v>
       </c>
       <c r="AB19" s="7">
         <f t="shared" si="5"/>
@@ -2543,10 +2558,10 @@
         <v>0</v>
       </c>
       <c r="F20" s="31">
-        <v>17201</v>
+        <v>16638</v>
       </c>
       <c r="G20" s="31">
-        <v>17213</v>
+        <v>16706</v>
       </c>
       <c r="H20" s="31">
         <v>20018</v>
@@ -2574,11 +2589,11 @@
       </c>
       <c r="P20" s="6">
         <f t="shared" si="0"/>
-        <v>0.35831684199562547</v>
+        <v>0.34658889698989687</v>
       </c>
       <c r="Q20" s="6">
         <f t="shared" si="1"/>
-        <v>0.30071628232005593</v>
+        <v>0.29185883997204753</v>
       </c>
       <c r="R20" s="6">
         <f t="shared" si="2"/>
@@ -2607,11 +2622,11 @@
       </c>
       <c r="Z20" s="6">
         <f t="shared" si="3"/>
-        <v>2.0436022335749078</v>
+        <v>1.9767137935131283</v>
       </c>
       <c r="AA20" s="7">
         <f t="shared" si="4"/>
-        <v>0.36703840330938015</v>
+        <v>0.35622747723734993</v>
       </c>
       <c r="AB20" s="7">
         <f t="shared" si="5"/>
@@ -2635,10 +2650,10 @@
         <v>0</v>
       </c>
       <c r="F21" s="31">
-        <v>14021</v>
+        <v>13569</v>
       </c>
       <c r="G21" s="31">
-        <v>14385</v>
+        <v>14358</v>
       </c>
       <c r="H21" s="31">
         <v>21553</v>
@@ -2666,11 +2681,11 @@
       </c>
       <c r="P21" s="6">
         <f t="shared" si="0"/>
-        <v>0.36063170349031609</v>
+        <v>0.34900589006918903</v>
       </c>
       <c r="Q21" s="6">
         <f t="shared" si="1"/>
-        <v>0.41356409740390421</v>
+        <v>0.41278785613661845</v>
       </c>
       <c r="R21" s="6">
         <f t="shared" si="2"/>
@@ -2699,11 +2714,11 @@
       </c>
       <c r="Z21" s="6">
         <f t="shared" si="3"/>
-        <v>0.48109387867142467</v>
+        <v>0.46558468295360966</v>
       </c>
       <c r="AA21" s="7">
         <f t="shared" si="4"/>
-        <v>0.37257187257187258</v>
+        <v>0.37187257187257189</v>
       </c>
       <c r="AB21" s="7">
         <f t="shared" si="5"/>
@@ -2727,10 +2742,10 @@
         <v>0</v>
       </c>
       <c r="F22" s="31">
-        <v>13818</v>
+        <v>13395</v>
       </c>
       <c r="G22" s="31">
-        <v>14817</v>
+        <v>14738</v>
       </c>
       <c r="H22" s="31">
         <v>21515</v>
@@ -2758,11 +2773,11 @@
       </c>
       <c r="P22" s="6">
         <f t="shared" si="0"/>
-        <v>0.34830611010284329</v>
+        <v>0.33764367816091956</v>
       </c>
       <c r="Q22" s="6">
         <f t="shared" si="1"/>
-        <v>0.37368540516002119</v>
+        <v>0.37169302161357848</v>
       </c>
       <c r="R22" s="6">
         <f t="shared" si="2"/>
@@ -2791,11 +2806,11 @@
       </c>
       <c r="Z22" s="6">
         <f t="shared" si="3"/>
-        <v>0.47145927871984716</v>
+        <v>0.45702685182025998</v>
       </c>
       <c r="AA22" s="7">
         <f t="shared" si="4"/>
-        <v>0.37842876845277623</v>
+        <v>0.37641109465188743</v>
       </c>
       <c r="AB22" s="7">
         <f t="shared" si="5"/>
@@ -2819,10 +2834,10 @@
         <v>0</v>
       </c>
       <c r="F23" s="31">
-        <v>10899</v>
+        <v>10523</v>
       </c>
       <c r="G23" s="31">
-        <v>12309</v>
+        <v>12292</v>
       </c>
       <c r="H23" s="31">
         <v>17491</v>
@@ -2850,11 +2865,11 @@
       </c>
       <c r="P23" s="6">
         <f t="shared" si="0"/>
-        <v>0.37928034521158127</v>
+        <v>0.3661957126948775</v>
       </c>
       <c r="Q23" s="6">
         <f t="shared" si="1"/>
-        <v>0.30961364322366436</v>
+        <v>0.30918603481235535</v>
       </c>
       <c r="R23" s="6">
         <f t="shared" si="2"/>
@@ -2883,11 +2898,11 @@
       </c>
       <c r="Z23" s="6">
         <f t="shared" si="3"/>
-        <v>0.47356072126873777</v>
+        <v>0.45722354985878777</v>
       </c>
       <c r="AA23" s="7">
         <f t="shared" si="4"/>
-        <v>0.41149333065891086</v>
+        <v>0.41092501587938357</v>
       </c>
       <c r="AB23" s="7">
         <f t="shared" si="5"/>
@@ -2911,10 +2926,10 @@
         <v>0</v>
       </c>
       <c r="F24" s="31">
-        <v>19691</v>
+        <v>18897</v>
       </c>
       <c r="G24" s="31">
-        <v>20547</v>
+        <v>20587</v>
       </c>
       <c r="H24" s="29">
         <v>25738</v>
@@ -2942,11 +2957,11 @@
       </c>
       <c r="P24" s="6">
         <f t="shared" si="0"/>
-        <v>0.45123516201475777</v>
+        <v>0.4330400109995875</v>
       </c>
       <c r="Q24" s="6">
         <f t="shared" si="1"/>
-        <v>0.47033374536464773</v>
+        <v>0.47124937050771415</v>
       </c>
       <c r="R24" s="6">
         <f t="shared" si="2"/>
@@ -2975,11 +2990,11 @@
       </c>
       <c r="Z24" s="6">
         <f t="shared" si="3"/>
-        <v>0.6041481299665572</v>
+        <v>0.57978707084343262</v>
       </c>
       <c r="AA24" s="7">
         <f t="shared" si="4"/>
-        <v>0.53820363045812925</v>
+        <v>0.53925138172197917</v>
       </c>
       <c r="AB24" s="7">
         <f t="shared" si="5"/>
@@ -3003,10 +3018,10 @@
         <v>0</v>
       </c>
       <c r="F25" s="31">
-        <v>7922</v>
+        <v>7718</v>
       </c>
       <c r="G25" s="31">
-        <v>8110</v>
+        <v>8151</v>
       </c>
       <c r="H25" s="31">
         <v>11328</v>
@@ -3034,11 +3049,11 @@
       </c>
       <c r="P25" s="6">
         <f t="shared" si="0"/>
-        <v>0.1813063578523367</v>
+        <v>0.17663752460292031</v>
       </c>
       <c r="Q25" s="6">
         <f t="shared" si="1"/>
-        <v>0.18543076641668191</v>
+        <v>0.18636820925553321</v>
       </c>
       <c r="R25" s="6">
         <f t="shared" si="2"/>
@@ -3067,11 +3082,11 @@
       </c>
       <c r="Z25" s="6">
         <f t="shared" si="3"/>
-        <v>0.25000788967084292</v>
+        <v>0.24356991826301005</v>
       </c>
       <c r="AA25" s="7">
         <f t="shared" si="4"/>
-        <v>0.21109896402727887</v>
+        <v>0.21216617210682492</v>
       </c>
       <c r="AB25" s="7">
         <f t="shared" si="5"/>
@@ -3095,10 +3110,10 @@
         <v>0</v>
       </c>
       <c r="F26" s="31">
-        <v>15880</v>
+        <v>15398</v>
       </c>
       <c r="G26" s="31">
-        <v>17764</v>
+        <v>17855</v>
       </c>
       <c r="H26" s="31">
         <v>25556</v>
@@ -3126,11 +3141,11 @@
       </c>
       <c r="P26" s="6">
         <f t="shared" si="0"/>
-        <v>0.48711656441717793</v>
+        <v>0.47233128834355831</v>
       </c>
       <c r="Q26" s="6">
         <f t="shared" si="1"/>
-        <v>0.47286182021454998</v>
+        <v>0.47528415896930815</v>
       </c>
       <c r="R26" s="6">
         <f t="shared" si="2"/>
@@ -3159,11 +3174,11 @@
       </c>
       <c r="Z26" s="6">
         <f t="shared" si="3"/>
-        <v>0.67216931216931219</v>
+        <v>0.65176719576719577</v>
       </c>
       <c r="AA26" s="7">
         <f t="shared" si="4"/>
-        <v>0.52865900839235758</v>
+        <v>0.53136718052496879</v>
       </c>
       <c r="AB26" s="7">
         <f t="shared" si="5"/>
@@ -3187,10 +3202,10 @@
         <v>913439</v>
       </c>
       <c r="F27" s="31">
-        <v>12823</v>
+        <v>12472</v>
       </c>
       <c r="G27" s="31">
-        <v>14028</v>
+        <v>13820</v>
       </c>
       <c r="H27" s="31">
         <v>20918</v>
@@ -3218,11 +3233,11 @@
       </c>
       <c r="P27" s="6">
         <f t="shared" si="0"/>
-        <v>1.0408279220779222</v>
+        <v>1.0123376623376623</v>
       </c>
       <c r="Q27" s="6">
         <f t="shared" si="1"/>
-        <v>0.49762327066335582</v>
+        <v>0.49024476764810215</v>
       </c>
       <c r="R27" s="6">
         <f t="shared" si="2"/>
@@ -3251,11 +3266,11 @@
       </c>
       <c r="Z27" s="6">
         <f t="shared" si="3"/>
-        <v>1.0958892402358773</v>
+        <v>1.065891804119306</v>
       </c>
       <c r="AA27" s="7">
         <f t="shared" si="4"/>
-        <v>0.67055449330783934</v>
+        <v>0.66061185468451245</v>
       </c>
       <c r="AB27" s="7">
         <f t="shared" si="5"/>
@@ -3279,10 +3294,10 @@
         <v>0</v>
       </c>
       <c r="F28" s="31">
-        <v>10233</v>
+        <v>9999</v>
       </c>
       <c r="G28" s="31">
-        <v>10833</v>
+        <v>10934</v>
       </c>
       <c r="H28" s="31">
         <v>12236</v>
@@ -3310,11 +3325,11 @@
       </c>
       <c r="P28" s="6">
         <f t="shared" si="0"/>
-        <v>1.649153908138598</v>
+        <v>1.6114423851732473</v>
       </c>
       <c r="Q28" s="6">
         <f t="shared" si="1"/>
-        <v>0.5308472582937227</v>
+        <v>0.535796540402803</v>
       </c>
       <c r="R28" s="6">
         <f t="shared" si="2"/>
@@ -3343,11 +3358,11 @@
       </c>
       <c r="Z28" s="6">
         <f t="shared" si="3"/>
-        <v>1.6734260016353231</v>
+        <v>1.635159443990188</v>
       </c>
       <c r="AA28" s="7">
         <f t="shared" si="4"/>
-        <v>0.50062387356162485</v>
+        <v>0.50529137205970698</v>
       </c>
       <c r="AB28" s="7">
         <f t="shared" si="5"/>
@@ -3371,10 +3386,10 @@
         <v>0</v>
       </c>
       <c r="F29" s="31">
-        <v>8791</v>
+        <v>8572</v>
       </c>
       <c r="G29" s="31">
-        <v>9778</v>
+        <v>9797</v>
       </c>
       <c r="H29" s="31">
         <v>11075</v>
@@ -3402,11 +3417,11 @@
       </c>
       <c r="P29" s="6">
         <f t="shared" si="0"/>
-        <v>1.4128897460623593</v>
+        <v>1.3776920604307297</v>
       </c>
       <c r="Q29" s="6">
         <f t="shared" si="1"/>
-        <v>0.48931591853075113</v>
+        <v>0.49026672671771004</v>
       </c>
       <c r="R29" s="6">
         <f t="shared" si="2"/>
@@ -3435,11 +3450,11 @@
       </c>
       <c r="Z29" s="6">
         <f t="shared" si="3"/>
-        <v>1.436672658931198</v>
+        <v>1.4008824971400555</v>
       </c>
       <c r="AA29" s="7">
         <f t="shared" si="4"/>
-        <v>0.44795675279457575</v>
+        <v>0.44882719442917351</v>
       </c>
       <c r="AB29" s="7">
         <f t="shared" si="5"/>
@@ -3463,10 +3478,10 @@
         <v>0</v>
       </c>
       <c r="F30" s="31">
-        <v>21931</v>
+        <v>21363</v>
       </c>
       <c r="G30" s="31">
-        <v>24149</v>
+        <v>24500</v>
       </c>
       <c r="H30" s="29">
         <v>27794</v>
@@ -3494,11 +3509,11 @@
       </c>
       <c r="P30" s="6">
         <f t="shared" si="0"/>
-        <v>1.6452363090772693</v>
+        <v>1.6026256564141035</v>
       </c>
       <c r="Q30" s="6">
         <f t="shared" si="1"/>
-        <v>0.6265632297234186</v>
+        <v>0.6356701779876498</v>
       </c>
       <c r="R30" s="6">
         <f t="shared" si="2"/>
@@ -3527,11 +3542,11 @@
       </c>
       <c r="Z30" s="6">
         <f t="shared" si="3"/>
-        <v>1.7390373483466814</v>
+        <v>1.6939973039410039</v>
       </c>
       <c r="AA30" s="7">
         <f t="shared" si="4"/>
-        <v>0.62124408314467994</v>
+        <v>0.63027371887219596</v>
       </c>
       <c r="AB30" s="7">
         <f t="shared" si="5"/>
@@ -3555,10 +3570,10 @@
         <v>0</v>
       </c>
       <c r="F31" s="31">
-        <v>7798</v>
+        <v>7655</v>
       </c>
       <c r="G31" s="31">
-        <v>7962</v>
+        <v>8143</v>
       </c>
       <c r="H31" s="31">
         <v>9296</v>
@@ -3586,11 +3601,11 @@
       </c>
       <c r="P31" s="6">
         <f t="shared" si="0"/>
-        <v>0.50531363400725759</v>
+        <v>0.49604717470191811</v>
       </c>
       <c r="Q31" s="6">
         <f t="shared" si="1"/>
-        <v>0.37338210467079347</v>
+        <v>0.3818701932095292</v>
       </c>
       <c r="R31" s="6">
         <f t="shared" si="2"/>
@@ -3619,11 +3634,11 @@
       </c>
       <c r="Z31" s="6">
         <f t="shared" si="3"/>
-        <v>0.51289134438305706</v>
+        <v>0.503485924756643</v>
       </c>
       <c r="AA31" s="7">
         <f t="shared" si="4"/>
-        <v>0.4266881028938907</v>
+        <v>0.43638799571275455</v>
       </c>
       <c r="AB31" s="7">
         <f t="shared" si="5"/>
@@ -3647,10 +3662,10 @@
         <v>0</v>
       </c>
       <c r="F32" s="31">
-        <v>5359</v>
+        <v>5191</v>
       </c>
       <c r="G32" s="31">
-        <v>6079</v>
+        <v>6208</v>
       </c>
       <c r="H32" s="31">
         <v>6770</v>
@@ -3678,11 +3693,11 @@
       </c>
       <c r="P32" s="6">
         <f t="shared" si="0"/>
-        <v>0.30211974292479421</v>
+        <v>0.29264855113316046</v>
       </c>
       <c r="Q32" s="6">
         <f t="shared" si="1"/>
-        <v>0.21368062146296882</v>
+        <v>0.2182150514956589</v>
       </c>
       <c r="R32" s="6">
         <f t="shared" si="2"/>
@@ -3711,11 +3726,11 @@
       </c>
       <c r="Z32" s="6">
         <f t="shared" si="3"/>
-        <v>0.29516413306895795</v>
+        <v>0.28591099361092753</v>
       </c>
       <c r="AA32" s="7">
         <f t="shared" si="4"/>
-        <v>0.24458839623400661</v>
+        <v>0.24977870765269172</v>
       </c>
       <c r="AB32" s="7">
         <f t="shared" si="5"/>
@@ -3739,10 +3754,10 @@
         <v>0</v>
       </c>
       <c r="F33" s="31">
-        <v>19021</v>
+        <v>18411</v>
       </c>
       <c r="G33" s="31">
-        <v>21802</v>
+        <v>21568</v>
       </c>
       <c r="H33" s="29">
         <v>25070</v>
@@ -3770,11 +3785,11 @@
       </c>
       <c r="P33" s="6">
         <f t="shared" si="0"/>
-        <v>1.0482199933869722</v>
+        <v>1.0146037694257688</v>
       </c>
       <c r="Q33" s="6">
         <f t="shared" si="1"/>
-        <v>0.85220654340773172</v>
+        <v>0.84305984442794046</v>
       </c>
       <c r="R33" s="6">
         <f t="shared" si="2"/>
@@ -3803,11 +3818,11 @@
       </c>
       <c r="Z33" s="6">
         <f t="shared" si="3"/>
-        <v>1.1344307270233196</v>
+        <v>1.0980497405618179</v>
       </c>
       <c r="AA33" s="7">
         <f t="shared" si="4"/>
-        <v>0.99398194583751254</v>
+        <v>0.98331357709492118</v>
       </c>
       <c r="AB33" s="7">
         <f t="shared" si="5"/>
@@ -3831,10 +3846,10 @@
         <v>153</v>
       </c>
       <c r="F34" s="31">
-        <v>11821</v>
+        <v>11543</v>
       </c>
       <c r="G34" s="31">
-        <v>8711</v>
+        <v>8690</v>
       </c>
       <c r="H34" s="31">
         <v>10845</v>
@@ -3862,11 +3877,11 @@
       </c>
       <c r="P34" s="6">
         <f t="shared" si="0"/>
-        <v>0.38712952349762569</v>
+        <v>0.37802521696413949</v>
       </c>
       <c r="Q34" s="6">
         <f t="shared" si="1"/>
-        <v>0.22819794095302962</v>
+        <v>0.22764781389987687</v>
       </c>
       <c r="R34" s="6">
         <f t="shared" si="2"/>
@@ -3895,11 +3910,11 @@
       </c>
       <c r="Z34" s="6">
         <f t="shared" si="3"/>
-        <v>0.53527440681036043</v>
+        <v>0.52268610758920486</v>
       </c>
       <c r="AA34" s="7">
         <f t="shared" si="4"/>
-        <v>0.25844830143895564</v>
+        <v>0.25782524847945409</v>
       </c>
       <c r="AB34" s="7">
         <f t="shared" si="5"/>
@@ -3923,10 +3938,10 @@
         <v>185</v>
       </c>
       <c r="F35" s="31">
-        <v>12811</v>
+        <v>12479</v>
       </c>
       <c r="G35" s="31">
-        <v>8893</v>
+        <v>8852</v>
       </c>
       <c r="H35" s="31">
         <v>10951</v>
@@ -3954,11 +3969,11 @@
       </c>
       <c r="P35" s="6">
         <f t="shared" si="0"/>
-        <v>0.99387121799844846</v>
+        <v>0.96811481768813035</v>
       </c>
       <c r="Q35" s="6">
         <f t="shared" si="1"/>
-        <v>0.37031022277743075</v>
+        <v>0.36860295648552988</v>
       </c>
       <c r="R35" s="6">
         <f t="shared" si="2"/>
@@ -3987,11 +4002,11 @@
       </c>
       <c r="Z35" s="6">
         <f t="shared" si="3"/>
-        <v>1.0590228982392329</v>
+        <v>1.0315780772092253</v>
       </c>
       <c r="AA35" s="7">
         <f t="shared" si="4"/>
-        <v>0.42383948146029932</v>
+        <v>0.42188542560289771</v>
       </c>
       <c r="AB35" s="7">
         <f t="shared" si="5"/>
@@ -4015,10 +4030,10 @@
         <v>16</v>
       </c>
       <c r="F36" s="31">
-        <v>2596</v>
+        <v>2529</v>
       </c>
       <c r="G36" s="31">
-        <v>2148</v>
+        <v>2150</v>
       </c>
       <c r="H36" s="31">
         <v>2558</v>
@@ -4046,11 +4061,11 @@
       </c>
       <c r="P36" s="6">
         <f t="shared" si="0"/>
-        <v>0.3708041708327382</v>
+        <v>0.36123410941294098</v>
       </c>
       <c r="Q36" s="6">
         <f t="shared" si="1"/>
-        <v>0.19768083931529543</v>
+        <v>0.19786489968709736</v>
       </c>
       <c r="R36" s="6">
         <f t="shared" si="2"/>
@@ -4079,11 +4094,11 @@
       </c>
       <c r="Z36" s="6">
         <f t="shared" si="3"/>
-        <v>0.40530835284933647</v>
+        <v>0.39484777517564401</v>
       </c>
       <c r="AA36" s="7">
         <f t="shared" si="4"/>
-        <v>0.24840985312825256</v>
+        <v>0.24864114721868857</v>
       </c>
       <c r="AB36" s="7">
         <f t="shared" si="5"/>
@@ -4107,10 +4122,10 @@
         <v>56</v>
       </c>
       <c r="F37" s="32">
-        <v>2792</v>
+        <v>2727</v>
       </c>
       <c r="G37" s="32">
-        <v>2766</v>
+        <v>2785</v>
       </c>
       <c r="H37" s="32">
         <v>3399</v>
@@ -4138,11 +4153,11 @@
       </c>
       <c r="P37" s="10">
         <f t="shared" si="0"/>
-        <v>0.42022877784467189</v>
+        <v>0.41044551475015051</v>
       </c>
       <c r="Q37" s="10">
         <f t="shared" si="1"/>
-        <v>0.23073073073073072</v>
+        <v>0.23231564898231566</v>
       </c>
       <c r="R37" s="10">
         <f t="shared" si="2"/>
@@ -4171,11 +4186,11 @@
       </c>
       <c r="Z37" s="10">
         <f t="shared" si="3"/>
-        <v>0.99572039942938662</v>
+        <v>0.97253922967189732</v>
       </c>
       <c r="AA37" s="11">
         <f t="shared" si="4"/>
-        <v>0.67877300613496927</v>
+        <v>0.68343558282208594</v>
       </c>
       <c r="AB37" s="11">
         <f t="shared" si="5"/>
@@ -4204,11 +4219,11 @@
       </c>
       <c r="F38" s="30">
         <f>AVERAGE(F3:F6)</f>
-        <v>57298.25</v>
+        <v>55515.75</v>
       </c>
       <c r="G38" s="30">
         <f t="shared" ref="G38:H38" si="7">AVERAGE(G3:G6)</f>
-        <v>71138.25</v>
+        <v>70856.75</v>
       </c>
       <c r="H38" s="30">
         <f t="shared" si="7"/>
@@ -4244,11 +4259,11 @@
       </c>
       <c r="P38" s="12">
         <f>AVERAGE(P3:P6)</f>
-        <v>0.69125936175095659</v>
+        <v>0.66979050341209145</v>
       </c>
       <c r="Q38" s="12">
         <f>AVERAGE(Q3:Q6)</f>
-        <v>0.80069819974345768</v>
+        <v>0.79749241269707905</v>
       </c>
       <c r="R38" s="12">
         <f>AVERAGE(R3:R6)</f>
@@ -4284,11 +4299,11 @@
       </c>
       <c r="Z38" s="12">
         <f>AVERAGE(Z3:Z6)</f>
-        <v>1.3034217767413772</v>
+        <v>1.262479503082379</v>
       </c>
       <c r="AA38" s="13">
         <f>AVERAGE(AA3:AA6)</f>
-        <v>0.89103703077792207</v>
+        <v>0.88747125140395022</v>
       </c>
       <c r="AB38" s="13">
         <f>AVERAGE(AB3:AB6)</f>
@@ -4301,27 +4316,27 @@
       </c>
       <c r="B39" s="21">
         <f>COUNTIF(B7:B37,"=0")/COUNTA(B7:B37)</f>
-        <v>0.70967741935483875</v>
+        <v>0.74193548387096775</v>
       </c>
       <c r="C39" s="21">
         <f>COUNTIF(C7:C37,"=0")/COUNTA(C7:C37)</f>
-        <v>0.70967741935483875</v>
+        <v>0.74193548387096775</v>
       </c>
       <c r="D39" s="21">
         <f>COUNTIF(D7:D37,"=0")/COUNTA(D7:D37)</f>
-        <v>0.70967741935483875</v>
+        <v>0.74193548387096775</v>
       </c>
       <c r="E39" s="21">
         <f>COUNTIF(E7:E37,"=0")/COUNTA(E7:E37)</f>
-        <v>0.70967741935483875</v>
+        <v>0.74193548387096775</v>
       </c>
       <c r="F39" s="31">
         <f>AVERAGE(F7:F37)</f>
-        <v>15020.645161290322</v>
+        <v>14557.709677419354</v>
       </c>
       <c r="G39" s="31">
         <f t="shared" ref="G39:H39" si="12">AVERAGE(G7:G37)</f>
-        <v>16375.451612903225</v>
+        <v>16467.16129032258</v>
       </c>
       <c r="H39" s="31">
         <f t="shared" si="12"/>
@@ -4357,11 +4372,11 @@
       </c>
       <c r="P39" s="14">
         <f>AVERAGE(P7:P37)</f>
-        <v>0.62791270735995464</v>
+        <v>0.61002938667910434</v>
       </c>
       <c r="Q39" s="14">
         <f>AVERAGE(Q7:Q37)</f>
-        <v>0.418755960634136</v>
+        <v>0.42028218641232301</v>
       </c>
       <c r="R39" s="14">
         <f>AVERAGE(R7:R37)</f>
@@ -4397,11 +4412,11 @@
       </c>
       <c r="Z39" s="14">
         <f>AVERAGE(Z7:Z37)</f>
-        <v>0.80703788820570832</v>
+        <v>0.78356464480484345</v>
       </c>
       <c r="AA39" s="14">
         <f>AVERAGE(AA7:AA37)</f>
-        <v>0.47409892040137158</v>
+        <v>0.47581856508550435</v>
       </c>
       <c r="AB39" s="23">
         <f>AVERAGE(AB7:AB37)</f>
@@ -4415,27 +4430,27 @@
       </c>
       <c r="B40" s="22">
         <f>COUNTIF(B3:B37,"=0")/COUNTA(B3:B37)</f>
-        <v>0.74285714285714288</v>
+        <v>0.77142857142857146</v>
       </c>
       <c r="C40" s="22">
         <f>COUNTIF(C3:C37,"=0")/COUNTA(C3:C37)</f>
-        <v>0.74285714285714288</v>
+        <v>0.77142857142857146</v>
       </c>
       <c r="D40" s="22">
         <f>COUNTIF(D3:D37,"=0")/COUNTA(D3:D37)</f>
-        <v>0.74285714285714288</v>
+        <v>0.77142857142857146</v>
       </c>
       <c r="E40" s="22">
         <f>COUNTIF(E3:E37,"=0")/COUNTA(E3:E37)</f>
-        <v>0.74285714285714288</v>
+        <v>0.77142857142857146</v>
       </c>
       <c r="F40" s="33">
         <f>AVERAGE(F3:F37)</f>
-        <v>19852.371428571427</v>
+        <v>19238.628571428573</v>
       </c>
       <c r="G40" s="33">
         <f t="shared" ref="G40:H40" si="15">AVERAGE(G3:G37)</f>
-        <v>22634.057142857142</v>
+        <v>22683.114285714284</v>
       </c>
       <c r="H40" s="33">
         <f t="shared" si="15"/>
@@ -4471,11 +4486,11 @@
       </c>
       <c r="P40" s="15">
         <f>AVERAGE(P3:P37)</f>
-        <v>0.63515232500464069</v>
+        <v>0.6168592285914456</v>
       </c>
       <c r="Q40" s="15">
         <f>AVERAGE(Q3:Q37)</f>
-        <v>0.46240650224662999</v>
+        <v>0.46339192655915235</v>
       </c>
       <c r="R40" s="15">
         <f>AVERAGE(R3:R37)</f>
@@ -4511,11 +4526,11 @@
       </c>
       <c r="Z40" s="15">
         <f>AVERAGE(Z3:Z37)</f>
-        <v>0.86376747546692756</v>
+        <v>0.83829777146513329</v>
       </c>
       <c r="AA40" s="16">
         <f>AVERAGE(AA3:AA37)</f>
-        <v>0.52174899015869147</v>
+        <v>0.52286458637904099</v>
       </c>
       <c r="AB40" s="16">
         <f>AVERAGE(AB3:AB37)</f>

</xml_diff>

<commit_message>
Improved performance of pow function.
git-svn-id: https://svn.code.sf.net/p/half/code/trunk@414 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -171,20 +171,20 @@
     <t>rsqrt</t>
   </si>
   <si>
-    <t>half MFLOPS</t>
-  </si>
-  <si>
-    <t>float MFLOPS</t>
-  </si>
-  <si>
-    <t>double MFLOPS</t>
+    <t>half kFLOPS</t>
+  </si>
+  <si>
+    <t>float kFLOPS</t>
+  </si>
+  <si>
+    <t>double kFLOPS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,25 +207,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="19">
@@ -453,12 +441,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -505,10 +492,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -994,13 +979,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="30">
-        <v>43513</v>
+        <v>44955</v>
       </c>
       <c r="G3" s="30">
-        <v>57380</v>
+        <v>56825</v>
       </c>
       <c r="H3" s="30">
-        <v>69936</v>
+        <v>70078</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -1021,19 +1006,19 @@
         <v>110295</v>
       </c>
       <c r="O3" s="30">
-        <v>675479</v>
+        <v>683626</v>
       </c>
       <c r="P3" s="6">
         <f>F3/M3</f>
-        <v>0.4245999219359875</v>
+        <v>0.43867096018735363</v>
       </c>
       <c r="Q3" s="6">
         <f>G3/N3</f>
-        <v>0.52024117140396209</v>
+        <v>0.51520921165964007</v>
       </c>
       <c r="R3" s="6">
         <f>H3/O3</f>
-        <v>0.10353541708920633</v>
+        <v>0.1025092667628206</v>
       </c>
       <c r="S3" s="1">
         <v>0</v>
@@ -1054,19 +1039,19 @@
         <v>95649</v>
       </c>
       <c r="Y3" s="30">
-        <v>168833</v>
+        <v>176438</v>
       </c>
       <c r="Z3" s="6">
         <f>F3/W3</f>
-        <v>0.77927218023568179</v>
+        <v>0.80509688742433472</v>
       </c>
       <c r="AA3" s="7">
         <f>G3/X3</f>
-        <v>0.59990172401175135</v>
+        <v>0.59409925874813119</v>
       </c>
       <c r="AB3" s="7">
         <f>H3/Y3</f>
-        <v>0.41423181487031563</v>
+        <v>0.39718201294505717</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
@@ -1086,13 +1071,13 @@
         <v>0</v>
       </c>
       <c r="F4" s="31">
-        <v>35043</v>
+        <v>36138</v>
       </c>
       <c r="G4" s="31">
-        <v>57116</v>
+        <v>57182</v>
       </c>
       <c r="H4" s="31">
-        <v>69492</v>
+        <v>70437</v>
       </c>
       <c r="I4" s="2">
         <v>0</v>
@@ -1113,19 +1098,19 @@
         <v>111055</v>
       </c>
       <c r="O4" s="30">
-        <v>675518</v>
+        <v>682484</v>
       </c>
       <c r="P4" s="6">
         <f t="shared" ref="P4:P37" si="0">F4/M4</f>
-        <v>0.34261495292380795</v>
+        <v>0.35332075361015242</v>
       </c>
       <c r="Q4" s="6">
         <f t="shared" ref="Q4:Q37" si="1">G4/N4</f>
-        <v>0.51430372338030705</v>
+        <v>0.51489802350186842</v>
       </c>
       <c r="R4" s="6">
         <f t="shared" ref="R4:R37" si="2">H4/O4</f>
-        <v>0.1028721662487158</v>
+        <v>0.10320681510482298</v>
       </c>
       <c r="S4" s="2">
         <v>0</v>
@@ -1146,19 +1131,19 @@
         <v>95378</v>
       </c>
       <c r="Y4" s="30">
-        <v>168681</v>
+        <v>177054</v>
       </c>
       <c r="Z4" s="6">
         <f t="shared" ref="Z4:Z37" si="3">F4/W4</f>
-        <v>0.76469689695805876</v>
+        <v>0.78859162920612758</v>
       </c>
       <c r="AA4" s="7">
         <f t="shared" ref="AA4:AA37" si="4">G4/X4</f>
-        <v>0.59883830652771075</v>
+        <v>0.59953029000398417</v>
       </c>
       <c r="AB4" s="7">
         <f t="shared" ref="AB4:AB37" si="5">H4/Y4</f>
-        <v>0.4119728955839721</v>
+        <v>0.39782778135484087</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
@@ -1178,13 +1163,13 @@
         <v>0</v>
       </c>
       <c r="F5" s="31">
-        <v>78428</v>
+        <v>80906</v>
       </c>
       <c r="G5" s="31">
-        <v>92022</v>
+        <v>92249</v>
       </c>
       <c r="H5" s="31">
-        <v>129255</v>
+        <v>129191</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
@@ -1205,19 +1190,19 @@
         <v>82152</v>
       </c>
       <c r="O5" s="30">
-        <v>666954</v>
+        <v>670506</v>
       </c>
       <c r="P5" s="6">
         <f t="shared" si="0"/>
-        <v>0.99185552407932009</v>
+        <v>1.0231940509915014</v>
       </c>
       <c r="Q5" s="6">
         <f t="shared" si="1"/>
-        <v>1.1201431492842535</v>
+        <v>1.1229063199922096</v>
       </c>
       <c r="R5" s="6">
         <f t="shared" si="2"/>
-        <v>0.19379897264279095</v>
+        <v>0.19267687388330604</v>
       </c>
       <c r="S5" s="2">
         <v>0</v>
@@ -1238,19 +1223,19 @@
         <v>77126</v>
       </c>
       <c r="Y5" s="30">
-        <v>122435</v>
+        <v>125643</v>
       </c>
       <c r="Z5" s="6">
         <f t="shared" si="3"/>
-        <v>1.6197104562070177</v>
+        <v>1.6708865987897812</v>
       </c>
       <c r="AA5" s="7">
         <f t="shared" si="4"/>
-        <v>1.1931385006353241</v>
+        <v>1.1960817363794312</v>
       </c>
       <c r="AB5" s="7">
         <f t="shared" si="5"/>
-        <v>1.0557030260954792</v>
+        <v>1.028238739921842</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -1270,13 +1255,13 @@
         <v>0</v>
       </c>
       <c r="F6" s="31">
-        <v>65079</v>
+        <v>67278</v>
       </c>
       <c r="G6" s="31">
-        <v>76909</v>
+        <v>76399</v>
       </c>
       <c r="H6" s="31">
-        <v>115168</v>
+        <v>114094</v>
       </c>
       <c r="I6" s="2">
         <v>0</v>
@@ -1297,19 +1282,19 @@
         <v>74288</v>
       </c>
       <c r="O6" s="30">
-        <v>631902</v>
+        <v>625886</v>
       </c>
       <c r="P6" s="6">
         <f t="shared" si="0"/>
-        <v>0.92009161470925049</v>
+        <v>0.95118123595029058</v>
       </c>
       <c r="Q6" s="6">
         <f t="shared" si="1"/>
-        <v>1.0352816067197932</v>
+        <v>1.0284164333405126</v>
       </c>
       <c r="R6" s="6">
         <f t="shared" si="2"/>
-        <v>0.1822561093334093</v>
+        <v>0.18229198288506213</v>
       </c>
       <c r="S6" s="2">
         <v>0</v>
@@ -1330,19 +1315,19 @@
         <v>66415</v>
       </c>
       <c r="Y6" s="30">
-        <v>111147</v>
+        <v>113052</v>
       </c>
       <c r="Z6" s="6">
         <f t="shared" si="3"/>
-        <v>1.8862384789287578</v>
+        <v>1.949973914555678</v>
       </c>
       <c r="AA6" s="7">
         <f t="shared" si="4"/>
-        <v>1.1580064744410148</v>
+        <v>1.1503274862606339</v>
       </c>
       <c r="AB6" s="7">
         <f t="shared" si="5"/>
-        <v>1.036177314727343</v>
+        <v>1.0092169974878817</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
@@ -1362,13 +1347,13 @@
         <v>0</v>
       </c>
       <c r="F7" s="31">
-        <v>52088</v>
+        <v>53659</v>
       </c>
       <c r="G7" s="31">
-        <v>76683</v>
+        <v>76021</v>
       </c>
       <c r="H7" s="31">
-        <v>98482</v>
+        <v>99916</v>
       </c>
       <c r="I7" s="2">
         <v>0</v>
@@ -1389,19 +1374,19 @@
         <v>98344</v>
       </c>
       <c r="O7" s="30">
-        <v>215278</v>
+        <v>211627</v>
       </c>
       <c r="P7" s="6">
         <f t="shared" si="0"/>
-        <v>0.5946797579632378</v>
+        <v>0.61261559538760135</v>
       </c>
       <c r="Q7" s="6">
         <f t="shared" si="1"/>
-        <v>0.77974253640283087</v>
+        <v>0.77301106320670299</v>
       </c>
       <c r="R7" s="6">
         <f t="shared" si="2"/>
-        <v>0.45746430197233345</v>
+        <v>0.4721325728758618</v>
       </c>
       <c r="S7" s="2">
         <v>0</v>
@@ -1422,19 +1407,19 @@
         <v>90813</v>
       </c>
       <c r="Y7" s="30">
-        <v>148472</v>
+        <v>150617</v>
       </c>
       <c r="Z7" s="6">
         <f t="shared" si="3"/>
-        <v>0.87744891599144248</v>
+        <v>0.90391321193335916</v>
       </c>
       <c r="AA7" s="7">
         <f t="shared" si="4"/>
-        <v>0.84440553665224138</v>
+        <v>0.83711583143382551</v>
       </c>
       <c r="AB7" s="7">
         <f t="shared" si="5"/>
-        <v>0.6633035185085403</v>
+        <v>0.66337797194207826</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
@@ -1454,13 +1439,13 @@
         <v>0</v>
       </c>
       <c r="F8" s="31">
-        <v>42537</v>
+        <v>43894</v>
       </c>
       <c r="G8" s="31">
-        <v>50910</v>
+        <v>49996</v>
       </c>
       <c r="H8" s="31">
-        <v>67064</v>
+        <v>67165</v>
       </c>
       <c r="I8" s="2">
         <v>666</v>
@@ -1481,19 +1466,19 @@
         <v>95793</v>
       </c>
       <c r="O8" s="30">
-        <v>489142</v>
+        <v>475341</v>
       </c>
       <c r="P8" s="6">
         <f t="shared" si="0"/>
-        <v>0.49210425849442962</v>
+        <v>0.50780319068938784</v>
       </c>
       <c r="Q8" s="6">
         <f t="shared" si="1"/>
-        <v>0.53145845729855001</v>
+        <v>0.5219170503063898</v>
       </c>
       <c r="R8" s="6">
         <f t="shared" si="2"/>
-        <v>0.13710538044167134</v>
+        <v>0.14129856250565384</v>
       </c>
       <c r="S8" s="2">
         <v>0</v>
@@ -1514,19 +1499,19 @@
         <v>75398</v>
       </c>
       <c r="Y8" s="30">
-        <v>166482</v>
+        <v>167167</v>
       </c>
       <c r="Z8" s="6">
         <f t="shared" si="3"/>
-        <v>1.1227037584459461</v>
+        <v>1.158519847972973</v>
       </c>
       <c r="AA8" s="7">
         <f t="shared" si="4"/>
-        <v>0.67521684925329584</v>
+        <v>0.66309451179076373</v>
       </c>
       <c r="AB8" s="7">
         <f t="shared" si="5"/>
-        <v>0.40283033601230162</v>
+        <v>0.40178384489761737</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
@@ -1546,13 +1531,13 @@
         <v>0</v>
       </c>
       <c r="F9" s="31">
-        <v>13047</v>
+        <v>13389</v>
       </c>
       <c r="G9" s="31">
-        <v>14418</v>
+        <v>14699</v>
       </c>
       <c r="H9" s="31">
-        <v>16790</v>
+        <v>16396</v>
       </c>
       <c r="I9" s="2">
         <v>2</v>
@@ -1573,19 +1558,19 @@
         <v>28510</v>
       </c>
       <c r="O9" s="30">
-        <v>51567</v>
+        <v>52703</v>
       </c>
       <c r="P9" s="6">
         <f t="shared" si="0"/>
-        <v>0.43273631840796017</v>
+        <v>0.44407960199004975</v>
       </c>
       <c r="Q9" s="6">
         <f t="shared" si="1"/>
-        <v>0.50571729217818306</v>
+        <v>0.51557348298842509</v>
       </c>
       <c r="R9" s="6">
         <f t="shared" si="2"/>
-        <v>0.32559582678845</v>
+        <v>0.31110183481016263</v>
       </c>
       <c r="S9" s="2">
         <v>0</v>
@@ -1606,19 +1591,19 @@
         <v>28287</v>
       </c>
       <c r="Y9" s="30">
-        <v>41368</v>
+        <v>41755</v>
       </c>
       <c r="Z9" s="6">
         <f t="shared" si="3"/>
-        <v>0.5354812230658732</v>
+        <v>0.54951775087215271</v>
       </c>
       <c r="AA9" s="7">
         <f t="shared" si="4"/>
-        <v>0.5097041043588928</v>
+        <v>0.51963799625269558</v>
       </c>
       <c r="AB9" s="7">
         <f t="shared" si="5"/>
-        <v>0.40586927093405528</v>
+        <v>0.39267153634295293</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
@@ -1638,13 +1623,13 @@
         <v>0</v>
       </c>
       <c r="F10" s="31">
-        <v>13691</v>
+        <v>12475</v>
       </c>
       <c r="G10" s="31">
-        <v>13767</v>
+        <v>13776</v>
       </c>
       <c r="H10" s="31">
-        <v>15499</v>
+        <v>15267</v>
       </c>
       <c r="I10" s="2">
         <v>1</v>
@@ -1665,19 +1650,19 @@
         <v>14245</v>
       </c>
       <c r="O10" s="30">
-        <v>20045</v>
+        <v>20134</v>
       </c>
       <c r="P10" s="6">
         <f t="shared" si="0"/>
-        <v>1.7385396825396826</v>
+        <v>1.5841269841269841</v>
       </c>
       <c r="Q10" s="6">
         <f t="shared" si="1"/>
-        <v>0.96644436644436649</v>
+        <v>0.96707616707616706</v>
       </c>
       <c r="R10" s="6">
         <f t="shared" si="2"/>
-        <v>0.7732102768770267</v>
+        <v>0.75826959372206215</v>
       </c>
       <c r="S10" s="2">
         <v>0</v>
@@ -1698,19 +1683,19 @@
         <v>14457</v>
       </c>
       <c r="Y10" s="30">
-        <v>18539</v>
+        <v>18528</v>
       </c>
       <c r="Z10" s="6">
         <f t="shared" si="3"/>
-        <v>1.5433434787509863</v>
+        <v>1.4062676135723142</v>
       </c>
       <c r="AA10" s="7">
         <f t="shared" si="4"/>
-        <v>0.95227225565470019</v>
+        <v>0.95289479145050837</v>
       </c>
       <c r="AB10" s="7">
         <f t="shared" si="5"/>
-        <v>0.83602136037542474</v>
+        <v>0.82399611398963735</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
@@ -1730,13 +1715,13 @@
         <v>310</v>
       </c>
       <c r="F11" s="31">
-        <v>11405</v>
+        <v>11488</v>
       </c>
       <c r="G11" s="31">
-        <v>11768</v>
+        <v>11445</v>
       </c>
       <c r="H11" s="31">
-        <v>13395</v>
+        <v>13299</v>
       </c>
       <c r="I11" s="2">
         <v>2</v>
@@ -1757,19 +1742,19 @@
         <v>25565</v>
       </c>
       <c r="O11" s="30">
-        <v>42106</v>
+        <v>42657</v>
       </c>
       <c r="P11" s="6">
         <f t="shared" si="0"/>
-        <v>0.8578412937194434</v>
+        <v>0.86408424219631441</v>
       </c>
       <c r="Q11" s="6">
         <f t="shared" si="1"/>
-        <v>0.46031683942890672</v>
+        <v>0.44768237825151574</v>
       </c>
       <c r="R11" s="6">
         <f t="shared" si="2"/>
-        <v>0.31812568280055098</v>
+        <v>0.31176594697236093</v>
       </c>
       <c r="S11" s="2">
         <v>0</v>
@@ -1790,19 +1775,19 @@
         <v>25576</v>
       </c>
       <c r="Y11" s="30">
-        <v>36824</v>
+        <v>37089</v>
       </c>
       <c r="Z11" s="6">
         <f t="shared" si="3"/>
-        <v>0.7887275242047026</v>
+        <v>0.79446749654218529</v>
       </c>
       <c r="AA11" s="7">
         <f t="shared" si="4"/>
-        <v>0.46011886143259306</v>
+        <v>0.44748983421958088</v>
       </c>
       <c r="AB11" s="7">
         <f t="shared" si="5"/>
-        <v>0.36375733217466871</v>
+        <v>0.35856992639327023</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
@@ -1822,13 +1807,13 @@
         <v>0</v>
       </c>
       <c r="F12" s="31">
-        <v>8923</v>
+        <v>9084</v>
       </c>
       <c r="G12" s="31">
-        <v>9771</v>
+        <v>10232</v>
       </c>
       <c r="H12" s="31">
-        <v>10793</v>
+        <v>11184</v>
       </c>
       <c r="I12" s="2">
         <v>1</v>
@@ -1849,19 +1834,19 @@
         <v>56752</v>
       </c>
       <c r="O12" s="30">
-        <v>186449</v>
+        <v>191930</v>
       </c>
       <c r="P12" s="6">
         <f t="shared" si="0"/>
-        <v>0.20748267683579036</v>
+        <v>0.21122634051062641</v>
       </c>
       <c r="Q12" s="6">
         <f t="shared" si="1"/>
-        <v>0.172170143783479</v>
+        <v>0.18029320552579645</v>
       </c>
       <c r="R12" s="6">
         <f t="shared" si="2"/>
-        <v>5.788714340114455E-2</v>
+        <v>5.8271244724639189E-2</v>
       </c>
       <c r="S12" s="2">
         <v>0</v>
@@ -1882,19 +1867,19 @@
         <v>50282</v>
       </c>
       <c r="Y12" s="30">
-        <v>89837</v>
+        <v>89605</v>
       </c>
       <c r="Z12" s="6">
         <f t="shared" si="3"/>
-        <v>0.28971719861034451</v>
+        <v>0.29494464105977469</v>
       </c>
       <c r="AA12" s="7">
         <f t="shared" si="4"/>
-        <v>0.19432401256911022</v>
+        <v>0.2034923034087745</v>
       </c>
       <c r="AB12" s="7">
         <f t="shared" si="5"/>
-        <v>0.12013980876476285</v>
+        <v>0.12481446347860052</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
@@ -1914,13 +1899,13 @@
         <v>0</v>
       </c>
       <c r="F13" s="31">
-        <v>8688</v>
+        <v>8946</v>
       </c>
       <c r="G13" s="31">
-        <v>9289</v>
+        <v>10035</v>
       </c>
       <c r="H13" s="31">
-        <v>11182</v>
+        <v>11035</v>
       </c>
       <c r="I13" s="2">
         <v>5</v>
@@ -1941,19 +1926,19 @@
         <v>53052</v>
       </c>
       <c r="O13" s="30">
-        <v>175291</v>
+        <v>176231</v>
       </c>
       <c r="P13" s="6">
         <f t="shared" si="0"/>
-        <v>0.20391972773148692</v>
+        <v>0.20997535500528108</v>
       </c>
       <c r="Q13" s="6">
         <f t="shared" si="1"/>
-        <v>0.17509236221066124</v>
+        <v>0.18915403754806606</v>
       </c>
       <c r="R13" s="6">
         <f t="shared" si="2"/>
-        <v>6.3791067425024675E-2</v>
+        <v>6.261667924485477E-2</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -1974,19 +1959,19 @@
         <v>47631</v>
       </c>
       <c r="Y13" s="30">
-        <v>86797</v>
+        <v>87052</v>
       </c>
       <c r="Z13" s="6">
         <f t="shared" si="3"/>
-        <v>0.28791092258748674</v>
+        <v>0.29646076352067868</v>
       </c>
       <c r="AA13" s="7">
         <f t="shared" si="4"/>
-        <v>0.19502004996745817</v>
+        <v>0.21068211878818416</v>
       </c>
       <c r="AB13" s="7">
         <f t="shared" si="5"/>
-        <v>0.12882933741949606</v>
+        <v>0.12676331388135828</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -2006,13 +1991,13 @@
         <v>0</v>
       </c>
       <c r="F14" s="31">
-        <v>5795</v>
+        <v>6304</v>
       </c>
       <c r="G14" s="31">
-        <v>9930</v>
+        <v>9359</v>
       </c>
       <c r="H14" s="31">
-        <v>10845</v>
+        <v>10742</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
@@ -2033,19 +2018,19 @@
         <v>26892</v>
       </c>
       <c r="O14" s="30">
-        <v>34903</v>
+        <v>34928</v>
       </c>
       <c r="P14" s="6">
         <f t="shared" si="0"/>
-        <v>0.31102404465435807</v>
+        <v>0.33834263632460282</v>
       </c>
       <c r="Q14" s="6">
         <f t="shared" si="1"/>
-        <v>0.36925479696564034</v>
+        <v>0.34802171649561209</v>
       </c>
       <c r="R14" s="6">
         <f t="shared" si="2"/>
-        <v>0.31071827636592841</v>
+        <v>0.30754695373339441</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -2066,19 +2051,19 @@
         <v>35216</v>
       </c>
       <c r="Y14" s="30">
-        <v>57616</v>
+        <v>57677</v>
       </c>
       <c r="Z14" s="6">
         <f t="shared" si="3"/>
-        <v>0.3569448721897136</v>
+        <v>0.38829688943640284</v>
       </c>
       <c r="AA14" s="7">
         <f t="shared" si="4"/>
-        <v>0.28197410268059975</v>
+        <v>0.26575988187187644</v>
       </c>
       <c r="AB14" s="7">
         <f t="shared" si="5"/>
-        <v>0.18822896417661761</v>
+        <v>0.18624408343013679</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
@@ -2098,13 +2083,13 @@
         <v>868</v>
       </c>
       <c r="F15" s="31">
-        <v>7093</v>
+        <v>7325</v>
       </c>
       <c r="G15" s="31">
-        <v>8216</v>
+        <v>8267</v>
       </c>
       <c r="H15" s="31">
-        <v>9356</v>
+        <v>9328</v>
       </c>
       <c r="I15" s="2">
         <v>2</v>
@@ -2125,19 +2110,19 @@
         <v>37054</v>
       </c>
       <c r="O15" s="30">
-        <v>82806</v>
+        <v>80877</v>
       </c>
       <c r="P15" s="6">
         <f t="shared" si="0"/>
-        <v>0.26333766474846854</v>
+        <v>0.27195099313161314</v>
       </c>
       <c r="Q15" s="6">
         <f t="shared" si="1"/>
-        <v>0.22173044745506559</v>
+        <v>0.22310681707777838</v>
       </c>
       <c r="R15" s="6">
         <f t="shared" si="2"/>
-        <v>0.1129869816196894</v>
+        <v>0.11533563312190116</v>
       </c>
       <c r="S15" s="2">
         <v>0</v>
@@ -2158,19 +2143,19 @@
         <v>32550</v>
       </c>
       <c r="Y15" s="30">
-        <v>54341</v>
+        <v>54051</v>
       </c>
       <c r="Z15" s="6">
         <f t="shared" si="3"/>
-        <v>0.30487857296367937</v>
+        <v>0.3148506339995702</v>
       </c>
       <c r="AA15" s="7">
         <f t="shared" si="4"/>
-        <v>0.25241167434715822</v>
+        <v>0.2539784946236559</v>
       </c>
       <c r="AB15" s="7">
         <f t="shared" si="5"/>
-        <v>0.17217202480631566</v>
+        <v>0.17257775064291134</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
@@ -2190,13 +2175,13 @@
         <v>0</v>
       </c>
       <c r="F16" s="31">
-        <v>21223</v>
+        <v>21587</v>
       </c>
       <c r="G16" s="31">
-        <v>21779</v>
+        <v>21281</v>
       </c>
       <c r="H16" s="31">
-        <v>24463</v>
+        <v>24211</v>
       </c>
       <c r="I16" s="2">
         <v>0</v>
@@ -2217,19 +2202,19 @@
         <v>86268</v>
       </c>
       <c r="O16" s="30">
-        <v>239487</v>
+        <v>243415</v>
       </c>
       <c r="P16" s="6">
         <f t="shared" si="0"/>
-        <v>0.27503758229226066</v>
+        <v>0.27975480794152713</v>
       </c>
       <c r="Q16" s="6">
         <f t="shared" si="1"/>
-        <v>0.25245745815366066</v>
+        <v>0.2466847498493068</v>
       </c>
       <c r="R16" s="6">
         <f t="shared" si="2"/>
-        <v>0.10214750696279964</v>
+        <v>9.9463878561304772E-2</v>
       </c>
       <c r="S16" s="2">
         <v>0</v>
@@ -2250,19 +2235,19 @@
         <v>78721</v>
       </c>
       <c r="Y16" s="30">
-        <v>128405</v>
+        <v>128436</v>
       </c>
       <c r="Z16" s="6">
         <f t="shared" si="3"/>
-        <v>0.45377378661535173</v>
+        <v>0.46155655334616208</v>
       </c>
       <c r="AA16" s="7">
         <f t="shared" si="4"/>
-        <v>0.27666061152678445</v>
+        <v>0.27033447237712938</v>
       </c>
       <c r="AB16" s="7">
         <f t="shared" si="5"/>
-        <v>0.19051438806900042</v>
+        <v>0.18850633778691334</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
@@ -2282,13 +2267,13 @@
         <v>0</v>
       </c>
       <c r="F17" s="31">
-        <v>44739</v>
+        <v>48872</v>
       </c>
       <c r="G17" s="31">
-        <v>48418</v>
-      </c>
-      <c r="H17" s="36">
-        <v>75106</v>
+        <v>52614</v>
+      </c>
+      <c r="H17" s="29">
+        <v>76503</v>
       </c>
       <c r="I17" s="2">
         <v>0</v>
@@ -2309,19 +2294,19 @@
         <v>75498</v>
       </c>
       <c r="O17" s="30">
-        <v>146565</v>
+        <v>146085</v>
       </c>
       <c r="P17" s="6">
         <f t="shared" si="0"/>
-        <v>0.64634921552197411</v>
+        <v>0.70605911757057416</v>
       </c>
       <c r="Q17" s="6">
         <f t="shared" si="1"/>
-        <v>0.64131500172189992</v>
+        <v>0.69689263291742831</v>
       </c>
       <c r="R17" s="6">
         <f t="shared" si="2"/>
-        <v>0.51244157882168317</v>
+        <v>0.52368826368210286</v>
       </c>
       <c r="S17" s="2">
         <v>0</v>
@@ -2342,19 +2327,19 @@
         <v>66205</v>
       </c>
       <c r="Y17" s="30">
-        <v>110443</v>
+        <v>110373</v>
       </c>
       <c r="Z17" s="6">
         <f t="shared" si="3"/>
-        <v>1.2370800497718788</v>
+        <v>1.3513618139084751</v>
       </c>
       <c r="AA17" s="7">
         <f t="shared" si="4"/>
-        <v>0.73133449135261686</v>
+        <v>0.79471339022732423</v>
       </c>
       <c r="AB17" s="7">
         <f t="shared" si="5"/>
-        <v>0.68004309915522032</v>
+        <v>0.69313147237096029</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
@@ -2374,13 +2359,13 @@
         <v>0</v>
       </c>
       <c r="F18" s="31">
-        <v>4723</v>
+        <v>4939</v>
       </c>
       <c r="G18" s="31">
-        <v>4742</v>
+        <v>4762</v>
       </c>
       <c r="H18" s="31">
-        <v>5298</v>
+        <v>5366</v>
       </c>
       <c r="I18" s="2">
         <v>20</v>
@@ -2401,19 +2386,19 @@
         <v>20295</v>
       </c>
       <c r="O18" s="30">
-        <v>29023</v>
+        <v>29080</v>
       </c>
       <c r="P18" s="6">
         <f t="shared" si="0"/>
-        <v>0.35112631031150099</v>
+        <v>0.36718459594082226</v>
       </c>
       <c r="Q18" s="6">
         <f t="shared" si="1"/>
-        <v>0.23365360926336537</v>
+        <v>0.2346390736634639</v>
       </c>
       <c r="R18" s="6">
         <f t="shared" si="2"/>
-        <v>0.18254487820004825</v>
+        <v>0.18452544704264098</v>
       </c>
       <c r="S18" s="2">
         <v>0</v>
@@ -2434,19 +2419,19 @@
         <v>13857</v>
       </c>
       <c r="Y18" s="30">
-        <v>20473</v>
+        <v>20508</v>
       </c>
       <c r="Z18" s="6">
         <f t="shared" si="3"/>
-        <v>0.46186192059456288</v>
+        <v>0.48298454918834344</v>
       </c>
       <c r="AA18" s="7">
         <f t="shared" si="4"/>
-        <v>0.34220971350220103</v>
+        <v>0.34365302735079745</v>
       </c>
       <c r="AB18" s="7">
         <f t="shared" si="5"/>
-        <v>0.25877985639622919</v>
+        <v>0.26165398868734152</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
@@ -2466,13 +2451,13 @@
         <v>13016</v>
       </c>
       <c r="F19" s="31">
-        <v>8258</v>
+        <v>13482</v>
       </c>
       <c r="G19" s="31">
-        <v>8657</v>
+        <v>14023</v>
       </c>
       <c r="H19" s="31">
-        <v>10277</v>
+        <v>17053</v>
       </c>
       <c r="I19" s="2">
         <v>64079</v>
@@ -2493,19 +2478,19 @@
         <v>14941</v>
       </c>
       <c r="O19" s="30">
-        <v>20708</v>
+        <v>21163</v>
       </c>
       <c r="P19" s="6">
         <f t="shared" si="0"/>
-        <v>0.53007253353873807</v>
+        <v>0.86539572501444251</v>
       </c>
       <c r="Q19" s="6">
         <f t="shared" si="1"/>
-        <v>0.57941235526403856</v>
+        <v>0.93855832942908779</v>
       </c>
       <c r="R19" s="6">
         <f t="shared" si="2"/>
-        <v>0.49628163028781147</v>
+        <v>0.80579312951849924</v>
       </c>
       <c r="S19" s="2">
         <v>0</v>
@@ -2526,19 +2511,19 @@
         <v>12189</v>
       </c>
       <c r="Y19" s="30">
-        <v>16667</v>
+        <v>17671</v>
       </c>
       <c r="Z19" s="6">
         <f t="shared" si="3"/>
-        <v>0.59392980437284237</v>
+        <v>0.96964902186421176</v>
       </c>
       <c r="AA19" s="7">
         <f t="shared" si="4"/>
-        <v>0.71023053572893591</v>
+        <v>1.1504635326934121</v>
       </c>
       <c r="AB19" s="7">
         <f t="shared" si="5"/>
-        <v>0.61660766784664311</v>
+        <v>0.96502744609812685</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
@@ -2558,13 +2543,13 @@
         <v>0</v>
       </c>
       <c r="F20" s="31">
-        <v>16638</v>
+        <v>17200</v>
       </c>
       <c r="G20" s="31">
-        <v>16706</v>
+        <v>17143</v>
       </c>
       <c r="H20" s="31">
-        <v>20018</v>
+        <v>20613</v>
       </c>
       <c r="I20" s="2">
         <v>50512</v>
@@ -2585,19 +2570,19 @@
         <v>57240</v>
       </c>
       <c r="O20" s="30">
-        <v>167594</v>
+        <v>168789</v>
       </c>
       <c r="P20" s="6">
         <f t="shared" si="0"/>
-        <v>0.34658889698989687</v>
+        <v>0.35829601083220497</v>
       </c>
       <c r="Q20" s="6">
         <f t="shared" si="1"/>
-        <v>0.29185883997204753</v>
+        <v>0.29949336128581411</v>
       </c>
       <c r="R20" s="6">
         <f t="shared" si="2"/>
-        <v>0.11944341682876475</v>
+        <v>0.12212288715496863</v>
       </c>
       <c r="S20" s="2">
         <v>0</v>
@@ -2618,19 +2603,19 @@
         <v>46897</v>
       </c>
       <c r="Y20" s="30">
-        <v>80184</v>
+        <v>83724</v>
       </c>
       <c r="Z20" s="6">
         <f t="shared" si="3"/>
-        <v>1.9767137935131283</v>
+        <v>2.0434834263989545</v>
       </c>
       <c r="AA20" s="7">
         <f t="shared" si="4"/>
-        <v>0.35622747723734993</v>
+        <v>0.36554577051837006</v>
       </c>
       <c r="AB20" s="7">
         <f t="shared" si="5"/>
-        <v>0.24965080315274868</v>
+        <v>0.24620180593378244</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
@@ -2650,13 +2635,13 @@
         <v>0</v>
       </c>
       <c r="F21" s="31">
-        <v>13569</v>
+        <v>14000</v>
       </c>
       <c r="G21" s="31">
-        <v>14358</v>
+        <v>14345</v>
       </c>
       <c r="H21" s="31">
-        <v>21553</v>
+        <v>21545</v>
       </c>
       <c r="I21" s="2">
         <v>4</v>
@@ -2677,19 +2662,19 @@
         <v>34783</v>
       </c>
       <c r="O21" s="30">
-        <v>71034</v>
+        <v>71456</v>
       </c>
       <c r="P21" s="6">
         <f t="shared" si="0"/>
-        <v>0.34900589006918903</v>
+        <v>0.36009156614110444</v>
       </c>
       <c r="Q21" s="6">
         <f t="shared" si="1"/>
-        <v>0.41278785613661845</v>
+        <v>0.41241411034125869</v>
       </c>
       <c r="R21" s="6">
         <f t="shared" si="2"/>
-        <v>0.30341808148210714</v>
+        <v>0.30151421854008059</v>
       </c>
       <c r="S21" s="2">
         <v>0</v>
@@ -2710,19 +2695,19 @@
         <v>38610</v>
       </c>
       <c r="Y21" s="30">
-        <v>54036</v>
+        <v>57013</v>
       </c>
       <c r="Z21" s="6">
         <f t="shared" si="3"/>
-        <v>0.46558468295360966</v>
+        <v>0.48037331869338457</v>
       </c>
       <c r="AA21" s="7">
         <f t="shared" si="4"/>
-        <v>0.37187257187257189</v>
+        <v>0.37153587153587153</v>
       </c>
       <c r="AB21" s="7">
         <f t="shared" si="5"/>
-        <v>0.39886372048264118</v>
+        <v>0.37789626927192044</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
@@ -2742,13 +2727,13 @@
         <v>0</v>
       </c>
       <c r="F22" s="31">
-        <v>13395</v>
+        <v>13805</v>
       </c>
       <c r="G22" s="31">
-        <v>14738</v>
+        <v>14883</v>
       </c>
       <c r="H22" s="31">
-        <v>21515</v>
+        <v>20638</v>
       </c>
       <c r="I22" s="2">
         <v>2</v>
@@ -2769,19 +2754,19 @@
         <v>39651</v>
       </c>
       <c r="O22" s="30">
-        <v>72352</v>
+        <v>72286</v>
       </c>
       <c r="P22" s="6">
         <f t="shared" si="0"/>
-        <v>0.33764367816091956</v>
+        <v>0.34797842306916715</v>
       </c>
       <c r="Q22" s="6">
         <f t="shared" si="1"/>
-        <v>0.37169302161357848</v>
+        <v>0.37534992812287205</v>
       </c>
       <c r="R22" s="6">
         <f t="shared" si="2"/>
-        <v>0.29736565678903143</v>
+        <v>0.28550480037628312</v>
       </c>
       <c r="S22" s="2">
         <v>0</v>
@@ -2802,19 +2787,19 @@
         <v>39154</v>
       </c>
       <c r="Y22" s="30">
-        <v>56497</v>
+        <v>58534</v>
       </c>
       <c r="Z22" s="6">
         <f t="shared" si="3"/>
-        <v>0.45702685182025998</v>
+        <v>0.47101572895697569</v>
       </c>
       <c r="AA22" s="7">
         <f t="shared" si="4"/>
-        <v>0.37641109465188743</v>
+        <v>0.38011441998263268</v>
       </c>
       <c r="AB22" s="7">
         <f t="shared" si="5"/>
-        <v>0.38081668053170964</v>
+        <v>0.35258140567875079</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
@@ -2834,13 +2819,13 @@
         <v>0</v>
       </c>
       <c r="F23" s="31">
-        <v>10523</v>
+        <v>10716</v>
       </c>
       <c r="G23" s="31">
-        <v>12292</v>
+        <v>12280</v>
       </c>
       <c r="H23" s="31">
-        <v>17491</v>
+        <v>17365</v>
       </c>
       <c r="I23" s="2">
         <v>6</v>
@@ -2861,19 +2846,19 @@
         <v>39756</v>
       </c>
       <c r="O23" s="30">
-        <v>81048</v>
+        <v>80586</v>
       </c>
       <c r="P23" s="6">
         <f t="shared" si="0"/>
-        <v>0.3661957126948775</v>
+        <v>0.37291202672605789</v>
       </c>
       <c r="Q23" s="6">
         <f t="shared" si="1"/>
-        <v>0.30918603481235535</v>
+        <v>0.30888419358084312</v>
       </c>
       <c r="R23" s="6">
         <f t="shared" si="2"/>
-        <v>0.21581038396999308</v>
+        <v>0.21548407912044276</v>
       </c>
       <c r="S23" s="2">
         <v>0</v>
@@ -2894,19 +2879,19 @@
         <v>29913</v>
       </c>
       <c r="Y23" s="30">
-        <v>50392</v>
+        <v>52277</v>
       </c>
       <c r="Z23" s="6">
         <f t="shared" si="3"/>
-        <v>0.45722354985878777</v>
+        <v>0.46560938518357592</v>
       </c>
       <c r="AA23" s="7">
         <f t="shared" si="4"/>
-        <v>0.41092501587938357</v>
+        <v>0.41052385250559958</v>
       </c>
       <c r="AB23" s="7">
         <f t="shared" si="5"/>
-        <v>0.34709874583267186</v>
+        <v>0.33217284848021117</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
@@ -2926,13 +2911,13 @@
         <v>0</v>
       </c>
       <c r="F24" s="31">
-        <v>18897</v>
+        <v>19547</v>
       </c>
       <c r="G24" s="31">
-        <v>20587</v>
+        <v>20529</v>
       </c>
       <c r="H24" s="29">
-        <v>25738</v>
+        <v>25779</v>
       </c>
       <c r="I24" s="2">
         <v>0</v>
@@ -2953,19 +2938,19 @@
         <v>43686</v>
       </c>
       <c r="O24" s="30">
-        <v>95237</v>
+        <v>96754</v>
       </c>
       <c r="P24" s="6">
         <f t="shared" si="0"/>
-        <v>0.4330400109995875</v>
+        <v>0.44793528576011732</v>
       </c>
       <c r="Q24" s="6">
         <f t="shared" si="1"/>
-        <v>0.47124937050771415</v>
+        <v>0.46992171405026784</v>
       </c>
       <c r="R24" s="6">
         <f t="shared" si="2"/>
-        <v>0.27025210789924087</v>
+        <v>0.26643859685387683</v>
       </c>
       <c r="S24" s="2">
         <v>0</v>
@@ -2986,19 +2971,19 @@
         <v>38177</v>
       </c>
       <c r="Y24" s="30">
-        <v>53238</v>
+        <v>55547</v>
       </c>
       <c r="Z24" s="6">
         <f t="shared" si="3"/>
-        <v>0.57978707084343262</v>
+        <v>0.59973000337495785</v>
       </c>
       <c r="AA24" s="7">
         <f t="shared" si="4"/>
-        <v>0.53925138172197917</v>
+        <v>0.53773214238939671</v>
       </c>
       <c r="AB24" s="7">
         <f t="shared" si="5"/>
-        <v>0.48345166985987453</v>
+        <v>0.46409347039444077</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
@@ -3018,13 +3003,13 @@
         <v>0</v>
       </c>
       <c r="F25" s="31">
-        <v>7718</v>
+        <v>7954</v>
       </c>
       <c r="G25" s="31">
-        <v>8151</v>
+        <v>8099</v>
       </c>
       <c r="H25" s="31">
-        <v>11328</v>
+        <v>11289</v>
       </c>
       <c r="I25" s="2">
         <v>3</v>
@@ -3045,19 +3030,19 @@
         <v>43736</v>
       </c>
       <c r="O25" s="30">
-        <v>88010</v>
+        <v>89254</v>
       </c>
       <c r="P25" s="6">
         <f t="shared" si="0"/>
-        <v>0.17663752460292031</v>
+        <v>0.18203872385224515</v>
       </c>
       <c r="Q25" s="6">
         <f t="shared" si="1"/>
-        <v>0.18636820925553321</v>
+        <v>0.18517925736235596</v>
       </c>
       <c r="R25" s="6">
         <f t="shared" si="2"/>
-        <v>0.1287126462901943</v>
+        <v>0.12648172630918503</v>
       </c>
       <c r="S25" s="2">
         <v>0</v>
@@ -3078,19 +3063,19 @@
         <v>38418</v>
       </c>
       <c r="Y25" s="30">
-        <v>55175</v>
+        <v>56801</v>
       </c>
       <c r="Z25" s="6">
         <f t="shared" si="3"/>
-        <v>0.24356991826301005</v>
+        <v>0.25101776753873828</v>
       </c>
       <c r="AA25" s="7">
         <f t="shared" si="4"/>
-        <v>0.21216617210682492</v>
+        <v>0.21081263990837629</v>
       </c>
       <c r="AB25" s="7">
         <f t="shared" si="5"/>
-        <v>0.20531037607612143</v>
+        <v>0.19874650094188481</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
@@ -3110,13 +3095,13 @@
         <v>0</v>
       </c>
       <c r="F26" s="31">
-        <v>15398</v>
+        <v>15902</v>
       </c>
       <c r="G26" s="31">
-        <v>17855</v>
+        <v>17771</v>
       </c>
       <c r="H26" s="31">
-        <v>25556</v>
+        <v>25471</v>
       </c>
       <c r="I26" s="2">
         <v>6</v>
@@ -3137,19 +3122,19 @@
         <v>37567</v>
       </c>
       <c r="O26" s="30">
-        <v>69491</v>
+        <v>69568</v>
       </c>
       <c r="P26" s="6">
         <f t="shared" si="0"/>
-        <v>0.47233128834355831</v>
+        <v>0.48779141104294477</v>
       </c>
       <c r="Q26" s="6">
         <f t="shared" si="1"/>
-        <v>0.47528415896930815</v>
+        <v>0.47304815396491601</v>
       </c>
       <c r="R26" s="6">
         <f t="shared" si="2"/>
-        <v>0.36775985379401649</v>
+        <v>0.36613097976080955</v>
       </c>
       <c r="S26" s="2">
         <v>0</v>
@@ -3170,19 +3155,19 @@
         <v>33602</v>
       </c>
       <c r="Y26" s="30">
-        <v>47059</v>
+        <v>49062</v>
       </c>
       <c r="Z26" s="6">
         <f t="shared" si="3"/>
-        <v>0.65176719576719577</v>
+        <v>0.67310052910052909</v>
       </c>
       <c r="AA26" s="7">
         <f t="shared" si="4"/>
-        <v>0.53136718052496879</v>
+        <v>0.5288673293256354</v>
       </c>
       <c r="AB26" s="7">
         <f t="shared" si="5"/>
-        <v>0.54306296351388683</v>
+        <v>0.51915943092413686</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
@@ -3202,13 +3187,13 @@
         <v>913439</v>
       </c>
       <c r="F27" s="31">
-        <v>12472</v>
+        <v>12818</v>
       </c>
       <c r="G27" s="31">
-        <v>13820</v>
+        <v>14029</v>
       </c>
       <c r="H27" s="31">
-        <v>20918</v>
+        <v>20837</v>
       </c>
       <c r="I27" s="2">
         <v>716930</v>
@@ -3229,19 +3214,19 @@
         <v>28190</v>
       </c>
       <c r="O27" s="30">
-        <v>47229</v>
+        <v>47123</v>
       </c>
       <c r="P27" s="6">
         <f t="shared" si="0"/>
-        <v>1.0123376623376623</v>
+        <v>1.0404220779220779</v>
       </c>
       <c r="Q27" s="6">
         <f t="shared" si="1"/>
-        <v>0.49024476764810215</v>
+        <v>0.49765874423554451</v>
       </c>
       <c r="R27" s="6">
         <f t="shared" si="2"/>
-        <v>0.44290584174977238</v>
+        <v>0.44218322263013815</v>
       </c>
       <c r="S27" s="2">
         <v>0</v>
@@ -3262,19 +3247,19 @@
         <v>20920</v>
       </c>
       <c r="Y27" s="30">
-        <v>33145</v>
+        <v>34550</v>
       </c>
       <c r="Z27" s="6">
         <f t="shared" si="3"/>
-        <v>1.065891804119306</v>
+        <v>1.0954619263310827</v>
       </c>
       <c r="AA27" s="7">
         <f t="shared" si="4"/>
-        <v>0.66061185468451245</v>
+        <v>0.67060229445506692</v>
       </c>
       <c r="AB27" s="7">
         <f t="shared" si="5"/>
-        <v>0.63110574747322368</v>
+        <v>0.60309696092619391</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
@@ -3294,13 +3279,13 @@
         <v>0</v>
       </c>
       <c r="F28" s="31">
-        <v>9999</v>
+        <v>10235</v>
       </c>
       <c r="G28" s="31">
-        <v>10934</v>
+        <v>10816</v>
       </c>
       <c r="H28" s="31">
-        <v>12236</v>
+        <v>12436</v>
       </c>
       <c r="I28" s="2">
         <v>2</v>
@@ -3321,19 +3306,19 @@
         <v>20407</v>
       </c>
       <c r="O28" s="30">
-        <v>34992</v>
+        <v>35396</v>
       </c>
       <c r="P28" s="6">
         <f t="shared" si="0"/>
-        <v>1.6114423851732473</v>
+        <v>1.6494762288477034</v>
       </c>
       <c r="Q28" s="6">
         <f t="shared" si="1"/>
-        <v>0.535796540402803</v>
+        <v>0.53001421081001621</v>
       </c>
       <c r="R28" s="6">
         <f t="shared" si="2"/>
-        <v>0.34967992684042065</v>
+        <v>0.35133913436546504</v>
       </c>
       <c r="S28" s="2">
         <v>0</v>
@@ -3354,19 +3339,19 @@
         <v>21639</v>
       </c>
       <c r="Y28" s="30">
-        <v>28036</v>
+        <v>30289</v>
       </c>
       <c r="Z28" s="6">
         <f t="shared" si="3"/>
-        <v>1.635159443990188</v>
+        <v>1.6737530662305806</v>
       </c>
       <c r="AA28" s="7">
         <f t="shared" si="4"/>
-        <v>0.50529137205970698</v>
+        <v>0.4998382550025417</v>
       </c>
       <c r="AB28" s="7">
         <f t="shared" si="5"/>
-        <v>0.43643886431730633</v>
+        <v>0.41057809765921621</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
@@ -3386,13 +3371,13 @@
         <v>0</v>
       </c>
       <c r="F29" s="31">
-        <v>8572</v>
+        <v>8791</v>
       </c>
       <c r="G29" s="31">
-        <v>9797</v>
+        <v>9730</v>
       </c>
       <c r="H29" s="31">
-        <v>11075</v>
+        <v>11251</v>
       </c>
       <c r="I29" s="2">
         <v>2</v>
@@ -3413,19 +3398,19 @@
         <v>19983</v>
       </c>
       <c r="O29" s="30">
-        <v>34354</v>
+        <v>35133</v>
       </c>
       <c r="P29" s="6">
         <f t="shared" si="0"/>
-        <v>1.3776920604307297</v>
+        <v>1.4128897460623593</v>
       </c>
       <c r="Q29" s="6">
         <f t="shared" si="1"/>
-        <v>0.49026672671771004</v>
+        <v>0.48691387679527598</v>
       </c>
       <c r="R29" s="6">
         <f t="shared" si="2"/>
-        <v>0.32237876229842233</v>
+        <v>0.32024022998320667</v>
       </c>
       <c r="S29" s="2">
         <v>0</v>
@@ -3446,19 +3431,19 @@
         <v>21828</v>
       </c>
       <c r="Y29" s="30">
-        <v>29632</v>
+        <v>31901</v>
       </c>
       <c r="Z29" s="6">
         <f t="shared" si="3"/>
-        <v>1.4008824971400555</v>
+        <v>1.436672658931198</v>
       </c>
       <c r="AA29" s="7">
         <f t="shared" si="4"/>
-        <v>0.44882719442917351</v>
+        <v>0.44575774234927618</v>
       </c>
       <c r="AB29" s="7">
         <f t="shared" si="5"/>
-        <v>0.37375134989200864</v>
+        <v>0.35268486881288985</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
@@ -3478,13 +3463,13 @@
         <v>0</v>
       </c>
       <c r="F30" s="31">
-        <v>21363</v>
+        <v>21929</v>
       </c>
       <c r="G30" s="31">
-        <v>24500</v>
+        <v>24304</v>
       </c>
       <c r="H30" s="29">
-        <v>27794</v>
+        <v>27994</v>
       </c>
       <c r="I30" s="2">
         <v>0</v>
@@ -3505,19 +3490,19 @@
         <v>38542</v>
       </c>
       <c r="O30" s="30">
-        <v>75465</v>
+        <v>75786</v>
       </c>
       <c r="P30" s="6">
         <f t="shared" si="0"/>
-        <v>1.6026256564141035</v>
+        <v>1.645086271567892</v>
       </c>
       <c r="Q30" s="6">
         <f t="shared" si="1"/>
-        <v>0.6356701779876498</v>
+        <v>0.63058481656374865</v>
       </c>
       <c r="R30" s="6">
         <f t="shared" si="2"/>
-        <v>0.36830318690783809</v>
+        <v>0.36938220779563508</v>
       </c>
       <c r="S30" s="2">
         <v>0</v>
@@ -3538,19 +3523,19 @@
         <v>38872</v>
       </c>
       <c r="Y30" s="30">
-        <v>48874</v>
+        <v>51907</v>
       </c>
       <c r="Z30" s="6">
         <f t="shared" si="3"/>
-        <v>1.6939973039410039</v>
+        <v>1.7388787566410278</v>
       </c>
       <c r="AA30" s="7">
         <f t="shared" si="4"/>
-        <v>0.63027371887219596</v>
+        <v>0.62523152912121838</v>
       </c>
       <c r="AB30" s="7">
         <f t="shared" si="5"/>
-        <v>0.5686868273519663</v>
+        <v>0.53931069027298828</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
@@ -3570,13 +3555,13 @@
         <v>0</v>
       </c>
       <c r="F31" s="31">
-        <v>7655</v>
+        <v>7909</v>
       </c>
       <c r="G31" s="31">
-        <v>8143</v>
+        <v>8172</v>
       </c>
       <c r="H31" s="31">
-        <v>9296</v>
+        <v>9280</v>
       </c>
       <c r="I31" s="2">
         <v>4</v>
@@ -3597,19 +3582,19 @@
         <v>21324</v>
       </c>
       <c r="O31" s="30">
-        <v>33377</v>
+        <v>33454</v>
       </c>
       <c r="P31" s="6">
         <f t="shared" si="0"/>
-        <v>0.49604717470191811</v>
+        <v>0.51250648004147226</v>
       </c>
       <c r="Q31" s="6">
         <f t="shared" si="1"/>
-        <v>0.3818701932095292</v>
+        <v>0.38323016319639841</v>
       </c>
       <c r="R31" s="6">
         <f t="shared" si="2"/>
-        <v>0.2785151451598406</v>
+        <v>0.27739582710587674</v>
       </c>
       <c r="S31" s="2">
         <v>0</v>
@@ -3630,19 +3615,19 @@
         <v>18660</v>
       </c>
       <c r="Y31" s="30">
-        <v>28398</v>
+        <v>28586</v>
       </c>
       <c r="Z31" s="6">
         <f t="shared" si="3"/>
-        <v>0.503485924756643</v>
+        <v>0.52019205472244145</v>
       </c>
       <c r="AA31" s="7">
         <f t="shared" si="4"/>
-        <v>0.43638799571275455</v>
+        <v>0.4379421221864952</v>
       </c>
       <c r="AB31" s="7">
         <f t="shared" si="5"/>
-        <v>0.32734699626734276</v>
+        <v>0.32463443643741691</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
@@ -3662,13 +3647,13 @@
         <v>0</v>
       </c>
       <c r="F32" s="31">
-        <v>5191</v>
+        <v>5344</v>
       </c>
       <c r="G32" s="31">
-        <v>6208</v>
+        <v>6175</v>
       </c>
       <c r="H32" s="31">
-        <v>6770</v>
+        <v>6838</v>
       </c>
       <c r="I32" s="2">
         <v>1</v>
@@ -3689,19 +3674,19 @@
         <v>28449</v>
       </c>
       <c r="O32" s="30">
-        <v>60018</v>
+        <v>57370</v>
       </c>
       <c r="P32" s="6">
         <f t="shared" si="0"/>
-        <v>0.29264855113316046</v>
+        <v>0.30127410080054123</v>
       </c>
       <c r="Q32" s="6">
         <f t="shared" si="1"/>
-        <v>0.2182150514956589</v>
+        <v>0.21705508102218005</v>
       </c>
       <c r="R32" s="6">
         <f t="shared" si="2"/>
-        <v>0.11279949348528774</v>
+        <v>0.11919121492069025</v>
       </c>
       <c r="S32" s="2">
         <v>0</v>
@@ -3722,19 +3707,19 @@
         <v>24854</v>
       </c>
       <c r="Y32" s="30">
-        <v>42708</v>
+        <v>43058</v>
       </c>
       <c r="Z32" s="6">
         <f t="shared" si="3"/>
-        <v>0.28591099361092753</v>
+        <v>0.29433795990306233</v>
       </c>
       <c r="AA32" s="7">
         <f t="shared" si="4"/>
-        <v>0.24977870765269172</v>
+        <v>0.24845095356884203</v>
       </c>
       <c r="AB32" s="7">
         <f t="shared" si="5"/>
-        <v>0.15851831038681277</v>
+        <v>0.15880904826048586</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.25">
@@ -3754,13 +3739,13 @@
         <v>0</v>
       </c>
       <c r="F33" s="31">
-        <v>18411</v>
+        <v>19006</v>
       </c>
       <c r="G33" s="31">
-        <v>21568</v>
+        <v>21700</v>
       </c>
       <c r="H33" s="29">
-        <v>25070</v>
+        <v>24892</v>
       </c>
       <c r="I33" s="2">
         <v>0</v>
@@ -3781,19 +3766,19 @@
         <v>25583</v>
       </c>
       <c r="O33" s="30">
-        <v>52293</v>
+        <v>52243</v>
       </c>
       <c r="P33" s="6">
         <f t="shared" si="0"/>
-        <v>1.0146037694257688</v>
+        <v>1.04739336492891</v>
       </c>
       <c r="Q33" s="6">
         <f t="shared" si="1"/>
-        <v>0.84305984442794046</v>
+        <v>0.84821952077551499</v>
       </c>
       <c r="R33" s="6">
         <f t="shared" si="2"/>
-        <v>0.47941407071692194</v>
+        <v>0.47646574660720098</v>
       </c>
       <c r="S33" s="2">
         <v>0</v>
@@ -3814,19 +3799,19 @@
         <v>21934</v>
       </c>
       <c r="Y33" s="30">
-        <v>37714</v>
+        <v>37747</v>
       </c>
       <c r="Z33" s="6">
         <f t="shared" si="3"/>
-        <v>1.0980497405618179</v>
+        <v>1.133536112602135</v>
       </c>
       <c r="AA33" s="7">
         <f t="shared" si="4"/>
-        <v>0.98331357709492118</v>
+        <v>0.98933163125740864</v>
       </c>
       <c r="AB33" s="7">
         <f t="shared" si="5"/>
-        <v>0.66473988439306353</v>
+        <v>0.65944313455373937</v>
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
@@ -3846,13 +3831,13 @@
         <v>153</v>
       </c>
       <c r="F34" s="31">
-        <v>11543</v>
+        <v>11819</v>
       </c>
       <c r="G34" s="31">
-        <v>8690</v>
+        <v>8760</v>
       </c>
       <c r="H34" s="31">
-        <v>10845</v>
+        <v>10841</v>
       </c>
       <c r="I34" s="2">
         <v>2</v>
@@ -3873,19 +3858,19 @@
         <v>38173</v>
       </c>
       <c r="O34" s="31">
-        <v>89047</v>
+        <v>89641</v>
       </c>
       <c r="P34" s="6">
         <f t="shared" si="0"/>
-        <v>0.37802521696413949</v>
+        <v>0.38706402488947111</v>
       </c>
       <c r="Q34" s="6">
         <f t="shared" si="1"/>
-        <v>0.22764781389987687</v>
+        <v>0.22948157074371939</v>
       </c>
       <c r="R34" s="6">
         <f t="shared" si="2"/>
-        <v>0.12178961671926061</v>
+        <v>0.12093796365502393</v>
       </c>
       <c r="S34" s="2">
         <v>0</v>
@@ -3906,19 +3891,19 @@
         <v>33705</v>
       </c>
       <c r="Y34" s="31">
-        <v>53355</v>
+        <v>53490</v>
       </c>
       <c r="Z34" s="6">
         <f t="shared" si="3"/>
-        <v>0.52268610758920486</v>
+        <v>0.53518384350661108</v>
       </c>
       <c r="AA34" s="7">
         <f t="shared" si="4"/>
-        <v>0.25782524847945409</v>
+        <v>0.2599020916777926</v>
       </c>
       <c r="AB34" s="7">
         <f t="shared" si="5"/>
-        <v>0.20326117514759628</v>
+        <v>0.2026733968966162</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.25">
@@ -3938,13 +3923,13 @@
         <v>185</v>
       </c>
       <c r="F35" s="31">
-        <v>12479</v>
+        <v>12795</v>
       </c>
       <c r="G35" s="31">
-        <v>8852</v>
+        <v>8859</v>
       </c>
       <c r="H35" s="31">
-        <v>10951</v>
+        <v>10984</v>
       </c>
       <c r="I35" s="2">
         <v>2</v>
@@ -3965,19 +3950,19 @@
         <v>24015</v>
       </c>
       <c r="O35" s="31">
-        <v>43887</v>
+        <v>44216</v>
       </c>
       <c r="P35" s="6">
         <f t="shared" si="0"/>
-        <v>0.96811481768813035</v>
+        <v>0.99262994569433671</v>
       </c>
       <c r="Q35" s="6">
         <f t="shared" si="1"/>
-        <v>0.36860295648552988</v>
+        <v>0.368894440974391</v>
       </c>
       <c r="R35" s="6">
         <f t="shared" si="2"/>
-        <v>0.24952719484129696</v>
+        <v>0.24841686267414512</v>
       </c>
       <c r="S35" s="2">
         <v>0</v>
@@ -3998,19 +3983,19 @@
         <v>20982</v>
       </c>
       <c r="Y35" s="31">
-        <v>32867</v>
+        <v>33323</v>
       </c>
       <c r="Z35" s="6">
         <f t="shared" si="3"/>
-        <v>1.0315780772092253</v>
+        <v>1.0577002562618831</v>
       </c>
       <c r="AA35" s="7">
         <f t="shared" si="4"/>
-        <v>0.42188542560289771</v>
+        <v>0.42221904489562484</v>
       </c>
       <c r="AB35" s="7">
         <f t="shared" si="5"/>
-        <v>0.33319134694374297</v>
+        <v>0.32962218287669176</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
@@ -4030,13 +4015,13 @@
         <v>16</v>
       </c>
       <c r="F36" s="31">
-        <v>2529</v>
+        <v>2600</v>
       </c>
       <c r="G36" s="31">
-        <v>2150</v>
+        <v>2153</v>
       </c>
       <c r="H36" s="31">
-        <v>2558</v>
+        <v>2560</v>
       </c>
       <c r="I36" s="2">
         <v>6</v>
@@ -4057,19 +4042,19 @@
         <v>10866</v>
       </c>
       <c r="O36" s="31">
-        <v>16551</v>
+        <v>16498</v>
       </c>
       <c r="P36" s="6">
         <f t="shared" si="0"/>
-        <v>0.36123410941294098</v>
+        <v>0.37137551778317385</v>
       </c>
       <c r="Q36" s="6">
         <f t="shared" si="1"/>
-        <v>0.19786489968709736</v>
+        <v>0.19814099024480031</v>
       </c>
       <c r="R36" s="6">
         <f t="shared" si="2"/>
-        <v>0.154552595009365</v>
+        <v>0.15517032367559705</v>
       </c>
       <c r="S36" s="2">
         <v>0</v>
@@ -4090,19 +4075,19 @@
         <v>8647</v>
       </c>
       <c r="Y36" s="31">
-        <v>12395</v>
+        <v>12164</v>
       </c>
       <c r="Z36" s="6">
         <f t="shared" si="3"/>
-        <v>0.39484777517564401</v>
+        <v>0.4059328649492584</v>
       </c>
       <c r="AA36" s="7">
         <f t="shared" si="4"/>
-        <v>0.24864114721868857</v>
+        <v>0.24898808835434255</v>
       </c>
       <c r="AB36" s="7">
         <f t="shared" si="5"/>
-        <v>0.20637353771682129</v>
+        <v>0.21045708648470898</v>
       </c>
     </row>
     <row r="37" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4122,13 +4107,13 @@
         <v>56</v>
       </c>
       <c r="F37" s="32">
-        <v>2727</v>
+        <v>2768</v>
       </c>
       <c r="G37" s="32">
-        <v>2785</v>
+        <v>2778</v>
       </c>
       <c r="H37" s="32">
-        <v>3399</v>
+        <v>3380</v>
       </c>
       <c r="I37" s="9">
         <v>2</v>
@@ -4149,19 +4134,19 @@
         <v>11988</v>
       </c>
       <c r="O37" s="32">
-        <v>18284</v>
+        <v>18301</v>
       </c>
       <c r="P37" s="10">
         <f t="shared" si="0"/>
-        <v>0.41044551475015051</v>
+        <v>0.41661649608669477</v>
       </c>
       <c r="Q37" s="10">
         <f t="shared" si="1"/>
-        <v>0.23231564898231566</v>
+        <v>0.23173173173173173</v>
       </c>
       <c r="R37" s="10">
         <f t="shared" si="2"/>
-        <v>0.18590024064756072</v>
+        <v>0.18468936123709087</v>
       </c>
       <c r="S37" s="9">
         <v>0</v>
@@ -4182,19 +4167,19 @@
         <v>4075</v>
       </c>
       <c r="Y37" s="32">
-        <v>5883</v>
+        <v>5877</v>
       </c>
       <c r="Z37" s="10">
         <f t="shared" si="3"/>
-        <v>0.97253922967189732</v>
+        <v>0.98716119828815974</v>
       </c>
       <c r="AA37" s="11">
         <f t="shared" si="4"/>
-        <v>0.68343558282208594</v>
+        <v>0.68171779141104294</v>
       </c>
       <c r="AB37" s="11">
         <f t="shared" si="5"/>
-        <v>0.57776644569097402</v>
+        <v>0.57512336225965632</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
@@ -4219,15 +4204,15 @@
       </c>
       <c r="F38" s="30">
         <f>AVERAGE(F3:F6)</f>
-        <v>55515.75</v>
+        <v>57319.25</v>
       </c>
       <c r="G38" s="30">
         <f t="shared" ref="G38:H38" si="7">AVERAGE(G3:G6)</f>
-        <v>70856.75</v>
+        <v>70663.75</v>
       </c>
       <c r="H38" s="30">
         <f t="shared" si="7"/>
-        <v>95962.75</v>
+        <v>95950</v>
       </c>
       <c r="I38" s="20">
         <f>COUNTIF(I3:I6,"=0")/COUNTA(I3:I6)</f>
@@ -4255,19 +4240,19 @@
       </c>
       <c r="O38" s="30">
         <f t="shared" si="9"/>
-        <v>662463.25</v>
+        <v>665625.5</v>
       </c>
       <c r="P38" s="12">
         <f>AVERAGE(P3:P6)</f>
-        <v>0.66979050341209145</v>
+        <v>0.69159175018482455</v>
       </c>
       <c r="Q38" s="12">
         <f>AVERAGE(Q3:Q6)</f>
-        <v>0.79749241269707905</v>
+        <v>0.79535749712355774</v>
       </c>
       <c r="R38" s="12">
         <f>AVERAGE(R3:R6)</f>
-        <v>0.1456156663285306</v>
+        <v>0.14517123465900292</v>
       </c>
       <c r="S38" s="20">
         <f>COUNTIF(S3:S6,"=0")/COUNTA(S3:S6)</f>
@@ -4295,19 +4280,19 @@
       </c>
       <c r="Y38" s="30">
         <f t="shared" si="11"/>
-        <v>142774</v>
+        <v>148046.75</v>
       </c>
       <c r="Z38" s="12">
         <f>AVERAGE(Z3:Z6)</f>
-        <v>1.262479503082379</v>
+        <v>1.3036372574939803</v>
       </c>
       <c r="AA38" s="13">
         <f>AVERAGE(AA3:AA6)</f>
-        <v>0.88747125140395022</v>
+        <v>0.88500969284804509</v>
       </c>
       <c r="AB38" s="13">
         <f>AVERAGE(AB3:AB6)</f>
-        <v>0.72952126281927754</v>
+        <v>0.70811638292740553</v>
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.25">
@@ -4332,15 +4317,15 @@
       </c>
       <c r="F39" s="31">
         <f>AVERAGE(F7:F37)</f>
-        <v>14557.709677419354</v>
+        <v>15180.064516129032</v>
       </c>
       <c r="G39" s="31">
         <f t="shared" ref="G39:H39" si="12">AVERAGE(G7:G37)</f>
-        <v>16467.16129032258</v>
+        <v>16743.096774193549</v>
       </c>
       <c r="H39" s="31">
         <f t="shared" si="12"/>
-        <v>21053.580645161292</v>
+        <v>21337.354838709678</v>
       </c>
       <c r="I39" s="21">
         <f>COUNTIF(I7:I37,"=0")/COUNTA(I7:I37)</f>
@@ -4368,19 +4353,19 @@
       </c>
       <c r="O39" s="31">
         <f t="shared" si="13"/>
-        <v>93020.419354838712</v>
+        <v>92904.032258064515</v>
       </c>
       <c r="P39" s="14">
         <f>AVERAGE(P7:P37)</f>
-        <v>0.61002938667910434</v>
+        <v>0.63214118993155821</v>
       </c>
       <c r="Q39" s="14">
         <f>AVERAGE(Q7:Q37)</f>
-        <v>0.42028218641232301</v>
+        <v>0.4331879538753996</v>
       </c>
       <c r="R39" s="14">
         <f>AVERAGE(R7:R37)</f>
-        <v>0.27802673398043543</v>
+        <v>0.28712577817035972</v>
       </c>
       <c r="S39" s="21">
         <f>COUNTIF(S7:S37,"=0")/COUNTA(S7:S37)</f>
@@ -4408,19 +4393,19 @@
       </c>
       <c r="Y39" s="31">
         <f t="shared" si="14"/>
-        <v>55672.645161290326</v>
+        <v>56657.387096774197</v>
       </c>
       <c r="Z39" s="14">
         <f>AVERAGE(Z7:Z37)</f>
-        <v>0.78356464480484345</v>
+        <v>0.81406231112358585</v>
       </c>
       <c r="AA39" s="14">
         <f>AVERAGE(AA7:AA37)</f>
-        <v>0.47581856508550435</v>
+        <v>0.49188463732045368</v>
       </c>
       <c r="AB39" s="23">
         <f>AVERAGE(AB7:AB37)</f>
-        <v>0.39085588418289635</v>
+        <v>0.39407752409702057</v>
       </c>
       <c r="AC39" s="24"/>
     </row>
@@ -4446,15 +4431,15 @@
       </c>
       <c r="F40" s="33">
         <f>AVERAGE(F3:F37)</f>
-        <v>19238.628571428573</v>
+        <v>19995.971428571429</v>
       </c>
       <c r="G40" s="33">
         <f t="shared" ref="G40:H40" si="15">AVERAGE(G3:G37)</f>
-        <v>22683.114285714284</v>
+        <v>22905.457142857143</v>
       </c>
       <c r="H40" s="33">
         <f t="shared" si="15"/>
-        <v>29614.628571428573</v>
+        <v>29864.514285714286</v>
       </c>
       <c r="I40" s="22">
         <f>COUNTIF(I3:I37,"=0")/COUNTA(I3:I37)</f>
@@ -4482,19 +4467,19 @@
       </c>
       <c r="O40" s="33">
         <f t="shared" si="16"/>
-        <v>158099.6</v>
+        <v>158357.91428571427</v>
       </c>
       <c r="P40" s="15">
         <f>AVERAGE(P3:P37)</f>
-        <v>0.6168592285914456</v>
+        <v>0.63893553967478856</v>
       </c>
       <c r="Q40" s="15">
         <f>AVERAGE(Q3:Q37)</f>
-        <v>0.46339192655915235</v>
+        <v>0.47457875881804618</v>
       </c>
       <c r="R40" s="15">
         <f>AVERAGE(R3:R37)</f>
-        <v>0.26289404053450338</v>
+        <v>0.27090240176906177</v>
       </c>
       <c r="S40" s="22">
         <f>COUNTIF(S3:S37,"=0")/COUNTA(S3:S37)</f>
@@ -4522,19 +4507,19 @@
       </c>
       <c r="Y40" s="33">
         <f t="shared" si="17"/>
-        <v>65627.085714285713</v>
+        <v>67101.885714285716</v>
       </c>
       <c r="Z40" s="15">
         <f>AVERAGE(Z3:Z37)</f>
-        <v>0.83829777146513329</v>
+        <v>0.8700137335659166</v>
       </c>
       <c r="AA40" s="16">
         <f>AVERAGE(AA3:AA37)</f>
-        <v>0.52286458637904099</v>
+        <v>0.53681321509503532</v>
       </c>
       <c r="AB40" s="16">
         <f>AVERAGE(AB3:AB37)</f>
-        <v>0.42956049888419706</v>
+        <v>0.42996767939192165</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.25">

</xml_diff>